<commit_message>
Names for first table
</commit_message>
<xml_diff>
--- a/res/Readdata/Plantilla.xlsx
+++ b/res/Readdata/Plantilla.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DB0786-9752-482B-9262-BBFAD3BA7889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B02120D-F88A-482A-9514-CD74EAC26F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notas" sheetId="3" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>Media filmafinity</t>
   </si>
@@ -332,6 +332,9 @@
   <si>
     <t>Pelis con nota</t>
   </si>
+  <si>
+    <t>Puntos</t>
+  </si>
 </sst>
 </file>
 
@@ -420,7 +423,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -787,12 +790,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -840,9 +874,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -895,33 +926,120 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="19">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF33CC33"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -997,6 +1115,28 @@
           <color indexed="64"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FF33CC33"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1100,7 +1240,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>5.3883439599484273</c:v>
+                  <c:v>2.0077163042251422</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1112,7 +1252,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.1305411517663022</c:v>
+                  <c:v>2.4541534533229714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2077,7 +2217,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.1305411517663022</c:v>
+                  <c:v>2.4541534533229714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2426,7 +2566,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>5.4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2695,7 +2835,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>5.4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3046,7 +3186,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3067,7 +3207,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -3832,7 +3972,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3853,7 +3993,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -4885,7 +5025,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.1305411517663022</c:v>
+                  <c:v>2.4541534533229714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5217,7 +5357,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>5.4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5976,7 +6116,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -5997,7 +6137,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -13604,27 +13744,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:N1048576" totalsRowShown="0" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:N1048576" totalsRowShown="0" tableBorderDxfId="16">
   <autoFilter ref="A1:N1048576" xr:uid="{B7E8E3F6-4A56-4C38-9CDA-83612E98463A}"/>
   <tableColumns count="14">
-    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="11"/>
-    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{65EE12B7-2552-4910-A353-7AE48A3D7AA6}" name="FA"/>
-    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{2E72113E-50BE-41C7-8BFD-59035950093F}" name="Varianza_FA" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{2E72113E-50BE-41C7-8BFD-59035950093F}" name="Varianza_FA" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{FF19B5AE-C56B-4CA5-B812-840E5C110430}" name="FA_redondeo"/>
     <tableColumn id="6" xr3:uid="{20BAA72D-A773-488D-B544-DAD2EF762D99}" name="Diferencia"/>
     <tableColumn id="7" xr3:uid="{E40D682E-5136-4AEB-BEE2-B6B87967AFB0}" name="Diferencia_abs"/>
-    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me_ha_gustado" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me_ha_gustado" dataDxfId="10">
       <calculatedColumnFormula>IF($H2&gt;0,1,0.1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia_ruido" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia_ruido" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="8">
       <calculatedColumnFormula>C2+(RAND()-0.5)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="5">
+  <autoFilter ref="B3:F13" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="0">
+      <calculatedColumnFormula>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="2">
+      <calculatedColumnFormula>(_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B3,MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="1">
+      <calculatedColumnFormula>(_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(B3,MediaFA,SQRT(VarFA),TRUE))*Pelis</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13895,8 +14055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8703B0C1-9812-4468-A745-94BA8D5548CD}">
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13904,15 +14064,15 @@
     <col min="1" max="1" width="7.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="19" customWidth="1"/>
     <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="73" customWidth="1"/>
-    <col min="5" max="6" width="12.140625" style="73" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="72" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" style="72" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="80" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="79" customWidth="1"/>
     <col min="11" max="12" width="7.42578125" style="30" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="78" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="77" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" customWidth="1"/>
     <col min="17" max="17" width="8.28515625" customWidth="1"/>
@@ -13937,10 +14097,10 @@
       <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="72" t="s">
         <v>56</v>
       </c>
       <c r="G1" t="s">
@@ -13964,7 +14124,7 @@
       <c r="M1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="78" t="s">
+      <c r="N1" s="77" t="s">
         <v>63</v>
       </c>
     </row>
@@ -13976,79 +14136,79 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>5.4</v>
-      </c>
-      <c r="D2" s="73">
+        <v>2</v>
+      </c>
+      <c r="D2" s="72">
         <v>130</v>
       </c>
-      <c r="E2" s="73">
+      <c r="E2" s="72">
         <v>26047</v>
       </c>
-      <c r="F2" s="81">
+      <c r="F2" s="80">
         <v>2.1</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2" si="0">ROUND($C2*2, 0)/2</f>
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <f>B2-C2</f>
-        <v>-3.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2" si="1">ABS(H2)</f>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="J2" s="80">
+        <v>0</v>
+      </c>
+      <c r="J2" s="79">
         <f t="shared" ref="J2" si="2">IF($H2&gt;0,1,0.1)</f>
         <v>0.1</v>
       </c>
       <c r="K2" s="30">
         <f t="shared" ref="K2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>2.1305411517663022</v>
+        <v>2.4541534533229714</v>
       </c>
       <c r="L2" s="30">
         <f t="shared" ref="L2" ca="1" si="4">C2+(RAND()-0.5)/10</f>
-        <v>5.3883439599484273</v>
+        <v>2.0077163042251422</v>
       </c>
       <c r="M2" s="17">
         <f t="shared" ref="M2" si="5">(B2-1)*10/9</f>
         <v>1.1111111111111112</v>
       </c>
-      <c r="N2" s="79">
+      <c r="N2" s="78">
         <f t="shared" ref="N2" si="6">(C2-1)*10/9</f>
-        <v>4.8888888888888893</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="O2" s="27"/>
       <c r="P2" s="27"/>
       <c r="Q2" s="27"/>
       <c r="R2" s="27"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O3" s="29"/>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
       <c r="R3" s="27"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O4" s="29"/>
       <c r="P4" s="29"/>
       <c r="Q4" s="29"/>
       <c r="R4" s="27"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
+      <c r="V4" s="55"/>
+      <c r="W4" s="55"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="55"/>
       <c r="AE5" s="1"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -14056,229 +14216,229 @@
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
+      <c r="V6" s="55"/>
+      <c r="W6" s="55"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O7" s="27"/>
       <c r="P7" s="27"/>
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
-      <c r="V7" s="56"/>
-      <c r="W7" s="56"/>
+      <c r="V7" s="55"/>
+      <c r="W7" s="55"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O8" s="27"/>
       <c r="P8" s="27"/>
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
-      <c r="V8" s="56"/>
-      <c r="W8" s="56"/>
+      <c r="V8" s="55"/>
+      <c r="W8" s="55"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O9" s="27"/>
       <c r="P9" s="27"/>
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
-      <c r="V9" s="56"/>
-      <c r="W9" s="56"/>
+      <c r="V9" s="55"/>
+      <c r="W9" s="55"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
       <c r="Q10" s="27"/>
       <c r="R10" s="27"/>
-      <c r="V10" s="56"/>
-      <c r="W10" s="56"/>
+      <c r="V10" s="55"/>
+      <c r="W10" s="55"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O11" s="27"/>
       <c r="P11" s="27"/>
       <c r="Q11" s="27"/>
       <c r="R11" s="27"/>
-      <c r="V11" s="56"/>
-      <c r="W11" s="56"/>
+      <c r="V11" s="55"/>
+      <c r="W11" s="55"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O12" s="27"/>
       <c r="P12" s="27"/>
       <c r="Q12" s="27"/>
       <c r="R12" s="27"/>
-      <c r="V12" s="56"/>
-      <c r="W12" s="56"/>
+      <c r="V12" s="55"/>
+      <c r="W12" s="55"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
       <c r="Q13" s="27"/>
       <c r="R13" s="27"/>
-      <c r="V13" s="56"/>
-      <c r="W13" s="56"/>
+      <c r="V13" s="55"/>
+      <c r="W13" s="55"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O14" s="27"/>
       <c r="P14" s="27"/>
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
-      <c r="V14" s="56"/>
-      <c r="W14" s="56"/>
+      <c r="V14" s="55"/>
+      <c r="W14" s="55"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O15" s="27"/>
       <c r="P15" s="27"/>
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
-      <c r="V15" s="56"/>
-      <c r="W15" s="56"/>
+      <c r="V15" s="55"/>
+      <c r="W15" s="55"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="O16" s="27"/>
       <c r="P16" s="27"/>
       <c r="Q16" s="27"/>
       <c r="R16" s="27"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="55"/>
     </row>
     <row r="17" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V17" s="56"/>
-      <c r="W17" s="56"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="55"/>
     </row>
     <row r="18" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V18" s="56"/>
-      <c r="W18" s="56"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="55"/>
     </row>
     <row r="19" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V19" s="56"/>
-      <c r="W19" s="56"/>
+      <c r="V19" s="55"/>
+      <c r="W19" s="55"/>
     </row>
     <row r="20" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
+      <c r="V20" s="55"/>
+      <c r="W20" s="55"/>
     </row>
     <row r="21" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
     </row>
     <row r="22" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V22" s="56"/>
-      <c r="W22" s="56"/>
+      <c r="V22" s="55"/>
+      <c r="W22" s="55"/>
     </row>
     <row r="23" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="55"/>
     </row>
     <row r="24" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="55"/>
     </row>
     <row r="25" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V25" s="56"/>
-      <c r="W25" s="56"/>
+      <c r="V25" s="55"/>
+      <c r="W25" s="55"/>
     </row>
     <row r="26" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V26" s="56"/>
-      <c r="W26" s="56"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
     </row>
     <row r="27" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V27" s="56"/>
-      <c r="W27" s="56"/>
+      <c r="V27" s="55"/>
+      <c r="W27" s="55"/>
     </row>
     <row r="28" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V28" s="56"/>
-      <c r="W28" s="56"/>
+      <c r="V28" s="55"/>
+      <c r="W28" s="55"/>
     </row>
     <row r="29" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
+      <c r="V29" s="55"/>
+      <c r="W29" s="55"/>
     </row>
     <row r="30" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V30" s="56"/>
-      <c r="W30" s="56"/>
+      <c r="V30" s="55"/>
+      <c r="W30" s="55"/>
     </row>
     <row r="31" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
+      <c r="V31" s="55"/>
+      <c r="W31" s="55"/>
     </row>
     <row r="32" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V32" s="56"/>
-      <c r="W32" s="56"/>
+      <c r="V32" s="55"/>
+      <c r="W32" s="55"/>
     </row>
     <row r="33" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V33" s="56"/>
-      <c r="W33" s="56"/>
+      <c r="V33" s="55"/>
+      <c r="W33" s="55"/>
     </row>
     <row r="34" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V34" s="56"/>
-      <c r="W34" s="56"/>
+      <c r="V34" s="55"/>
+      <c r="W34" s="55"/>
     </row>
     <row r="35" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V35" s="56"/>
-      <c r="W35" s="56"/>
+      <c r="V35" s="55"/>
+      <c r="W35" s="55"/>
     </row>
     <row r="36" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V36" s="56"/>
-      <c r="W36" s="56"/>
+      <c r="V36" s="55"/>
+      <c r="W36" s="55"/>
     </row>
     <row r="37" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V37" s="56"/>
-      <c r="W37" s="56"/>
+      <c r="V37" s="55"/>
+      <c r="W37" s="55"/>
     </row>
     <row r="38" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V38" s="56"/>
-      <c r="W38" s="56"/>
+      <c r="V38" s="55"/>
+      <c r="W38" s="55"/>
     </row>
     <row r="39" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V39" s="56"/>
-      <c r="W39" s="56"/>
+      <c r="V39" s="55"/>
+      <c r="W39" s="55"/>
     </row>
     <row r="40" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V40" s="56"/>
-      <c r="W40" s="56"/>
+      <c r="V40" s="55"/>
+      <c r="W40" s="55"/>
     </row>
     <row r="41" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V41" s="56"/>
-      <c r="W41" s="56"/>
+      <c r="V41" s="55"/>
+      <c r="W41" s="55"/>
     </row>
     <row r="42" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V42" s="56"/>
-      <c r="W42" s="56"/>
+      <c r="V42" s="55"/>
+      <c r="W42" s="55"/>
     </row>
     <row r="43" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V43" s="55"/>
-      <c r="W43" s="55"/>
+      <c r="V43" s="54"/>
+      <c r="W43" s="54"/>
     </row>
     <row r="44" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V44" s="55"/>
-      <c r="W44" s="55"/>
+      <c r="V44" s="54"/>
+      <c r="W44" s="54"/>
     </row>
     <row r="45" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V45" s="55"/>
-      <c r="W45" s="55"/>
+      <c r="V45" s="54"/>
+      <c r="W45" s="54"/>
     </row>
     <row r="46" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V46" s="55"/>
-      <c r="W46" s="55"/>
+      <c r="V46" s="54"/>
+      <c r="W46" s="54"/>
     </row>
     <row r="47" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V47" s="55"/>
-      <c r="W47" s="55"/>
+      <c r="V47" s="54"/>
+      <c r="W47" s="54"/>
     </row>
     <row r="48" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V48" s="55"/>
-      <c r="W48" s="55"/>
+      <c r="V48" s="54"/>
+      <c r="W48" s="54"/>
     </row>
     <row r="49" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V49" s="55"/>
-      <c r="W49" s="55"/>
+      <c r="V49" s="54"/>
+      <c r="W49" s="54"/>
     </row>
     <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14381,7 +14541,7 @@
       </c>
       <c r="B3" s="7">
         <f>AVERAGE(Tabla1[FA])</f>
-        <v>5.4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -14402,7 +14562,7 @@
       </c>
       <c r="H3" s="7">
         <f>MEDIAN(Tabla1[FA])</f>
-        <v>5.4</v>
+        <v>2</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>22</v>
@@ -14414,16 +14574,16 @@
       <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="58">
+      <c r="L3" s="57">
         <f>MAX(Tabla1[FA])</f>
-        <v>5.4</v>
+        <v>2</v>
       </c>
       <c r="M3" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="58">
+      <c r="N3" s="57">
         <f>MIN(Notas!C:C)</f>
-        <v>5.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -14465,14 +14625,14 @@
       <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="59">
+      <c r="L4" s="58">
         <f>MAX(NotasMias)</f>
         <v>2</v>
       </c>
       <c r="M4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="59">
+      <c r="N4" s="58">
         <f>MIN(NotasMias)</f>
         <v>2</v>
       </c>
@@ -14483,7 +14643,7 @@
       </c>
       <c r="B5" s="1">
         <f>AVERAGE(Tabla1[Diferencia])</f>
-        <v>-3.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="G5" s="27"/>
     </row>
@@ -14493,7 +14653,7 @@
       </c>
       <c r="B6" s="1">
         <f>AVERAGE(Tabla1[Diferencia_abs])</f>
-        <v>3.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -14512,7 +14672,7 @@
       </c>
       <c r="B8">
         <f>MAX(Tabla1[Diferencia_abs])</f>
-        <v>3.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -14521,7 +14681,7 @@
         <f>CORREL(Notas!B:B,Notas!C:C)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E8" s="54"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="32"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -14530,7 +14690,7 @@
       </c>
       <c r="B9">
         <f>MIN(Tabla1[Diferencia])</f>
-        <v>-3.4000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -14539,7 +14699,7 @@
       </c>
       <c r="B10">
         <f>MAX(Tabla1[Diferencia])</f>
-        <v>-3.4000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -14562,7 +14722,7 @@
       <c r="F15" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="77">
+      <c r="G15" s="76">
         <v>7.8</v>
       </c>
     </row>
@@ -14572,7 +14732,7 @@
       </c>
       <c r="B16" s="15">
         <f>(MediaFA-1)*10/9</f>
-        <v>4.8888888888888893</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>8</v>
@@ -14581,11 +14741,11 @@
         <f>STDEVP(Tabla1[FA_rees])</f>
         <v>0</v>
       </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66" t="s">
+      <c r="E16" s="65"/>
+      <c r="F16" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="75">
+      <c r="G16" s="74">
         <f>COUNTIF(NotasFA,"&lt;="&amp;G15)/Pelis_con_nota</f>
         <v>1</v>
       </c>
@@ -14605,11 +14765,11 @@
         <f>STDEVP(Tabla1[Mia_rees])</f>
         <v>0</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66" t="s">
+      <c r="E17" s="65"/>
+      <c r="F17" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="76">
+      <c r="G17" s="75">
         <f>COUNTIF(NotasMias,"&lt;="&amp;G15)/Pelis</f>
         <v>1</v>
       </c>
@@ -14638,252 +14798,253 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB957686-4157-457C-B9AD-66FD2970B9E3}">
-  <dimension ref="B2:S40"/>
+  <dimension ref="B3:S40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="19" max="19" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="B3" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="89" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="81">
         <v>1</v>
       </c>
       <c r="C4" s="21">
-        <f t="shared" ref="C4:C13" si="0">COUNTIF(NotasMias,$B4)</f>
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
         <v>0</v>
       </c>
       <c r="D4" s="25">
-        <f>COUNTIF(NotasFA,"&lt;=($B6+0,5)")</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="43" t="e">
+        <f>COUNTIF(NotasFA,"&lt;=([@[Puntos]]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="42" t="e">
         <f>_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE)*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F4" s="42" t="e">
+      <c r="F4" s="66" t="e">
         <f>_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE)*Pelis</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="82">
         <v>2</v>
       </c>
       <c r="C5" s="3">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <f>COUNTIFS(NotasFA,"&gt;0",NotasFA,"&lt;=([@Puntos]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="43" t="e">
+        <f t="shared" ref="E5:E13" si="0">(_xlfn.NORM.DIST(B5,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F5" s="84" t="e">
+        <f t="shared" ref="F5:F13" si="1">(_xlfn.NORM.DIST(B5,MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE))*Pelis</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="82">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <f>COUNTIFS(NotasFA,"&gt;0",NotasFA,"&lt;=([@Puntos]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="43" t="e">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <f>COUNTIF(NotasFA,"&gt;1,5")-COUNTIF(Notas!G:G,"&gt;2,5")</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="44" t="e">
-        <f t="shared" ref="E5:E13" si="1">(_xlfn.NORM.DIST(B5,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F5" s="33" t="e">
-        <f t="shared" ref="F5:F13" si="2">(_xlfn.NORM.DIST(B5,MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE))*Pelis</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <f>COUNTIF(Notas!G:G,"&gt;2,5")-COUNTIF(Notas!G:G,"&gt;3,5")</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="44" t="e">
+      <c r="F6" s="84" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="F6" s="33" t="e">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="82">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <f>COUNTIFS(NotasFA,"&gt;0",NotasFA,"&lt;=([@Puntos]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="43" t="e">
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <f>COUNTIF(Notas!G:G,"&gt;3,5")-COUNTIF(Notas!G:G,"&gt;4,5")</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="44" t="e">
+      <c r="F7" s="84" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="F7" s="33" t="e">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="82">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <f>COUNTIFS(NotasFA,"&gt;0",NotasFA,"&lt;=([@Puntos]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="43" t="e">
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <f>COUNTIF(Notas!G:G,"&gt;4,5")-COUNTIF(Notas!G:G,"&gt;5,5")</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="44" t="e">
+      <c r="F8" s="84" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="F8" s="33" t="e">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="82">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <f>COUNTIFS(NotasFA,"&gt;0",NotasFA,"&lt;=([@Puntos]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="43" t="e">
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <f>COUNTIF(Notas!G:G,"&gt;5,5")-COUNTIF(Notas!G:G,"&gt;6,5")</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="44" t="e">
+      <c r="F9" s="84" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="F9" s="33" t="e">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="82">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <f>COUNTIFS(NotasFA,"&gt;0",NotasFA,"&lt;=([@Puntos]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="43" t="e">
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <f>COUNTIF(Notas!G:G,"&gt;6,5")-COUNTIF(Notas!G:G,"&gt;7,5")</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="44" t="e">
+      <c r="F10" s="84" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="F10" s="33" t="e">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="82">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <f>COUNTIFS(NotasFA,"&gt;0",NotasFA,"&lt;=([@Puntos]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="43" t="e">
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <f>COUNTIF(Notas!G:G,"&gt;7,5")-COUNTIF(Notas!G:G,"&gt;8,5")</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="44" t="e">
+      <c r="F11" s="84" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="F11" s="33" t="e">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="82">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <f>COUNTIFS(NotasFA,"&gt;0",NotasFA,"&lt;=([@Puntos]+0,5)")</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="43" t="e">
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="22">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <f>COUNTIF(Notas!G:G,"&gt;8,5")-COUNTIF(Notas!G:G,"&gt;9,5")</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="44" t="e">
+      <c r="F12" s="84" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="F12" s="33" t="e">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="83">
+        <v>10</v>
+      </c>
+      <c r="C13" s="24">
+        <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="26">
+        <f>COUNTIF(NotasFA,"&gt;DESREF([@Puntos];-1;0)+0,5")</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="43" t="e">
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="23">
-        <v>10</v>
-      </c>
-      <c r="C13" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="26">
-        <f>COUNTIF(Notas!G:G,"&gt;9,5")</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="44" t="e">
+      <c r="F13" s="84" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="F13" s="33" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="67" t="e">
+      <c r="E14" s="66" t="e">
         <f>SUM(E4:E13)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F14" s="67" t="e">
+      <c r="F14" s="66" t="e">
         <f>SUM(F4:F13)</f>
         <v>#NUM!</v>
       </c>
@@ -14896,10 +15057,10 @@
       <c r="C19" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="65" t="s">
+      <c r="E19" s="64" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="40" t="s">
@@ -14914,15 +15075,15 @@
         <f>C21/2</f>
         <v>0</v>
       </c>
-      <c r="D20" s="46">
+      <c r="D20" s="45">
         <f>COUNTIF(Notas!G:G,Normales!B20)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="43" t="e">
+      <c r="E20" s="42" t="e">
         <f>_xlfn.NORM.DIST(B20,MediaMia,SQRT(VarMia),TRUE)*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F20" s="51" t="e">
+      <c r="F20" s="50" t="e">
         <f>_xlfn.NORM.DIST(B20,MediaFA,SQRT(VarFA),TRUE)*Pelis</f>
         <v>#NUM!</v>
       </c>
@@ -14942,16 +15103,16 @@
         <f>COUNTIF(Notas!B:B,B21)/2</f>
         <v>0</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D21" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B21)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="44" t="e">
-        <f t="shared" ref="E21:E39" si="3">(_xlfn.NORM.DIST(B21,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B20,MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
+      <c r="E21" s="43" t="e">
+        <f t="shared" ref="E21:E39" si="2">(_xlfn.NORM.DIST(B21,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B20,MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F21" s="52" t="e">
-        <f t="shared" ref="F21:F39" si="4">(_xlfn.NORM.DIST(B21,MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(B20,MediaFA,SQRT(VarFA),TRUE))*Pelis</f>
+      <c r="F21" s="51" t="e">
+        <f t="shared" ref="F21:F39" si="3">(_xlfn.NORM.DIST(B21,MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(B20,MediaFA,SQRT(VarFA),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
       <c r="R21" t="s">
@@ -14970,16 +15131,16 @@
         <f>(C21+C23)/2</f>
         <v>0.25</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B22)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="44" t="e">
+      <c r="E22" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F22" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F22" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -14991,16 +15152,16 @@
         <f>COUNTIF(Notas!B:B,B23)/2</f>
         <v>0.5</v>
       </c>
-      <c r="D23" s="47">
+      <c r="D23" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B23)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="44" t="e">
+        <v>1</v>
+      </c>
+      <c r="E23" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F23" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F23" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15012,16 +15173,16 @@
         <f>(C23+C25)/2</f>
         <v>0.25</v>
       </c>
-      <c r="D24" s="47">
+      <c r="D24" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B24)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="44" t="e">
+      <c r="E24" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F24" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F24" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15033,16 +15194,16 @@
         <f>COUNTIF(Notas!B:B,B25)/2</f>
         <v>0</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B25)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="44" t="e">
+      <c r="E25" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F25" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F25" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15054,16 +15215,16 @@
         <f>(C25+C27)/2</f>
         <v>0</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B26)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="44" t="e">
+      <c r="E26" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F26" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F26" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15075,16 +15236,16 @@
         <f>COUNTIF(Notas!B:B,B27)/2</f>
         <v>0</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B27)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="44" t="e">
+      <c r="E27" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F27" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F27" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15096,16 +15257,16 @@
         <f>(C27+C29)/2</f>
         <v>0</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D28" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B28)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="44" t="e">
+      <c r="E28" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F28" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F28" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15117,16 +15278,16 @@
         <f>COUNTIF(Notas!B:B,B29)/2</f>
         <v>0</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D29" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B29)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="44" t="e">
+      <c r="E29" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F29" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F29" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15138,16 +15299,16 @@
         <f>(C29+C31)/2</f>
         <v>0</v>
       </c>
-      <c r="D30" s="47">
+      <c r="D30" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B30)</f>
-        <v>1</v>
-      </c>
-      <c r="E30" s="44" t="e">
+        <v>0</v>
+      </c>
+      <c r="E30" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F30" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F30" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15159,16 +15320,16 @@
         <f>COUNTIF(Notas!B:B,B31)/2</f>
         <v>0</v>
       </c>
-      <c r="D31" s="47">
+      <c r="D31" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B31)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="44" t="e">
+      <c r="E31" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F31" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F31" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15180,16 +15341,16 @@
         <f>(C31+C33)/2</f>
         <v>0</v>
       </c>
-      <c r="D32" s="47">
+      <c r="D32" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B32)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="44" t="e">
+      <c r="E32" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F32" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F32" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15201,16 +15362,16 @@
         <f>COUNTIF(Notas!B:B,B33)/2</f>
         <v>0</v>
       </c>
-      <c r="D33" s="47">
+      <c r="D33" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B33)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="44" t="e">
+      <c r="E33" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F33" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F33" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15222,16 +15383,16 @@
         <f>(C33+C35)/2</f>
         <v>0</v>
       </c>
-      <c r="D34" s="47">
+      <c r="D34" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B34)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="44" t="e">
+      <c r="E34" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F34" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F34" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15243,16 +15404,16 @@
         <f>COUNTIF(Notas!B:B,B35)/2</f>
         <v>0</v>
       </c>
-      <c r="D35" s="47">
+      <c r="D35" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B35)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="44" t="e">
+      <c r="E35" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F35" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F35" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15264,16 +15425,16 @@
         <f>(C35+C37)/2</f>
         <v>0</v>
       </c>
-      <c r="D36" s="47">
+      <c r="D36" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B36)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="44" t="e">
+      <c r="E36" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F36" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F36" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15285,16 +15446,16 @@
         <f>COUNTIF(Notas!B:B,B37)/2</f>
         <v>0</v>
       </c>
-      <c r="D37" s="47">
+      <c r="D37" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B37)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="44" t="e">
+      <c r="E37" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F37" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F37" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15306,16 +15467,16 @@
         <f>(C37+C39)/2</f>
         <v>0</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="46">
         <f>COUNTIF(Notas!G:G,Normales!B38)</f>
         <v>0</v>
       </c>
-      <c r="E38" s="44" t="e">
+      <c r="E38" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F38" s="51" t="e">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F38" s="52" t="e">
-        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15327,21 +15488,21 @@
         <f>COUNTIF(Notas!B:B,B39)/2</f>
         <v>0</v>
       </c>
-      <c r="D39" s="48">
+      <c r="D39" s="47">
         <f>COUNTIF(Notas!G:G,Normales!B39)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="44" t="e">
+      <c r="E39" s="43" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F39" s="51" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="F39" s="52" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="50">
+      <c r="C40" s="49">
         <f>SUM(C20:C39)</f>
         <v>1</v>
       </c>
@@ -15349,11 +15510,11 @@
         <f>SUM(D20:D39)</f>
         <v>1</v>
       </c>
-      <c r="E40" s="67" t="e">
+      <c r="E40" s="66" t="e">
         <f>SUM(E20:E39)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F40" s="67" t="e">
+      <c r="F40" s="66" t="e">
         <f>SUM(F20:F39)</f>
         <v>#NUM!</v>
       </c>
@@ -15361,6 +15522,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -15386,7 +15550,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
+      <c r="A1" s="56"/>
       <c r="E1" t="s">
         <v>15</v>
       </c>
@@ -15466,34 +15630,34 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F4" s="19"/>
-      <c r="P4" s="60">
+      <c r="P4" s="59">
         <v>5</v>
       </c>
-      <c r="Q4" s="61">
+      <c r="Q4" s="60">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P4)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="42" t="e">
+      <c r="R4" s="41" t="e">
         <f>EXP((P4-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T4" s="60">
+      <c r="T4" s="59">
         <v>10</v>
       </c>
-      <c r="U4" s="61">
+      <c r="U4" s="60">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T4)</f>
         <v>0</v>
       </c>
-      <c r="V4" s="42" t="e">
+      <c r="V4" s="41" t="e">
         <f>EXP((T4-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P5" s="62">
+      <c r="P5" s="61">
         <v>10</v>
       </c>
-      <c r="Q5" s="55">
+      <c r="Q5" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P5)-COUNTIF(Notas!D:D,"&lt;="&amp;P4)</f>
         <v>0</v>
       </c>
@@ -15501,10 +15665,10 @@
         <f>EXP((P5-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T5" s="62">
+      <c r="T5" s="61">
         <v>20</v>
       </c>
-      <c r="U5" s="55">
+      <c r="U5" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T5)-COUNTIF(Notas!D:D,"&lt;="&amp;T4)</f>
         <v>0</v>
       </c>
@@ -15514,10 +15678,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P6" s="62">
+      <c r="P6" s="61">
         <v>15</v>
       </c>
-      <c r="Q6" s="55">
+      <c r="Q6" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P6)-COUNTIF(Notas!D:D,"&lt;="&amp;P5)</f>
         <v>0</v>
       </c>
@@ -15525,10 +15689,10 @@
         <f>EXP((P6-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T6" s="62">
+      <c r="T6" s="61">
         <v>30</v>
       </c>
-      <c r="U6" s="55">
+      <c r="U6" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T6)-COUNTIF(Notas!D:D,"&lt;="&amp;T5)</f>
         <v>0</v>
       </c>
@@ -15538,10 +15702,10 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P7" s="62">
+      <c r="P7" s="61">
         <v>20</v>
       </c>
-      <c r="Q7" s="55">
+      <c r="Q7" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P7)-COUNTIF(Notas!D:D,"&lt;="&amp;P6)</f>
         <v>0</v>
       </c>
@@ -15549,10 +15713,10 @@
         <f>EXP((P7-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T7" s="62">
+      <c r="T7" s="61">
         <v>40</v>
       </c>
-      <c r="U7" s="55">
+      <c r="U7" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T7)-COUNTIF(Notas!D:D,"&lt;="&amp;T6)</f>
         <v>0</v>
       </c>
@@ -15562,10 +15726,10 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P8" s="62">
+      <c r="P8" s="61">
         <v>25</v>
       </c>
-      <c r="Q8" s="55">
+      <c r="Q8" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P8)-COUNTIF(Notas!D:D,"&lt;="&amp;P7)</f>
         <v>0</v>
       </c>
@@ -15573,10 +15737,10 @@
         <f>EXP((P8-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T8" s="62">
+      <c r="T8" s="61">
         <v>50</v>
       </c>
-      <c r="U8" s="55">
+      <c r="U8" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T8)-COUNTIF(Notas!D:D,"&lt;="&amp;T7)</f>
         <v>0</v>
       </c>
@@ -15586,10 +15750,10 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P9" s="62">
+      <c r="P9" s="61">
         <v>30</v>
       </c>
-      <c r="Q9" s="55">
+      <c r="Q9" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P9)-COUNTIF(Notas!D:D,"&lt;="&amp;P8)</f>
         <v>0</v>
       </c>
@@ -15597,10 +15761,10 @@
         <f>EXP((P9-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="62">
+      <c r="T9" s="61">
         <v>60</v>
       </c>
-      <c r="U9" s="55">
+      <c r="U9" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T9)-COUNTIF(Notas!D:D,"&lt;="&amp;T8)</f>
         <v>0</v>
       </c>
@@ -15610,10 +15774,10 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P10" s="62">
+      <c r="P10" s="61">
         <v>35</v>
       </c>
-      <c r="Q10" s="55">
+      <c r="Q10" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P10)-COUNTIF(Notas!D:D,"&lt;="&amp;P9)</f>
         <v>0</v>
       </c>
@@ -15621,10 +15785,10 @@
         <f>EXP((P10-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T10" s="62">
+      <c r="T10" s="61">
         <v>70</v>
       </c>
-      <c r="U10" s="55">
+      <c r="U10" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T10)-COUNTIF(Notas!D:D,"&lt;="&amp;T9)</f>
         <v>0</v>
       </c>
@@ -15634,10 +15798,10 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P11" s="62">
+      <c r="P11" s="61">
         <v>40</v>
       </c>
-      <c r="Q11" s="55">
+      <c r="Q11" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P11)-COUNTIF(Notas!D:D,"&lt;="&amp;P10)</f>
         <v>0</v>
       </c>
@@ -15645,10 +15809,10 @@
         <f>EXP((P11-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T11" s="62">
+      <c r="T11" s="61">
         <v>80</v>
       </c>
-      <c r="U11" s="55">
+      <c r="U11" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T11)-COUNTIF(Notas!D:D,"&lt;="&amp;T10)</f>
         <v>0</v>
       </c>
@@ -15658,10 +15822,10 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P12" s="62">
+      <c r="P12" s="61">
         <v>45</v>
       </c>
-      <c r="Q12" s="55">
+      <c r="Q12" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P12)-COUNTIF(Notas!D:D,"&lt;="&amp;P11)</f>
         <v>0</v>
       </c>
@@ -15669,10 +15833,10 @@
         <f>EXP((P12-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T12" s="62">
+      <c r="T12" s="61">
         <v>90</v>
       </c>
-      <c r="U12" s="55">
+      <c r="U12" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T12)-COUNTIF(Notas!D:D,"&lt;="&amp;T11)</f>
         <v>0</v>
       </c>
@@ -15682,10 +15846,10 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P13" s="62">
+      <c r="P13" s="61">
         <v>50</v>
       </c>
-      <c r="Q13" s="55">
+      <c r="Q13" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P13)-COUNTIF(Notas!D:D,"&lt;="&amp;P12)</f>
         <v>0</v>
       </c>
@@ -15693,10 +15857,10 @@
         <f>EXP((P13-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T13" s="62">
+      <c r="T13" s="61">
         <v>100</v>
       </c>
-      <c r="U13" s="55">
+      <c r="U13" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T13)-COUNTIF(Notas!D:D,"&lt;="&amp;T12)</f>
         <v>0</v>
       </c>
@@ -15706,10 +15870,10 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P14" s="62">
+      <c r="P14" s="61">
         <v>55</v>
       </c>
-      <c r="Q14" s="55">
+      <c r="Q14" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P14)-COUNTIF(Notas!D:D,"&lt;="&amp;P13)</f>
         <v>0</v>
       </c>
@@ -15717,10 +15881,10 @@
         <f>EXP((P14-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T14" s="62">
+      <c r="T14" s="61">
         <v>110</v>
       </c>
-      <c r="U14" s="55">
+      <c r="U14" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T14)-COUNTIF(Notas!D:D,"&lt;="&amp;T13)</f>
         <v>0</v>
       </c>
@@ -15730,10 +15894,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P15" s="62">
+      <c r="P15" s="61">
         <v>60</v>
       </c>
-      <c r="Q15" s="55">
+      <c r="Q15" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P15)-COUNTIF(Notas!D:D,"&lt;="&amp;P14)</f>
         <v>0</v>
       </c>
@@ -15741,10 +15905,10 @@
         <f>EXP((P15-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T15" s="62">
+      <c r="T15" s="61">
         <v>120</v>
       </c>
-      <c r="U15" s="55">
+      <c r="U15" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T15)-COUNTIF(Notas!D:D,"&lt;="&amp;T14)</f>
         <v>0</v>
       </c>
@@ -15754,10 +15918,10 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P16" s="62">
+      <c r="P16" s="61">
         <v>65</v>
       </c>
-      <c r="Q16" s="55">
+      <c r="Q16" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P16)-COUNTIF(Notas!D:D,"&lt;="&amp;P15)</f>
         <v>0</v>
       </c>
@@ -15765,10 +15929,10 @@
         <f>EXP((P16-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T16" s="62">
+      <c r="T16" s="61">
         <v>130</v>
       </c>
-      <c r="U16" s="55">
+      <c r="U16" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T16)-COUNTIF(Notas!D:D,"&lt;="&amp;T15)</f>
         <v>1</v>
       </c>
@@ -15778,10 +15942,10 @@
       </c>
     </row>
     <row r="17" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P17" s="62">
+      <c r="P17" s="61">
         <v>70</v>
       </c>
-      <c r="Q17" s="55">
+      <c r="Q17" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P17)-COUNTIF(Notas!D:D,"&lt;="&amp;P16)</f>
         <v>0</v>
       </c>
@@ -15789,10 +15953,10 @@
         <f>EXP((P17-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T17" s="62">
+      <c r="T17" s="61">
         <v>140</v>
       </c>
-      <c r="U17" s="55">
+      <c r="U17" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T17)-COUNTIF(Notas!D:D,"&lt;="&amp;T16)</f>
         <v>0</v>
       </c>
@@ -15802,10 +15966,10 @@
       </c>
     </row>
     <row r="18" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P18" s="62">
+      <c r="P18" s="61">
         <v>75</v>
       </c>
-      <c r="Q18" s="55">
+      <c r="Q18" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P18)-COUNTIF(Notas!D:D,"&lt;="&amp;P17)</f>
         <v>0</v>
       </c>
@@ -15813,10 +15977,10 @@
         <f>EXP((P18-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T18" s="62">
+      <c r="T18" s="61">
         <v>150</v>
       </c>
-      <c r="U18" s="55">
+      <c r="U18" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T18)-COUNTIF(Notas!D:D,"&lt;="&amp;T17)</f>
         <v>0</v>
       </c>
@@ -15826,10 +15990,10 @@
       </c>
     </row>
     <row r="19" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P19" s="62">
+      <c r="P19" s="61">
         <v>80</v>
       </c>
-      <c r="Q19" s="55">
+      <c r="Q19" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P19)-COUNTIF(Notas!D:D,"&lt;="&amp;P18)</f>
         <v>0</v>
       </c>
@@ -15837,10 +16001,10 @@
         <f>EXP((P19-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T19" s="62">
+      <c r="T19" s="61">
         <v>160</v>
       </c>
-      <c r="U19" s="55">
+      <c r="U19" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T19)-COUNTIF(Notas!D:D,"&lt;="&amp;T18)</f>
         <v>0</v>
       </c>
@@ -15850,10 +16014,10 @@
       </c>
     </row>
     <row r="20" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P20" s="62">
+      <c r="P20" s="61">
         <v>85</v>
       </c>
-      <c r="Q20" s="55">
+      <c r="Q20" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P20)-COUNTIF(Notas!D:D,"&lt;="&amp;P19)</f>
         <v>0</v>
       </c>
@@ -15861,10 +16025,10 @@
         <f>EXP((P20-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T20" s="62">
+      <c r="T20" s="61">
         <v>170</v>
       </c>
-      <c r="U20" s="55">
+      <c r="U20" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T20)-COUNTIF(Notas!D:D,"&lt;="&amp;T19)</f>
         <v>0</v>
       </c>
@@ -15874,10 +16038,10 @@
       </c>
     </row>
     <row r="21" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P21" s="62">
+      <c r="P21" s="61">
         <v>90</v>
       </c>
-      <c r="Q21" s="55">
+      <c r="Q21" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P21)-COUNTIF(Notas!D:D,"&lt;="&amp;P20)</f>
         <v>0</v>
       </c>
@@ -15885,10 +16049,10 @@
         <f>EXP((P21-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T21" s="62">
+      <c r="T21" s="61">
         <v>180</v>
       </c>
-      <c r="U21" s="55">
+      <c r="U21" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T21)-COUNTIF(Notas!D:D,"&lt;="&amp;T20)</f>
         <v>0</v>
       </c>
@@ -15898,10 +16062,10 @@
       </c>
     </row>
     <row r="22" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P22" s="62">
+      <c r="P22" s="61">
         <v>95</v>
       </c>
-      <c r="Q22" s="55">
+      <c r="Q22" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P22)-COUNTIF(Notas!D:D,"&lt;="&amp;P21)</f>
         <v>0</v>
       </c>
@@ -15909,10 +16073,10 @@
         <f>EXP((P22-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T22" s="62">
+      <c r="T22" s="61">
         <v>190</v>
       </c>
-      <c r="U22" s="55">
+      <c r="U22" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T22)-COUNTIF(Notas!D:D,"&lt;="&amp;T21)</f>
         <v>0</v>
       </c>
@@ -15922,10 +16086,10 @@
       </c>
     </row>
     <row r="23" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P23" s="62">
+      <c r="P23" s="61">
         <v>100</v>
       </c>
-      <c r="Q23" s="55">
+      <c r="Q23" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P23)-COUNTIF(Notas!D:D,"&lt;="&amp;P22)</f>
         <v>0</v>
       </c>
@@ -15933,10 +16097,10 @@
         <f>EXP((P23-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T23" s="62">
+      <c r="T23" s="61">
         <v>200</v>
       </c>
-      <c r="U23" s="55">
+      <c r="U23" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T23)-COUNTIF(Notas!D:D,"&lt;="&amp;T22)</f>
         <v>0</v>
       </c>
@@ -15946,10 +16110,10 @@
       </c>
     </row>
     <row r="24" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P24" s="62">
+      <c r="P24" s="61">
         <v>105</v>
       </c>
-      <c r="Q24" s="55">
+      <c r="Q24" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P24)-COUNTIF(Notas!D:D,"&lt;="&amp;P23)</f>
         <v>0</v>
       </c>
@@ -15957,10 +16121,10 @@
         <f>EXP((P24-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T24" s="62">
+      <c r="T24" s="61">
         <v>210</v>
       </c>
-      <c r="U24" s="55">
+      <c r="U24" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T24)-COUNTIF(Notas!D:D,"&lt;="&amp;T23)</f>
         <v>0</v>
       </c>
@@ -15970,10 +16134,10 @@
       </c>
     </row>
     <row r="25" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P25" s="62">
+      <c r="P25" s="61">
         <v>110</v>
       </c>
-      <c r="Q25" s="55">
+      <c r="Q25" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P25)-COUNTIF(Notas!D:D,"&lt;="&amp;P24)</f>
         <v>0</v>
       </c>
@@ -15981,10 +16145,10 @@
         <f>EXP((P25-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T25" s="62">
+      <c r="T25" s="61">
         <v>220</v>
       </c>
-      <c r="U25" s="55">
+      <c r="U25" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T25)-COUNTIF(Notas!D:D,"&lt;="&amp;T24)</f>
         <v>0</v>
       </c>
@@ -15994,10 +16158,10 @@
       </c>
     </row>
     <row r="26" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P26" s="62">
+      <c r="P26" s="61">
         <v>115</v>
       </c>
-      <c r="Q26" s="55">
+      <c r="Q26" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P26)-COUNTIF(Notas!D:D,"&lt;="&amp;P25)</f>
         <v>0</v>
       </c>
@@ -16005,10 +16169,10 @@
         <f>EXP((P26-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T26" s="62">
+      <c r="T26" s="61">
         <v>230</v>
       </c>
-      <c r="U26" s="55">
+      <c r="U26" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T26)-COUNTIF(Notas!D:D,"&lt;="&amp;T25)</f>
         <v>0</v>
       </c>
@@ -16018,10 +16182,10 @@
       </c>
     </row>
     <row r="27" spans="16:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P27" s="62">
+      <c r="P27" s="61">
         <v>120</v>
       </c>
-      <c r="Q27" s="55">
+      <c r="Q27" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P27)-COUNTIF(Notas!D:D,"&lt;="&amp;P26)</f>
         <v>0</v>
       </c>
@@ -16029,10 +16193,10 @@
         <f>EXP((P27-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T27" s="63">
+      <c r="T27" s="62">
         <v>240</v>
       </c>
-      <c r="U27" s="64">
+      <c r="U27" s="63">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T27)-COUNTIF(Notas!D:D,"&lt;="&amp;T26)</f>
         <v>0</v>
       </c>
@@ -16042,10 +16206,10 @@
       </c>
     </row>
     <row r="28" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P28" s="62">
+      <c r="P28" s="61">
         <v>125</v>
       </c>
-      <c r="Q28" s="55">
+      <c r="Q28" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P28)-COUNTIF(Notas!D:D,"&lt;="&amp;P27)</f>
         <v>0</v>
       </c>
@@ -16060,10 +16224,10 @@
       </c>
     </row>
     <row r="29" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P29" s="62">
+      <c r="P29" s="61">
         <v>130</v>
       </c>
-      <c r="Q29" s="55">
+      <c r="Q29" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P29)-COUNTIF(Notas!D:D,"&lt;="&amp;P28)</f>
         <v>1</v>
       </c>
@@ -16073,10 +16237,10 @@
       </c>
     </row>
     <row r="30" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P30" s="62">
+      <c r="P30" s="61">
         <v>135</v>
       </c>
-      <c r="Q30" s="55">
+      <c r="Q30" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P30)-COUNTIF(Notas!D:D,"&lt;="&amp;P29)</f>
         <v>0</v>
       </c>
@@ -16086,10 +16250,10 @@
       </c>
     </row>
     <row r="31" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P31" s="62">
+      <c r="P31" s="61">
         <v>140</v>
       </c>
-      <c r="Q31" s="55">
+      <c r="Q31" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P31)-COUNTIF(Notas!D:D,"&lt;="&amp;P30)</f>
         <v>0</v>
       </c>
@@ -16099,10 +16263,10 @@
       </c>
     </row>
     <row r="32" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P32" s="62">
+      <c r="P32" s="61">
         <v>145</v>
       </c>
-      <c r="Q32" s="55">
+      <c r="Q32" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P32)-COUNTIF(Notas!D:D,"&lt;="&amp;P31)</f>
         <v>0</v>
       </c>
@@ -16112,10 +16276,10 @@
       </c>
     </row>
     <row r="33" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P33" s="62">
+      <c r="P33" s="61">
         <v>150</v>
       </c>
-      <c r="Q33" s="55">
+      <c r="Q33" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P33)-COUNTIF(Notas!D:D,"&lt;="&amp;P32)</f>
         <v>0</v>
       </c>
@@ -16125,10 +16289,10 @@
       </c>
     </row>
     <row r="34" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P34" s="62">
+      <c r="P34" s="61">
         <v>155</v>
       </c>
-      <c r="Q34" s="55">
+      <c r="Q34" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P34)-COUNTIF(Notas!D:D,"&lt;="&amp;P33)</f>
         <v>0</v>
       </c>
@@ -16138,10 +16302,10 @@
       </c>
     </row>
     <row r="35" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P35" s="62">
+      <c r="P35" s="61">
         <v>160</v>
       </c>
-      <c r="Q35" s="55">
+      <c r="Q35" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P35)-COUNTIF(Notas!D:D,"&lt;="&amp;P34)</f>
         <v>0</v>
       </c>
@@ -16151,10 +16315,10 @@
       </c>
     </row>
     <row r="36" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P36" s="62">
+      <c r="P36" s="61">
         <v>165</v>
       </c>
-      <c r="Q36" s="55">
+      <c r="Q36" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P36)-COUNTIF(Notas!D:D,"&lt;="&amp;P35)</f>
         <v>0</v>
       </c>
@@ -16164,10 +16328,10 @@
       </c>
     </row>
     <row r="37" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P37" s="62">
+      <c r="P37" s="61">
         <v>170</v>
       </c>
-      <c r="Q37" s="55">
+      <c r="Q37" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P37)-COUNTIF(Notas!D:D,"&lt;="&amp;P36)</f>
         <v>0</v>
       </c>
@@ -16177,10 +16341,10 @@
       </c>
     </row>
     <row r="38" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P38" s="62">
+      <c r="P38" s="61">
         <v>175</v>
       </c>
-      <c r="Q38" s="55">
+      <c r="Q38" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P38)-COUNTIF(Notas!D:D,"&lt;="&amp;P37)</f>
         <v>0</v>
       </c>
@@ -16190,10 +16354,10 @@
       </c>
     </row>
     <row r="39" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P39" s="62">
+      <c r="P39" s="61">
         <v>180</v>
       </c>
-      <c r="Q39" s="55">
+      <c r="Q39" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P39)-COUNTIF(Notas!D:D,"&lt;="&amp;P38)</f>
         <v>0</v>
       </c>
@@ -16203,10 +16367,10 @@
       </c>
     </row>
     <row r="40" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P40" s="62">
+      <c r="P40" s="61">
         <v>185</v>
       </c>
-      <c r="Q40" s="55">
+      <c r="Q40" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P40)-COUNTIF(Notas!D:D,"&lt;="&amp;P39)</f>
         <v>0</v>
       </c>
@@ -16216,10 +16380,10 @@
       </c>
     </row>
     <row r="41" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P41" s="62">
+      <c r="P41" s="61">
         <v>190</v>
       </c>
-      <c r="Q41" s="55">
+      <c r="Q41" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P41)-COUNTIF(Notas!D:D,"&lt;="&amp;P40)</f>
         <v>0</v>
       </c>
@@ -16229,10 +16393,10 @@
       </c>
     </row>
     <row r="42" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P42" s="62">
+      <c r="P42" s="61">
         <v>195</v>
       </c>
-      <c r="Q42" s="55">
+      <c r="Q42" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P42)-COUNTIF(Notas!D:D,"&lt;="&amp;P41)</f>
         <v>0</v>
       </c>
@@ -16242,10 +16406,10 @@
       </c>
     </row>
     <row r="43" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P43" s="62">
+      <c r="P43" s="61">
         <v>200</v>
       </c>
-      <c r="Q43" s="55">
+      <c r="Q43" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P43)-COUNTIF(Notas!D:D,"&lt;="&amp;P42)</f>
         <v>0</v>
       </c>
@@ -16255,10 +16419,10 @@
       </c>
     </row>
     <row r="44" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P44" s="62">
+      <c r="P44" s="61">
         <v>205</v>
       </c>
-      <c r="Q44" s="55">
+      <c r="Q44" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P44)-COUNTIF(Notas!D:D,"&lt;="&amp;P43)</f>
         <v>0</v>
       </c>
@@ -16268,10 +16432,10 @@
       </c>
     </row>
     <row r="45" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P45" s="62">
+      <c r="P45" s="61">
         <v>210</v>
       </c>
-      <c r="Q45" s="55">
+      <c r="Q45" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P45)-COUNTIF(Notas!D:D,"&lt;="&amp;P44)</f>
         <v>0</v>
       </c>
@@ -16281,10 +16445,10 @@
       </c>
     </row>
     <row r="46" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P46" s="62">
+      <c r="P46" s="61">
         <v>215</v>
       </c>
-      <c r="Q46" s="55">
+      <c r="Q46" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P46)-COUNTIF(Notas!D:D,"&lt;="&amp;P45)</f>
         <v>0</v>
       </c>
@@ -16294,10 +16458,10 @@
       </c>
     </row>
     <row r="47" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P47" s="62">
+      <c r="P47" s="61">
         <v>220</v>
       </c>
-      <c r="Q47" s="55">
+      <c r="Q47" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P47)-COUNTIF(Notas!D:D,"&lt;="&amp;P46)</f>
         <v>0</v>
       </c>
@@ -16307,10 +16471,10 @@
       </c>
     </row>
     <row r="48" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P48" s="62">
+      <c r="P48" s="61">
         <v>225</v>
       </c>
-      <c r="Q48" s="55">
+      <c r="Q48" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P48)-COUNTIF(Notas!D:D,"&lt;="&amp;P47)</f>
         <v>0</v>
       </c>
@@ -16320,10 +16484,10 @@
       </c>
     </row>
     <row r="49" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P49" s="62">
+      <c r="P49" s="61">
         <v>230</v>
       </c>
-      <c r="Q49" s="55">
+      <c r="Q49" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P49)-COUNTIF(Notas!D:D,"&lt;="&amp;P48)</f>
         <v>0</v>
       </c>
@@ -16333,10 +16497,10 @@
       </c>
     </row>
     <row r="50" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P50" s="62">
+      <c r="P50" s="61">
         <v>235</v>
       </c>
-      <c r="Q50" s="55">
+      <c r="Q50" s="54">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P50)-COUNTIF(Notas!D:D,"&lt;="&amp;P49)</f>
         <v>0</v>
       </c>
@@ -16346,10 +16510,10 @@
       </c>
     </row>
     <row r="51" spans="16:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P51" s="63">
+      <c r="P51" s="62">
         <v>240</v>
       </c>
-      <c r="Q51" s="64">
+      <c r="Q51" s="63">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P51)-COUNTIF(Notas!D:D,"&lt;="&amp;P50)</f>
         <v>0</v>
       </c>
@@ -16424,16 +16588,16 @@
       <c r="C6" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="64" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="40" t="s">
@@ -16448,23 +16612,23 @@
         <f>C8/2</f>
         <v>0</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <f>COUNTIF(Notas!G:G,B7)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="70">
+      <c r="E7" s="69">
         <f>LOG(_xlfn.NORM.DIST($B7,$E$3,SQRT($E$4),TRUE)^$C7)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="70">
+      <c r="F7" s="69">
         <f>LOG(_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE)^D7)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="42">
         <f>_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE)*Pelis</f>
         <v>5.7925488621560443E-3</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="50">
         <f>_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)*Pelis</f>
         <v>1.0670751456919622E-5</v>
       </c>
@@ -16477,23 +16641,23 @@
         <f>COUNTIF(Notas!B:B,B8)/2</f>
         <v>0</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="46">
         <f>COUNTIF(Notas!G:G,B8)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="71">
+      <c r="E8" s="70">
         <f>LOG((_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE))^C8)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="71">
+      <c r="F8" s="70">
         <f>LOG((_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE))^$D8)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="43">
         <f t="shared" ref="G8:G26" si="0">(_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE))*Pelis</f>
         <v>5.3035236315983354E-3</v>
       </c>
-      <c r="H8" s="52">
+      <c r="H8" s="51">
         <f t="shared" ref="H8:H26" si="1">(_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE))*Pelis</f>
         <v>8.9532107336445599E-6</v>
       </c>
@@ -16506,23 +16670,23 @@
         <f>(C8+C10)/2</f>
         <v>0.25</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="46">
         <f>COUNTIF(Notas!G:G,B9)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="71">
+      <c r="E9" s="70">
         <f t="shared" ref="E9:E26" si="2">LOG((_xlfn.NORM.DIST(B9,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE))^C9)</f>
         <v>-0.510165965966482</v>
       </c>
-      <c r="F9" s="71">
+      <c r="F9" s="70">
         <f t="shared" ref="F9:F26" si="3">LOG((_xlfn.NORM.DIST(B9,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE))^$D9)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="43">
         <f t="shared" si="0"/>
         <v>9.1061780178500785E-3</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="51">
         <f t="shared" si="1"/>
         <v>4.6530954287035938E-5</v>
       </c>
@@ -16535,23 +16699,23 @@
         <f>COUNTIF(Notas!B:B,B10)/2</f>
         <v>0.5</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="46">
         <f>COUNTIF(Notas!G:G,B10)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="71">
+        <v>1</v>
+      </c>
+      <c r="E10" s="70">
         <f t="shared" si="2"/>
         <v>-0.91513515531428258</v>
       </c>
-      <c r="F10" s="71">
+      <c r="F10" s="70">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="44">
+        <v>-3.6826615796688</v>
+      </c>
+      <c r="G10" s="43">
         <f t="shared" si="0"/>
         <v>1.478188057990508E-2</v>
       </c>
-      <c r="H10" s="52">
+      <c r="H10" s="51">
         <f t="shared" si="1"/>
         <v>2.0765310065299676E-4</v>
       </c>
@@ -16564,23 +16728,23 @@
         <f>(C10+C12)/2</f>
         <v>0.25</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="46">
         <f>COUNTIF(Notas!G:G,B11)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="71">
+      <c r="E11" s="70">
         <f t="shared" si="2"/>
         <v>-0.41106363090054054</v>
       </c>
-      <c r="F11" s="71">
+      <c r="F11" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="43">
         <f t="shared" si="0"/>
         <v>2.2685349595145655E-2</v>
       </c>
-      <c r="H11" s="52">
+      <c r="H11" s="51">
         <f t="shared" si="1"/>
         <v>7.9576485490160656E-4</v>
       </c>
@@ -16593,23 +16757,23 @@
         <f>COUNTIF(Notas!B:B,B12)/2</f>
         <v>0</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="46">
         <f>COUNTIF(Notas!G:G,B12)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="71">
+      <c r="E12" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="71">
+      <c r="F12" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G12" s="44">
+      <c r="G12" s="43">
         <f t="shared" si="0"/>
         <v>3.2914235407240124E-2</v>
       </c>
-      <c r="H12" s="52">
+      <c r="H12" s="51">
         <f t="shared" si="1"/>
         <v>2.6187638771519059E-3</v>
       </c>
@@ -16622,23 +16786,23 @@
         <f>(C12+C14)/2</f>
         <v>0</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="46">
         <f>COUNTIF(Notas!G:G,B13)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="71">
+      <c r="E13" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F13" s="71">
+      <c r="F13" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="43">
         <f t="shared" si="0"/>
         <v>4.5148654453109976E-2</v>
       </c>
-      <c r="H13" s="52">
+      <c r="H13" s="51">
         <f t="shared" si="1"/>
         <v>7.400945940858444E-3</v>
       </c>
@@ -16651,23 +16815,23 @@
         <f>COUNTIF(Notas!B:B,B14)/2</f>
         <v>0</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="46">
         <f>COUNTIF(Notas!G:G,B14)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="71">
+      <c r="E14" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F14" s="71">
+      <c r="F14" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G14" s="44">
+      <c r="G14" s="43">
         <f t="shared" si="0"/>
         <v>5.8550256516192611E-2</v>
       </c>
-      <c r="H14" s="52">
+      <c r="H14" s="51">
         <f t="shared" si="1"/>
         <v>1.796263352278547E-2</v>
       </c>
@@ -16680,23 +16844,23 @@
         <f>(C14+C16)/2</f>
         <v>0</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="46">
         <f>COUNTIF(Notas!G:G,B15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="71">
+      <c r="E15" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F15" s="71">
+      <c r="F15" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G15" s="44">
+      <c r="G15" s="43">
         <f t="shared" si="0"/>
         <v>7.1785364468036045E-2</v>
       </c>
-      <c r="H15" s="52">
+      <c r="H15" s="51">
         <f t="shared" si="1"/>
         <v>3.744170915363889E-2</v>
       </c>
@@ -16709,23 +16873,23 @@
         <f>COUNTIF(Notas!B:B,B16)/2</f>
         <v>0</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="46">
         <f>COUNTIF(Notas!G:G,B16)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="71">
+      <c r="E16" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F16" s="71">
+      <c r="F16" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G16" s="44">
+      <c r="G16" s="43">
         <f t="shared" si="0"/>
         <v>8.320822664083477E-2</v>
       </c>
-      <c r="H16" s="52">
+      <c r="H16" s="51">
         <f t="shared" si="1"/>
         <v>6.7027571512691578E-2</v>
       </c>
@@ -16738,23 +16902,23 @@
         <f>(C16+C18)/2</f>
         <v>0</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="46">
         <f>COUNTIF(Notas!G:G,B17)</f>
-        <v>1</v>
-      </c>
-      <c r="E17" s="71">
+        <v>0</v>
+      </c>
+      <c r="E17" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F17" s="71">
+      <c r="F17" s="70">
         <f t="shared" si="3"/>
-        <v>-0.98692905260139052</v>
-      </c>
-      <c r="G17" s="44">
+        <v>0</v>
+      </c>
+      <c r="G17" s="43">
         <f t="shared" si="0"/>
         <v>9.1184278782524775E-2</v>
       </c>
-      <c r="H17" s="52">
+      <c r="H17" s="51">
         <f t="shared" si="1"/>
         <v>0.10305544605641351</v>
       </c>
@@ -16767,23 +16931,23 @@
         <f>COUNTIF(Notas!B:B,B18)/2</f>
         <v>0</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D18" s="46">
         <f>COUNTIF(Notas!G:G,B18)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="71">
+      <c r="E18" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18" s="71">
+      <c r="F18" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G18" s="44">
+      <c r="G18" s="43">
         <f t="shared" si="0"/>
         <v>9.4470686747302468E-2</v>
       </c>
-      <c r="H18" s="52">
+      <c r="H18" s="51">
         <f t="shared" si="1"/>
         <v>0.13608606230328921</v>
       </c>
@@ -16796,23 +16960,23 @@
         <f>(C18+C20)/2</f>
         <v>0</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="46">
         <f>COUNTIF(Notas!G:G,B19)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="71">
+      <c r="E19" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F19" s="71">
+      <c r="F19" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G19" s="44">
+      <c r="G19" s="43">
         <f t="shared" si="0"/>
         <v>9.2533204903991528E-2</v>
       </c>
-      <c r="H19" s="52">
+      <c r="H19" s="51">
         <f t="shared" si="1"/>
         <v>0.15434239427286445</v>
       </c>
@@ -16825,23 +16989,23 @@
         <f>COUNTIF(Notas!B:B,B20)/2</f>
         <v>0</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="46">
         <f>COUNTIF(Notas!G:G,B20)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="71">
+      <c r="E20" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F20" s="71">
+      <c r="F20" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G20" s="44">
+      <c r="G20" s="43">
         <f t="shared" si="0"/>
         <v>8.5688304490451506E-2</v>
       </c>
-      <c r="H20" s="52">
+      <c r="H20" s="51">
         <f t="shared" si="1"/>
         <v>0.15034443690384314</v>
       </c>
@@ -16854,23 +17018,23 @@
         <f>(C20+C22)/2</f>
         <v>0</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D21" s="46">
         <f>COUNTIF(Notas!G:G,B21)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="71">
+      <c r="E21" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F21" s="71">
+      <c r="F21" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G21" s="44">
+      <c r="G21" s="43">
         <f t="shared" si="0"/>
         <v>7.5018583302613351E-2</v>
       </c>
-      <c r="H21" s="52">
+      <c r="H21" s="51">
         <f t="shared" si="1"/>
         <v>0.12578234601277249</v>
       </c>
@@ -16883,23 +17047,23 @@
         <f>COUNTIF(Notas!B:B,B22)/2</f>
         <v>0</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="46">
         <f>COUNTIF(Notas!G:G,B22)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="71">
+      <c r="E22" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F22" s="71">
+      <c r="F22" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G22" s="44">
+      <c r="G22" s="43">
         <f t="shared" si="0"/>
         <v>6.2092542712243848E-2</v>
       </c>
-      <c r="H22" s="52">
+      <c r="H22" s="51">
         <f t="shared" si="1"/>
         <v>9.0381567263075557E-2</v>
       </c>
@@ -16912,23 +17076,23 @@
         <f>(C22+C24)/2</f>
         <v>0</v>
       </c>
-      <c r="D23" s="47">
+      <c r="D23" s="46">
         <f>COUNTIF(Notas!G:G,B23)</f>
         <v>0</v>
       </c>
-      <c r="E23" s="71">
+      <c r="E23" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23" s="71">
+      <c r="F23" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G23" s="44">
+      <c r="G23" s="43">
         <f t="shared" si="0"/>
         <v>4.8588465796543967E-2</v>
       </c>
-      <c r="H23" s="52">
+      <c r="H23" s="51">
         <f t="shared" si="1"/>
         <v>5.5778081184472583E-2</v>
       </c>
@@ -16941,23 +17105,23 @@
         <f>COUNTIF(Notas!B:B,B24)/2</f>
         <v>0</v>
       </c>
-      <c r="D24" s="47">
+      <c r="D24" s="46">
         <f>COUNTIF(Notas!G:G,B24)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="71">
+      <c r="E24" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24" s="71">
+      <c r="F24" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G24" s="44">
+      <c r="G24" s="43">
         <f t="shared" si="0"/>
         <v>3.5945946585823285E-2</v>
       </c>
-      <c r="H24" s="52">
+      <c r="H24" s="51">
         <f t="shared" si="1"/>
         <v>2.9564091935930681E-2</v>
       </c>
@@ -16970,23 +17134,23 @@
         <f>(C24+C26)/2</f>
         <v>0</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="46">
         <f>COUNTIF(Notas!G:G,B25)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="71">
+      <c r="E25" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25" s="71">
+      <c r="F25" s="70">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G25" s="44">
+      <c r="G25" s="43">
         <f t="shared" si="0"/>
         <v>2.5141400473080999E-2</v>
       </c>
-      <c r="H25" s="52">
+      <c r="H25" s="51">
         <f t="shared" si="1"/>
         <v>1.345781882502084E-2</v>
       </c>
@@ -16999,23 +17163,23 @@
         <f>COUNTIF(Notas!B:B,B26)/2</f>
         <v>0</v>
       </c>
-      <c r="D26" s="48">
+      <c r="D26" s="47">
         <f>COUNTIF(Notas!G:G,B26)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="72">
+      <c r="E26" s="71">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F26" s="72">
+      <c r="F26" s="71">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G26" s="45">
+      <c r="G26" s="44">
         <f t="shared" si="0"/>
         <v>1.6624614389095349E-2</v>
       </c>
-      <c r="H26" s="53">
+      <c r="H26" s="52">
         <f t="shared" si="1"/>
         <v>5.2611911884490326E-3</v>
       </c>
@@ -17027,7 +17191,7 @@
       </c>
       <c r="F28">
         <f>SUM(F7:F26)</f>
-        <v>-0.98692905260139052</v>
+        <v>-3.6826615796688</v>
       </c>
     </row>
   </sheetData>
@@ -17046,21 +17210,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="73"/>
+    <col min="2" max="2" width="11.42578125" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="73">
+      <c r="B1" s="72">
         <f>AVERAGE(Visionados)</f>
         <v>26047</v>
       </c>
       <c r="D1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="73">
+      <c r="E1" s="72">
         <f>MAX(Visionados)</f>
         <v>26047</v>
       </c>
@@ -17069,7 +17233,7 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="73">
+      <c r="B2" s="72">
         <f>MEDIAN(Visionados)</f>
         <v>26047</v>
       </c>
@@ -17085,7 +17249,7 @@
       <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="74">
+      <c r="B4" s="73">
         <v>62533</v>
       </c>
       <c r="C4" t="s">

</xml_diff>

<commit_message>
Delete borders in reescala
</commit_message>
<xml_diff>
--- a/res/Readdata/Plantilla.xlsx
+++ b/res/Readdata/Plantilla.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7287BA-BC8B-4F97-A7AB-B4CF1E3E08E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E1AEC5-5890-4D82-8D6E-5D763BC59F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -526,19 +526,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -783,17 +770,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -829,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -847,16 +823,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -865,95 +839,93 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -964,6 +936,12 @@
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="26">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
@@ -1171,34 +1149,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="166" formatCode="0.0"/>
     </dxf>
     <dxf>
@@ -1369,7 +1319,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>4.0219169802939234</c:v>
+                  <c:v>3.9809247423692589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1381,7 +1331,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.7385316934738819</c:v>
+                  <c:v>1.978746940923525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2346,7 +2296,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.7385316934738819</c:v>
+                  <c:v>1.978746940923525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5154,7 +5104,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.7385316934738819</c:v>
+                  <c:v>1.978746940923525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13892,26 +13842,26 @@
     <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="15">
       <calculatedColumnFormula>C2+(RAND()-0.5)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="14">
   <autoFilter ref="B3:F13" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="12">
       <calculatedColumnFormula>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="10">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B3,MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="9">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13920,18 +13870,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="B19:F39" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="4">
       <calculatedColumnFormula>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="3">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="2">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B20,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14205,24 +14155,24 @@
   <dimension ref="A1:AE165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="17" customWidth="1"/>
     <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="72" customWidth="1"/>
-    <col min="5" max="6" width="12.140625" style="72" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="70" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" style="70" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="79" customWidth="1"/>
-    <col min="11" max="12" width="7.42578125" style="30" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="77" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="75" customWidth="1"/>
+    <col min="11" max="12" width="7.42578125" style="28" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="68" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="68" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" style="52" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" customWidth="1"/>
     <col min="17" max="17" width="8.28515625" customWidth="1"/>
     <col min="18" max="18" width="8.85546875" customWidth="1"/>
@@ -14246,10 +14196,10 @@
       <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="70" t="s">
         <v>55</v>
       </c>
       <c r="G1" t="s">
@@ -14261,7 +14211,7 @@
       <c r="I1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="29" t="s">
         <v>58</v>
       </c>
       <c r="K1" t="s">
@@ -14270,30 +14220,30 @@
       <c r="L1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="77" t="s">
+      <c r="N1" s="68" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+      <c r="A2" s="17">
         <v>555555</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="17">
         <v>2</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2" s="72">
+      <c r="D2" s="70">
         <v>130</v>
       </c>
-      <c r="E2" s="72">
+      <c r="E2" s="70">
         <v>26047</v>
       </c>
-      <c r="F2" s="80">
+      <c r="F2" s="76">
         <v>2.1</v>
       </c>
       <c r="G2">
@@ -14308,277 +14258,277 @@
         <f t="shared" ref="I2" si="1">ABS(H2)</f>
         <v>2</v>
       </c>
-      <c r="J2" s="79">
+      <c r="J2" s="75">
         <f t="shared" ref="J2" si="2">IF($H2&gt;0,1,0.1)</f>
         <v>0.1</v>
       </c>
-      <c r="K2" s="30">
+      <c r="K2" s="28">
         <f t="shared" ref="K2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>1.7385316934738819</v>
-      </c>
-      <c r="L2" s="30">
+        <v>1.978746940923525</v>
+      </c>
+      <c r="L2" s="28">
         <f t="shared" ref="L2" ca="1" si="4">C2+(RAND()-0.5)/10</f>
-        <v>4.0219169802939234</v>
-      </c>
-      <c r="M2" s="17">
+        <v>3.9809247423692589</v>
+      </c>
+      <c r="M2" s="68">
         <f t="shared" ref="M2" si="5">(B2-1)*10/9</f>
         <v>1.1111111111111112</v>
       </c>
-      <c r="N2" s="78">
+      <c r="N2" s="68">
         <f t="shared" ref="N2" si="6">(C2-1)*10/9</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="27"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="25"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="27"/>
-      <c r="V4" s="55"/>
-      <c r="W4" s="55"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="25"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="V5" s="55"/>
-      <c r="W5" s="55"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
       <c r="AE5" s="1"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="V6" s="55"/>
-      <c r="W6" s="55"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="V7" s="55"/>
-      <c r="W7" s="55"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="V8" s="55"/>
-      <c r="W8" s="55"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="V8" s="53"/>
+      <c r="W8" s="53"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="55"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="53"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="V10" s="55"/>
-      <c r="W10" s="55"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="V10" s="53"/>
+      <c r="W10" s="53"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="V11" s="55"/>
-      <c r="W11" s="55"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="V11" s="53"/>
+      <c r="W11" s="53"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="V12" s="55"/>
-      <c r="W12" s="55"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="V12" s="53"/>
+      <c r="W12" s="53"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="V13" s="55"/>
-      <c r="W13" s="55"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="V13" s="53"/>
+      <c r="W13" s="53"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="V14" s="55"/>
-      <c r="W14" s="55"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="27"/>
-      <c r="V15" s="55"/>
-      <c r="W15" s="55"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="V16" s="55"/>
-      <c r="W16" s="55"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
     </row>
     <row r="17" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V17" s="55"/>
-      <c r="W17" s="55"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
     </row>
     <row r="18" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V18" s="55"/>
-      <c r="W18" s="55"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
     </row>
     <row r="19" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V19" s="55"/>
-      <c r="W19" s="55"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
     </row>
     <row r="20" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V20" s="55"/>
-      <c r="W20" s="55"/>
+      <c r="V20" s="53"/>
+      <c r="W20" s="53"/>
     </row>
     <row r="21" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V21" s="55"/>
-      <c r="W21" s="55"/>
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
     </row>
     <row r="22" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V22" s="55"/>
-      <c r="W22" s="55"/>
+      <c r="V22" s="53"/>
+      <c r="W22" s="53"/>
     </row>
     <row r="23" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V23" s="55"/>
-      <c r="W23" s="55"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
     </row>
     <row r="24" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V24" s="55"/>
-      <c r="W24" s="55"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
     </row>
     <row r="25" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V25" s="55"/>
-      <c r="W25" s="55"/>
+      <c r="V25" s="53"/>
+      <c r="W25" s="53"/>
     </row>
     <row r="26" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V26" s="55"/>
-      <c r="W26" s="55"/>
+      <c r="V26" s="53"/>
+      <c r="W26" s="53"/>
     </row>
     <row r="27" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V27" s="55"/>
-      <c r="W27" s="55"/>
+      <c r="V27" s="53"/>
+      <c r="W27" s="53"/>
     </row>
     <row r="28" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V28" s="55"/>
-      <c r="W28" s="55"/>
+      <c r="V28" s="53"/>
+      <c r="W28" s="53"/>
     </row>
     <row r="29" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V29" s="55"/>
-      <c r="W29" s="55"/>
+      <c r="V29" s="53"/>
+      <c r="W29" s="53"/>
     </row>
     <row r="30" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V30" s="55"/>
-      <c r="W30" s="55"/>
+      <c r="V30" s="53"/>
+      <c r="W30" s="53"/>
     </row>
     <row r="31" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V31" s="55"/>
-      <c r="W31" s="55"/>
+      <c r="V31" s="53"/>
+      <c r="W31" s="53"/>
     </row>
     <row r="32" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V32" s="55"/>
-      <c r="W32" s="55"/>
+      <c r="V32" s="53"/>
+      <c r="W32" s="53"/>
     </row>
     <row r="33" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V33" s="55"/>
-      <c r="W33" s="55"/>
+      <c r="V33" s="53"/>
+      <c r="W33" s="53"/>
     </row>
     <row r="34" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V34" s="55"/>
-      <c r="W34" s="55"/>
+      <c r="V34" s="53"/>
+      <c r="W34" s="53"/>
     </row>
     <row r="35" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V35" s="55"/>
-      <c r="W35" s="55"/>
+      <c r="V35" s="53"/>
+      <c r="W35" s="53"/>
     </row>
     <row r="36" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V36" s="55"/>
-      <c r="W36" s="55"/>
+      <c r="V36" s="53"/>
+      <c r="W36" s="53"/>
     </row>
     <row r="37" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V37" s="55"/>
-      <c r="W37" s="55"/>
+      <c r="V37" s="53"/>
+      <c r="W37" s="53"/>
     </row>
     <row r="38" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V38" s="55"/>
-      <c r="W38" s="55"/>
+      <c r="V38" s="53"/>
+      <c r="W38" s="53"/>
     </row>
     <row r="39" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V39" s="55"/>
-      <c r="W39" s="55"/>
+      <c r="V39" s="53"/>
+      <c r="W39" s="53"/>
     </row>
     <row r="40" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V40" s="55"/>
-      <c r="W40" s="55"/>
+      <c r="V40" s="53"/>
+      <c r="W40" s="53"/>
     </row>
     <row r="41" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V41" s="55"/>
-      <c r="W41" s="55"/>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
     </row>
     <row r="42" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V42" s="55"/>
-      <c r="W42" s="55"/>
+      <c r="V42" s="53"/>
+      <c r="W42" s="53"/>
     </row>
     <row r="43" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V43" s="54"/>
-      <c r="W43" s="54"/>
+      <c r="V43" s="52"/>
+      <c r="W43" s="52"/>
     </row>
     <row r="44" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V44" s="54"/>
-      <c r="W44" s="54"/>
+      <c r="V44" s="52"/>
+      <c r="W44" s="52"/>
     </row>
     <row r="45" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V45" s="54"/>
-      <c r="W45" s="54"/>
+      <c r="V45" s="52"/>
+      <c r="W45" s="52"/>
     </row>
     <row r="46" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V46" s="54"/>
-      <c r="W46" s="54"/>
+      <c r="V46" s="52"/>
+      <c r="W46" s="52"/>
     </row>
     <row r="47" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V47" s="54"/>
-      <c r="W47" s="54"/>
+      <c r="V47" s="52"/>
+      <c r="W47" s="52"/>
     </row>
     <row r="48" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V48" s="54"/>
-      <c r="W48" s="54"/>
+      <c r="V48" s="52"/>
+      <c r="W48" s="52"/>
     </row>
     <row r="49" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V49" s="54"/>
-      <c r="W49" s="54"/>
+      <c r="V49" s="52"/>
+      <c r="W49" s="52"/>
     </row>
     <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14659,7 +14609,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="27"/>
+    <col min="5" max="5" width="11.42578125" style="25"/>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
@@ -14672,7 +14622,7 @@
         <f>COUNT(Tabla1[Mia])</f>
         <v>1</v>
       </c>
-      <c r="G1" s="27"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -14682,7 +14632,7 @@
         <f>COUNT(Tabla1[FA])</f>
         <v>1</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -14699,21 +14649,21 @@
         <f>STDEVP(Tabla1[FA])</f>
         <v>0</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="8">
         <f>_xlfn.VAR.P(Tabla1[FA])</f>
         <v>0</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="26" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="7">
         <f>MEDIAN(Tabla1[FA])</f>
         <v>4</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="27" t="s">
         <v>22</v>
       </c>
       <c r="J3" s="7" t="e">
@@ -14723,14 +14673,14 @@
       <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="57">
+      <c r="L3" s="55">
         <f>MAX(Tabla1[FA])</f>
         <v>4</v>
       </c>
       <c r="M3" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="57">
+      <c r="N3" s="55">
         <f>MIN(Notas!C:C)</f>
         <v>4</v>
       </c>
@@ -14750,21 +14700,21 @@
         <f>STDEVP(NotasMias)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="6">
         <f>_xlfn.VAR.P(NotasMias)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="26" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="5">
         <f>MEDIAN(NotasMias)</f>
         <v>2</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="27" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="5" t="e">
@@ -14774,14 +14724,14 @@
       <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="58">
+      <c r="L4" s="56">
         <f>MAX(NotasMias)</f>
         <v>2</v>
       </c>
       <c r="M4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="58">
+      <c r="N4" s="56">
         <f>MIN(NotasMias)</f>
         <v>2</v>
       </c>
@@ -14794,7 +14744,7 @@
         <f>AVERAGE(Tabla1[Diferencia])</f>
         <v>-2</v>
       </c>
-      <c r="G5" s="27"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -14811,9 +14761,9 @@
         <f>STDEVP(Tabla1[Diferencia_abs])</f>
         <v>0</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="29"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -14826,12 +14776,12 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="32" t="e">
+      <c r="D8" s="30" t="e">
         <f>CORREL(Notas!B:B,Notas!C:C)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="32"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -14861,8 +14811,8 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F14" s="27"/>
-      <c r="G14" s="27" t="s">
+      <c r="F14" s="25"/>
+      <c r="G14" s="25" t="s">
         <v>65</v>
       </c>
       <c r="H14" t="s">
@@ -14879,17 +14829,17 @@
       <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="76">
+      <c r="F15" s="25"/>
+      <c r="G15" s="74">
         <v>7.8</v>
       </c>
-      <c r="H15" s="94">
+      <c r="H15" s="90">
         <v>1000</v>
       </c>
-      <c r="I15" s="94">
+      <c r="I15" s="90">
         <v>90</v>
       </c>
-      <c r="J15" s="95">
+      <c r="J15" s="91">
         <v>1.6</v>
       </c>
     </row>
@@ -14908,23 +14858,23 @@
         <f>STDEVP(Tabla1[FA_rees])</f>
         <v>0</v>
       </c>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65" t="s">
+      <c r="E16" s="63"/>
+      <c r="F16" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="74">
+      <c r="G16" s="72">
         <f>COUNTIF(NotasFA,"&lt;="&amp;G15)/Pelis_con_nota</f>
         <v>1</v>
       </c>
-      <c r="H16" s="74">
+      <c r="H16" s="72">
         <f>COUNTIF(Tabla1[Visionados],"&lt;="&amp;H15)/Pelis_con_nota</f>
         <v>0</v>
       </c>
-      <c r="I16" s="74">
+      <c r="I16" s="72">
         <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;I15)/Pelis_con_nota</f>
         <v>0</v>
       </c>
-      <c r="J16" s="74">
+      <c r="J16" s="72">
         <f>COUNTIF(Tabla1[Varianza_FA],"&lt;="&amp;J15)/Pelis_con_nota</f>
         <v>0</v>
       </c>
@@ -14944,30 +14894,30 @@
         <f>STDEVP(Tabla1[Mia_rees])</f>
         <v>0</v>
       </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65" t="s">
+      <c r="E17" s="63"/>
+      <c r="F17" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="75">
+      <c r="G17" s="73">
         <f>COUNTIF(NotasMias,"&lt;="&amp;G15)/Pelis</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14993,45 +14943,45 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="85" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="81">
+      <c r="B4" s="77">
         <v>1</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="19">
         <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
         <v>0</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <f>COUNTIF(NotasFA,"&lt;=([@[Puntos]]+0,5)")</f>
         <v>0</v>
       </c>
-      <c r="E4" s="42" t="e">
+      <c r="E4" s="40" t="e">
         <f>_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F4" s="66" t="e">
+      <c r="F4" s="64" t="e">
         <f>_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="82">
+      <c r="B5" s="78">
         <v>2</v>
       </c>
       <c r="C5" s="3">
@@ -15042,17 +14992,17 @@
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
         <v>0</v>
       </c>
-      <c r="E5" s="43" t="e">
+      <c r="E5" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F5" s="84" t="e">
+      <c r="F5" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="82">
+      <c r="B6" s="78">
         <v>3</v>
       </c>
       <c r="C6" s="3">
@@ -15063,17 +15013,17 @@
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
         <v>0</v>
       </c>
-      <c r="E6" s="43" t="e">
+      <c r="E6" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F6" s="84" t="e">
+      <c r="F6" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="82">
+      <c r="B7" s="78">
         <v>4</v>
       </c>
       <c r="C7" s="3">
@@ -15084,17 +15034,17 @@
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
         <v>1</v>
       </c>
-      <c r="E7" s="43" t="e">
+      <c r="E7" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F7" s="84" t="e">
+      <c r="F7" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="82">
+      <c r="B8" s="78">
         <v>5</v>
       </c>
       <c r="C8" s="3">
@@ -15105,17 +15055,17 @@
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
         <v>0</v>
       </c>
-      <c r="E8" s="43" t="e">
+      <c r="E8" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F8" s="84" t="e">
+      <c r="F8" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="82">
+      <c r="B9" s="78">
         <v>6</v>
       </c>
       <c r="C9" s="3">
@@ -15126,17 +15076,17 @@
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
         <v>0</v>
       </c>
-      <c r="E9" s="43" t="e">
+      <c r="E9" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F9" s="84" t="e">
+      <c r="F9" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="82">
+      <c r="B10" s="78">
         <v>7</v>
       </c>
       <c r="C10" s="3">
@@ -15147,17 +15097,17 @@
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
         <v>0</v>
       </c>
-      <c r="E10" s="43" t="e">
+      <c r="E10" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F10" s="84" t="e">
+      <c r="F10" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="82">
+      <c r="B11" s="78">
         <v>8</v>
       </c>
       <c r="C11" s="3">
@@ -15168,17 +15118,17 @@
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
         <v>0</v>
       </c>
-      <c r="E11" s="43" t="e">
+      <c r="E11" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F11" s="84" t="e">
+      <c r="F11" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="82">
+      <c r="B12" s="78">
         <v>9</v>
       </c>
       <c r="C12" s="3">
@@ -15189,511 +15139,511 @@
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
         <v>0</v>
       </c>
-      <c r="E12" s="43" t="e">
+      <c r="E12" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F12" s="84" t="e">
+      <c r="F12" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="83">
+      <c r="B13" s="79">
         <v>10</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="22">
         <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
         <v>0</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="24">
         <f ca="1">COUNTIF(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="43" t="e">
+      <c r="E13" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F13" s="84" t="e">
+      <c r="F13" s="80" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="66" t="e">
+      <c r="E14" s="64" t="e">
         <f>SUM(E4:E13)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F14" s="66" t="e">
+      <c r="F14" s="64" t="e">
         <f>SUM(F4:F13)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="19" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="85" t="s">
+      <c r="B19" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="86" t="s">
+      <c r="C19" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="92" t="s">
+      <c r="D19" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="E19" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="92" t="s">
+      <c r="F19" s="88" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="81">
+      <c r="B20" s="77">
         <v>0.5</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="33">
         <f>C21/2</f>
         <v>0</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="43">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E20" s="42" t="e">
+      <c r="E20" s="40" t="e">
         <f>(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F20" s="90" t="e">
+      <c r="F20" s="86" t="e">
         <f>_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
       <c r="R20" t="s">
         <v>30</v>
       </c>
-      <c r="S20" s="32" t="e" cm="1">
+      <c r="S20" s="30" t="e" cm="1">
         <f t="array" aca="1" ref="S20" ca="1">_xlfn.CHISQ.DIST(SUM((C22:C39-E22:E39)^2/E22:E39),18,TRUE)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="82">
+      <c r="B21" s="78">
         <v>1</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0</v>
       </c>
-      <c r="D21" s="46">
+      <c r="D21" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E21" s="43" t="e">
+      <c r="E21" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F21" s="91" t="e">
+      <c r="F21" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
       <c r="R21" t="s">
         <v>31</v>
       </c>
-      <c r="S21" s="32" t="e" cm="1">
+      <c r="S21" s="30" t="e" cm="1">
         <f t="array" aca="1" ref="S21" ca="1">_xlfn.CHISQ.DIST(SUM((D25:D39-F25:F39)^2/F25:F39),18,TRUE)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="82">
+      <c r="B22" s="78">
         <v>1.5</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0.25</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D22" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E22" s="43" t="e">
+      <c r="E22" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F22" s="91" t="e">
+      <c r="F22" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="82">
+      <c r="B23" s="78">
         <v>2</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0.5</v>
       </c>
-      <c r="D23" s="46">
+      <c r="D23" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E23" s="43" t="e">
+      <c r="E23" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F23" s="91" t="e">
+      <c r="F23" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="82">
+      <c r="B24" s="78">
         <v>2.5</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0.25</v>
       </c>
-      <c r="D24" s="46">
+      <c r="D24" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E24" s="43" t="e">
+      <c r="E24" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F24" s="91" t="e">
+      <c r="F24" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="82">
+      <c r="B25" s="78">
         <v>3</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C25" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0</v>
       </c>
-      <c r="D25" s="46">
+      <c r="D25" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E25" s="43" t="e">
+      <c r="E25" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F25" s="91" t="e">
+      <c r="F25" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="82">
+      <c r="B26" s="78">
         <v>3.5</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0</v>
       </c>
-      <c r="D26" s="46">
+      <c r="D26" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E26" s="43" t="e">
+      <c r="E26" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F26" s="91" t="e">
+      <c r="F26" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="82">
+      <c r="B27" s="78">
         <v>4</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0</v>
       </c>
-      <c r="D27" s="46">
+      <c r="D27" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>1</v>
       </c>
-      <c r="E27" s="43" t="e">
+      <c r="E27" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F27" s="91" t="e">
+      <c r="F27" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="82">
+      <c r="B28" s="78">
         <v>4.5</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C28" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0</v>
       </c>
-      <c r="D28" s="46">
+      <c r="D28" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E28" s="43" t="e">
+      <c r="E28" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F28" s="91" t="e">
+      <c r="F28" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="82">
+      <c r="B29" s="78">
         <v>5</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C29" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0</v>
       </c>
-      <c r="D29" s="46">
+      <c r="D29" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E29" s="43" t="e">
+      <c r="E29" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F29" s="91" t="e">
+      <c r="F29" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="82">
+      <c r="B30" s="78">
         <v>5.5</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C30" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0</v>
       </c>
-      <c r="D30" s="46">
+      <c r="D30" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E30" s="43" t="e">
+      <c r="E30" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F30" s="91" t="e">
+      <c r="F30" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="82">
+      <c r="B31" s="78">
         <v>6</v>
       </c>
-      <c r="C31" s="36">
+      <c r="C31" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0</v>
       </c>
-      <c r="D31" s="46">
+      <c r="D31" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E31" s="43" t="e">
+      <c r="E31" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F31" s="91" t="e">
+      <c r="F31" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="82">
+      <c r="B32" s="78">
         <v>6.5</v>
       </c>
-      <c r="C32" s="36">
+      <c r="C32" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0</v>
       </c>
-      <c r="D32" s="46">
+      <c r="D32" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E32" s="43" t="e">
+      <c r="E32" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F32" s="91" t="e">
+      <c r="F32" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="82">
+      <c r="B33" s="78">
         <v>7</v>
       </c>
-      <c r="C33" s="36">
+      <c r="C33" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0</v>
       </c>
-      <c r="D33" s="46">
+      <c r="D33" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E33" s="43" t="e">
+      <c r="E33" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F33" s="91" t="e">
+      <c r="F33" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="82">
+      <c r="B34" s="78">
         <v>7.5</v>
       </c>
-      <c r="C34" s="36">
+      <c r="C34" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0</v>
       </c>
-      <c r="D34" s="46">
+      <c r="D34" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E34" s="43" t="e">
+      <c r="E34" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F34" s="91" t="e">
+      <c r="F34" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="82">
+      <c r="B35" s="78">
         <v>8</v>
       </c>
-      <c r="C35" s="36">
+      <c r="C35" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0</v>
       </c>
-      <c r="D35" s="46">
+      <c r="D35" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E35" s="43" t="e">
+      <c r="E35" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F35" s="91" t="e">
+      <c r="F35" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="82">
+      <c r="B36" s="78">
         <v>8.5</v>
       </c>
-      <c r="C36" s="36">
+      <c r="C36" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0</v>
       </c>
-      <c r="D36" s="46">
+      <c r="D36" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E36" s="43" t="e">
+      <c r="E36" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F36" s="91" t="e">
+      <c r="F36" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="82">
+      <c r="B37" s="78">
         <v>9</v>
       </c>
-      <c r="C37" s="36">
+      <c r="C37" s="34">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
         <v>0</v>
       </c>
-      <c r="D37" s="46">
+      <c r="D37" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E37" s="43" t="e">
+      <c r="E37" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F37" s="91" t="e">
+      <c r="F37" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="82">
+      <c r="B38" s="78">
         <v>9.5</v>
       </c>
-      <c r="C38" s="36">
+      <c r="C38" s="34">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
         <v>0</v>
       </c>
-      <c r="D38" s="46">
+      <c r="D38" s="44">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E38" s="43" t="e">
+      <c r="E38" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F38" s="91" t="e">
+      <c r="F38" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="83">
+      <c r="B39" s="79">
         <v>10</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="35">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])*2/3</f>
         <v>0</v>
       </c>
-      <c r="D39" s="47">
+      <c r="D39" s="45">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
         <v>0</v>
       </c>
-      <c r="E39" s="43" t="e">
+      <c r="E39" s="41" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F39" s="91" t="e">
+      <c r="F39" s="87" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="49">
+      <c r="C40" s="47">
         <f ca="1">SUM(Normal_continua[Yo])</f>
         <v>1</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="17">
         <f>SUM(Normal_continua[FilmAffinity])</f>
         <v>1</v>
       </c>
-      <c r="E40" s="66" t="e">
+      <c r="E40" s="64" t="e">
         <f>SUM(Normal_continua[Normal Yo])</f>
         <v>#NUM!</v>
       </c>
-      <c r="F40" s="66" t="e">
+      <c r="F40" s="64" t="e">
         <f>SUM(Normal_continua[Normal F.A.])</f>
         <v>#NUM!</v>
       </c>
@@ -15731,11 +15681,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="56"/>
+      <c r="A1" s="54"/>
       <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="19">
+      <c r="F1" s="17">
         <f>AVERAGE(Tabla1[Duracion])</f>
         <v>130</v>
       </c>
@@ -15762,14 +15712,14 @@
       <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="17">
         <f>AVERAGEIF(Tabla1[Duracion],"&gt;50")</f>
         <v>130</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="19" cm="1">
+      <c r="H2" s="17" cm="1">
         <f t="array" ref="H2">STDEVP(IF(Tabla1[Duracion]&gt;50,Tabla1[Duracion]))</f>
         <v>0</v>
       </c>
@@ -15785,7 +15735,7 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="19" t="e">
+      <c r="F3" s="17" t="e">
         <f>_xlfn.VAR.S(Tabla1[Duracion])</f>
         <v>#DIV/0!</v>
       </c>
@@ -15810,895 +15760,895 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F4" s="19"/>
-      <c r="P4" s="59">
+      <c r="F4" s="17"/>
+      <c r="P4" s="57">
         <v>5</v>
       </c>
-      <c r="Q4" s="60">
+      <c r="Q4" s="58">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P4)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="41" t="e">
+      <c r="R4" s="39" t="e">
         <f>EXP((P4-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T4" s="59">
+      <c r="T4" s="57">
         <v>10</v>
       </c>
-      <c r="U4" s="60">
+      <c r="U4" s="58">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T4)</f>
         <v>0</v>
       </c>
-      <c r="V4" s="41" t="e">
+      <c r="V4" s="39" t="e">
         <f>EXP((T4-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P5" s="61">
+      <c r="P5" s="59">
         <v>10</v>
       </c>
-      <c r="Q5" s="54">
+      <c r="Q5" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P5)-COUNTIF(Notas!D:D,"&lt;="&amp;P4)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="33" t="e">
+      <c r="R5" s="31" t="e">
         <f>EXP((P5-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T5" s="61">
+      <c r="T5" s="59">
         <v>20</v>
       </c>
-      <c r="U5" s="54">
+      <c r="U5" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T5)-COUNTIF(Notas!D:D,"&lt;="&amp;T4)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="33" t="e">
+      <c r="V5" s="31" t="e">
         <f t="shared" ref="V5:V27" si="0">EXP((T5-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P6" s="61">
+      <c r="P6" s="59">
         <v>15</v>
       </c>
-      <c r="Q6" s="54">
+      <c r="Q6" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P6)-COUNTIF(Notas!D:D,"&lt;="&amp;P5)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="33" t="e">
+      <c r="R6" s="31" t="e">
         <f>EXP((P6-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T6" s="61">
+      <c r="T6" s="59">
         <v>30</v>
       </c>
-      <c r="U6" s="54">
+      <c r="U6" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T6)-COUNTIF(Notas!D:D,"&lt;="&amp;T5)</f>
         <v>0</v>
       </c>
-      <c r="V6" s="33" t="e">
+      <c r="V6" s="31" t="e">
         <f>_xlfn.NORM.DIST($T6,$F$2,SQRT($H$2),TRUE)*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P7" s="61">
+      <c r="P7" s="59">
         <v>20</v>
       </c>
-      <c r="Q7" s="54">
+      <c r="Q7" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P7)-COUNTIF(Notas!D:D,"&lt;="&amp;P6)</f>
         <v>0</v>
       </c>
-      <c r="R7" s="33" t="e">
+      <c r="R7" s="31" t="e">
         <f>EXP((P7-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T7" s="61">
+      <c r="T7" s="59">
         <v>40</v>
       </c>
-      <c r="U7" s="54">
+      <c r="U7" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T7)-COUNTIF(Notas!D:D,"&lt;="&amp;T6)</f>
         <v>0</v>
       </c>
-      <c r="V7" s="33" t="e">
+      <c r="V7" s="31" t="e">
         <f>(_xlfn.NORM.DIST($T7,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($T6,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P8" s="61">
+      <c r="P8" s="59">
         <v>25</v>
       </c>
-      <c r="Q8" s="54">
+      <c r="Q8" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P8)-COUNTIF(Notas!D:D,"&lt;="&amp;P7)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="33" t="e">
+      <c r="R8" s="31" t="e">
         <f>EXP((P8-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T8" s="61">
+      <c r="T8" s="59">
         <v>50</v>
       </c>
-      <c r="U8" s="54">
+      <c r="U8" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T8)-COUNTIF(Notas!D:D,"&lt;="&amp;T7)</f>
         <v>0</v>
       </c>
-      <c r="V8" s="33" t="e">
+      <c r="V8" s="31" t="e">
         <f t="shared" ref="V8:V26" si="1">(_xlfn.NORM.DIST($T8,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($T7,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P9" s="61">
+      <c r="P9" s="59">
         <v>30</v>
       </c>
-      <c r="Q9" s="54">
+      <c r="Q9" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P9)-COUNTIF(Notas!D:D,"&lt;="&amp;P8)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="33" t="e">
+      <c r="R9" s="31" t="e">
         <f>EXP((P9-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="61">
+      <c r="T9" s="59">
         <v>60</v>
       </c>
-      <c r="U9" s="54">
+      <c r="U9" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T9)-COUNTIF(Notas!D:D,"&lt;="&amp;T8)</f>
         <v>0</v>
       </c>
-      <c r="V9" s="33" t="e">
+      <c r="V9" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P10" s="61">
+      <c r="P10" s="59">
         <v>35</v>
       </c>
-      <c r="Q10" s="54">
+      <c r="Q10" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P10)-COUNTIF(Notas!D:D,"&lt;="&amp;P9)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="33" t="e">
+      <c r="R10" s="31" t="e">
         <f>EXP((P10-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T10" s="61">
+      <c r="T10" s="59">
         <v>70</v>
       </c>
-      <c r="U10" s="54">
+      <c r="U10" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T10)-COUNTIF(Notas!D:D,"&lt;="&amp;T9)</f>
         <v>0</v>
       </c>
-      <c r="V10" s="33" t="e">
+      <c r="V10" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P11" s="61">
+      <c r="P11" s="59">
         <v>40</v>
       </c>
-      <c r="Q11" s="54">
+      <c r="Q11" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P11)-COUNTIF(Notas!D:D,"&lt;="&amp;P10)</f>
         <v>0</v>
       </c>
-      <c r="R11" s="33" t="e">
+      <c r="R11" s="31" t="e">
         <f>EXP((P11-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T11" s="61">
+      <c r="T11" s="59">
         <v>80</v>
       </c>
-      <c r="U11" s="54">
+      <c r="U11" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T11)-COUNTIF(Notas!D:D,"&lt;="&amp;T10)</f>
         <v>0</v>
       </c>
-      <c r="V11" s="33" t="e">
+      <c r="V11" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P12" s="61">
+      <c r="P12" s="59">
         <v>45</v>
       </c>
-      <c r="Q12" s="54">
+      <c r="Q12" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P12)-COUNTIF(Notas!D:D,"&lt;="&amp;P11)</f>
         <v>0</v>
       </c>
-      <c r="R12" s="33" t="e">
+      <c r="R12" s="31" t="e">
         <f>EXP((P12-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T12" s="61">
+      <c r="T12" s="59">
         <v>90</v>
       </c>
-      <c r="U12" s="54">
+      <c r="U12" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T12)-COUNTIF(Notas!D:D,"&lt;="&amp;T11)</f>
         <v>0</v>
       </c>
-      <c r="V12" s="33" t="e">
+      <c r="V12" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P13" s="61">
+      <c r="P13" s="59">
         <v>50</v>
       </c>
-      <c r="Q13" s="54">
+      <c r="Q13" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P13)-COUNTIF(Notas!D:D,"&lt;="&amp;P12)</f>
         <v>0</v>
       </c>
-      <c r="R13" s="33" t="e">
+      <c r="R13" s="31" t="e">
         <f>EXP((P13-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T13" s="61">
+      <c r="T13" s="59">
         <v>100</v>
       </c>
-      <c r="U13" s="54">
+      <c r="U13" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T13)-COUNTIF(Notas!D:D,"&lt;="&amp;T12)</f>
         <v>0</v>
       </c>
-      <c r="V13" s="33" t="e">
+      <c r="V13" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P14" s="61">
+      <c r="P14" s="59">
         <v>55</v>
       </c>
-      <c r="Q14" s="54">
+      <c r="Q14" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P14)-COUNTIF(Notas!D:D,"&lt;="&amp;P13)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="33" t="e">
+      <c r="R14" s="31" t="e">
         <f>EXP((P14-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T14" s="61">
+      <c r="T14" s="59">
         <v>110</v>
       </c>
-      <c r="U14" s="54">
+      <c r="U14" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T14)-COUNTIF(Notas!D:D,"&lt;="&amp;T13)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="33" t="e">
+      <c r="V14" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P15" s="61">
+      <c r="P15" s="59">
         <v>60</v>
       </c>
-      <c r="Q15" s="54">
+      <c r="Q15" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P15)-COUNTIF(Notas!D:D,"&lt;="&amp;P14)</f>
         <v>0</v>
       </c>
-      <c r="R15" s="33" t="e">
+      <c r="R15" s="31" t="e">
         <f>EXP((P15-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T15" s="61">
+      <c r="T15" s="59">
         <v>120</v>
       </c>
-      <c r="U15" s="54">
+      <c r="U15" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T15)-COUNTIF(Notas!D:D,"&lt;="&amp;T14)</f>
         <v>0</v>
       </c>
-      <c r="V15" s="33" t="e">
+      <c r="V15" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P16" s="61">
+      <c r="P16" s="59">
         <v>65</v>
       </c>
-      <c r="Q16" s="54">
+      <c r="Q16" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P16)-COUNTIF(Notas!D:D,"&lt;="&amp;P15)</f>
         <v>0</v>
       </c>
-      <c r="R16" s="33" t="e">
+      <c r="R16" s="31" t="e">
         <f>EXP((P16-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T16" s="61">
+      <c r="T16" s="59">
         <v>130</v>
       </c>
-      <c r="U16" s="54">
+      <c r="U16" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T16)-COUNTIF(Notas!D:D,"&lt;="&amp;T15)</f>
         <v>1</v>
       </c>
-      <c r="V16" s="33" t="e">
+      <c r="V16" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="17" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P17" s="61">
+      <c r="P17" s="59">
         <v>70</v>
       </c>
-      <c r="Q17" s="54">
+      <c r="Q17" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P17)-COUNTIF(Notas!D:D,"&lt;="&amp;P16)</f>
         <v>0</v>
       </c>
-      <c r="R17" s="33" t="e">
+      <c r="R17" s="31" t="e">
         <f>EXP((P17-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T17" s="61">
+      <c r="T17" s="59">
         <v>140</v>
       </c>
-      <c r="U17" s="54">
+      <c r="U17" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T17)-COUNTIF(Notas!D:D,"&lt;="&amp;T16)</f>
         <v>0</v>
       </c>
-      <c r="V17" s="33" t="e">
+      <c r="V17" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="18" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P18" s="61">
+      <c r="P18" s="59">
         <v>75</v>
       </c>
-      <c r="Q18" s="54">
+      <c r="Q18" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P18)-COUNTIF(Notas!D:D,"&lt;="&amp;P17)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="33" t="e">
+      <c r="R18" s="31" t="e">
         <f>EXP((P18-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T18" s="61">
+      <c r="T18" s="59">
         <v>150</v>
       </c>
-      <c r="U18" s="54">
+      <c r="U18" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T18)-COUNTIF(Notas!D:D,"&lt;="&amp;T17)</f>
         <v>0</v>
       </c>
-      <c r="V18" s="33" t="e">
+      <c r="V18" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="19" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P19" s="61">
+      <c r="P19" s="59">
         <v>80</v>
       </c>
-      <c r="Q19" s="54">
+      <c r="Q19" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P19)-COUNTIF(Notas!D:D,"&lt;="&amp;P18)</f>
         <v>0</v>
       </c>
-      <c r="R19" s="33" t="e">
+      <c r="R19" s="31" t="e">
         <f>EXP((P19-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T19" s="61">
+      <c r="T19" s="59">
         <v>160</v>
       </c>
-      <c r="U19" s="54">
+      <c r="U19" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T19)-COUNTIF(Notas!D:D,"&lt;="&amp;T18)</f>
         <v>0</v>
       </c>
-      <c r="V19" s="33" t="e">
+      <c r="V19" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="20" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P20" s="61">
+      <c r="P20" s="59">
         <v>85</v>
       </c>
-      <c r="Q20" s="54">
+      <c r="Q20" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P20)-COUNTIF(Notas!D:D,"&lt;="&amp;P19)</f>
         <v>0</v>
       </c>
-      <c r="R20" s="33" t="e">
+      <c r="R20" s="31" t="e">
         <f>EXP((P20-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T20" s="61">
+      <c r="T20" s="59">
         <v>170</v>
       </c>
-      <c r="U20" s="54">
+      <c r="U20" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T20)-COUNTIF(Notas!D:D,"&lt;="&amp;T19)</f>
         <v>0</v>
       </c>
-      <c r="V20" s="33" t="e">
+      <c r="V20" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="21" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P21" s="61">
+      <c r="P21" s="59">
         <v>90</v>
       </c>
-      <c r="Q21" s="54">
+      <c r="Q21" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P21)-COUNTIF(Notas!D:D,"&lt;="&amp;P20)</f>
         <v>0</v>
       </c>
-      <c r="R21" s="33" t="e">
+      <c r="R21" s="31" t="e">
         <f>EXP((P21-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T21" s="61">
+      <c r="T21" s="59">
         <v>180</v>
       </c>
-      <c r="U21" s="54">
+      <c r="U21" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T21)-COUNTIF(Notas!D:D,"&lt;="&amp;T20)</f>
         <v>0</v>
       </c>
-      <c r="V21" s="33" t="e">
+      <c r="V21" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="22" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P22" s="61">
+      <c r="P22" s="59">
         <v>95</v>
       </c>
-      <c r="Q22" s="54">
+      <c r="Q22" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P22)-COUNTIF(Notas!D:D,"&lt;="&amp;P21)</f>
         <v>0</v>
       </c>
-      <c r="R22" s="33" t="e">
+      <c r="R22" s="31" t="e">
         <f>EXP((P22-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T22" s="61">
+      <c r="T22" s="59">
         <v>190</v>
       </c>
-      <c r="U22" s="54">
+      <c r="U22" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T22)-COUNTIF(Notas!D:D,"&lt;="&amp;T21)</f>
         <v>0</v>
       </c>
-      <c r="V22" s="33" t="e">
+      <c r="V22" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="23" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P23" s="61">
+      <c r="P23" s="59">
         <v>100</v>
       </c>
-      <c r="Q23" s="54">
+      <c r="Q23" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P23)-COUNTIF(Notas!D:D,"&lt;="&amp;P22)</f>
         <v>0</v>
       </c>
-      <c r="R23" s="33" t="e">
+      <c r="R23" s="31" t="e">
         <f>EXP((P23-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T23" s="61">
+      <c r="T23" s="59">
         <v>200</v>
       </c>
-      <c r="U23" s="54">
+      <c r="U23" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T23)-COUNTIF(Notas!D:D,"&lt;="&amp;T22)</f>
         <v>0</v>
       </c>
-      <c r="V23" s="33" t="e">
+      <c r="V23" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="24" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P24" s="61">
+      <c r="P24" s="59">
         <v>105</v>
       </c>
-      <c r="Q24" s="54">
+      <c r="Q24" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P24)-COUNTIF(Notas!D:D,"&lt;="&amp;P23)</f>
         <v>0</v>
       </c>
-      <c r="R24" s="33" t="e">
+      <c r="R24" s="31" t="e">
         <f>EXP((P24-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T24" s="61">
+      <c r="T24" s="59">
         <v>210</v>
       </c>
-      <c r="U24" s="54">
+      <c r="U24" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T24)-COUNTIF(Notas!D:D,"&lt;="&amp;T23)</f>
         <v>0</v>
       </c>
-      <c r="V24" s="33" t="e">
+      <c r="V24" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="25" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P25" s="61">
+      <c r="P25" s="59">
         <v>110</v>
       </c>
-      <c r="Q25" s="54">
+      <c r="Q25" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P25)-COUNTIF(Notas!D:D,"&lt;="&amp;P24)</f>
         <v>0</v>
       </c>
-      <c r="R25" s="33" t="e">
+      <c r="R25" s="31" t="e">
         <f>EXP((P25-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T25" s="61">
+      <c r="T25" s="59">
         <v>220</v>
       </c>
-      <c r="U25" s="54">
+      <c r="U25" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T25)-COUNTIF(Notas!D:D,"&lt;="&amp;T24)</f>
         <v>0</v>
       </c>
-      <c r="V25" s="33" t="e">
+      <c r="V25" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="26" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P26" s="61">
+      <c r="P26" s="59">
         <v>115</v>
       </c>
-      <c r="Q26" s="54">
+      <c r="Q26" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P26)-COUNTIF(Notas!D:D,"&lt;="&amp;P25)</f>
         <v>0</v>
       </c>
-      <c r="R26" s="33" t="e">
+      <c r="R26" s="31" t="e">
         <f>EXP((P26-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T26" s="61">
+      <c r="T26" s="59">
         <v>230</v>
       </c>
-      <c r="U26" s="54">
+      <c r="U26" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T26)-COUNTIF(Notas!D:D,"&lt;="&amp;T25)</f>
         <v>0</v>
       </c>
-      <c r="V26" s="33" t="e">
+      <c r="V26" s="31" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="27" spans="16:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P27" s="61">
+      <c r="P27" s="59">
         <v>120</v>
       </c>
-      <c r="Q27" s="54">
+      <c r="Q27" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P27)-COUNTIF(Notas!D:D,"&lt;="&amp;P26)</f>
         <v>0</v>
       </c>
-      <c r="R27" s="33" t="e">
+      <c r="R27" s="31" t="e">
         <f>EXP((P27-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T27" s="62">
+      <c r="T27" s="60">
         <v>240</v>
       </c>
-      <c r="U27" s="63">
+      <c r="U27" s="61">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;T27)-COUNTIF(Notas!D:D,"&lt;="&amp;T26)</f>
         <v>0</v>
       </c>
-      <c r="V27" s="34" t="e">
+      <c r="V27" s="32" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P28" s="61">
+      <c r="P28" s="59">
         <v>125</v>
       </c>
-      <c r="Q28" s="54">
+      <c r="Q28" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P28)-COUNTIF(Notas!D:D,"&lt;="&amp;P27)</f>
         <v>0</v>
       </c>
-      <c r="R28" s="33" t="e">
+      <c r="R28" s="31" t="e">
         <f>EXP((P28-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T28" s="27"/>
-      <c r="V28" s="19" t="e">
+      <c r="T28" s="25"/>
+      <c r="V28" s="17" t="e">
         <f>SUM(V4:V27)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P29" s="61">
+      <c r="P29" s="59">
         <v>130</v>
       </c>
-      <c r="Q29" s="54">
+      <c r="Q29" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P29)-COUNTIF(Notas!D:D,"&lt;="&amp;P28)</f>
         <v>1</v>
       </c>
-      <c r="R29" s="33" t="e">
+      <c r="R29" s="31" t="e">
         <f>EXP((P29-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P30" s="61">
+      <c r="P30" s="59">
         <v>135</v>
       </c>
-      <c r="Q30" s="54">
+      <c r="Q30" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P30)-COUNTIF(Notas!D:D,"&lt;="&amp;P29)</f>
         <v>0</v>
       </c>
-      <c r="R30" s="33" t="e">
+      <c r="R30" s="31" t="e">
         <f>EXP((P30-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P31" s="61">
+      <c r="P31" s="59">
         <v>140</v>
       </c>
-      <c r="Q31" s="54">
+      <c r="Q31" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P31)-COUNTIF(Notas!D:D,"&lt;="&amp;P30)</f>
         <v>0</v>
       </c>
-      <c r="R31" s="33" t="e">
+      <c r="R31" s="31" t="e">
         <f>EXP((P31-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P32" s="61">
+      <c r="P32" s="59">
         <v>145</v>
       </c>
-      <c r="Q32" s="54">
+      <c r="Q32" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P32)-COUNTIF(Notas!D:D,"&lt;="&amp;P31)</f>
         <v>0</v>
       </c>
-      <c r="R32" s="33" t="e">
+      <c r="R32" s="31" t="e">
         <f>EXP((P32-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P33" s="61">
+      <c r="P33" s="59">
         <v>150</v>
       </c>
-      <c r="Q33" s="54">
+      <c r="Q33" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P33)-COUNTIF(Notas!D:D,"&lt;="&amp;P32)</f>
         <v>0</v>
       </c>
-      <c r="R33" s="33" t="e">
+      <c r="R33" s="31" t="e">
         <f>EXP((P33-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P34" s="61">
+      <c r="P34" s="59">
         <v>155</v>
       </c>
-      <c r="Q34" s="54">
+      <c r="Q34" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P34)-COUNTIF(Notas!D:D,"&lt;="&amp;P33)</f>
         <v>0</v>
       </c>
-      <c r="R34" s="33" t="e">
+      <c r="R34" s="31" t="e">
         <f>EXP((P34-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P35" s="61">
+      <c r="P35" s="59">
         <v>160</v>
       </c>
-      <c r="Q35" s="54">
+      <c r="Q35" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P35)-COUNTIF(Notas!D:D,"&lt;="&amp;P34)</f>
         <v>0</v>
       </c>
-      <c r="R35" s="33" t="e">
+      <c r="R35" s="31" t="e">
         <f>EXP((P35-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P36" s="61">
+      <c r="P36" s="59">
         <v>165</v>
       </c>
-      <c r="Q36" s="54">
+      <c r="Q36" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P36)-COUNTIF(Notas!D:D,"&lt;="&amp;P35)</f>
         <v>0</v>
       </c>
-      <c r="R36" s="33" t="e">
+      <c r="R36" s="31" t="e">
         <f>EXP((P36-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P37" s="61">
+      <c r="P37" s="59">
         <v>170</v>
       </c>
-      <c r="Q37" s="54">
+      <c r="Q37" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P37)-COUNTIF(Notas!D:D,"&lt;="&amp;P36)</f>
         <v>0</v>
       </c>
-      <c r="R37" s="33" t="e">
+      <c r="R37" s="31" t="e">
         <f>EXP((P37-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P38" s="61">
+      <c r="P38" s="59">
         <v>175</v>
       </c>
-      <c r="Q38" s="54">
+      <c r="Q38" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P38)-COUNTIF(Notas!D:D,"&lt;="&amp;P37)</f>
         <v>0</v>
       </c>
-      <c r="R38" s="33" t="e">
+      <c r="R38" s="31" t="e">
         <f>EXP((P38-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P39" s="61">
+      <c r="P39" s="59">
         <v>180</v>
       </c>
-      <c r="Q39" s="54">
+      <c r="Q39" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P39)-COUNTIF(Notas!D:D,"&lt;="&amp;P38)</f>
         <v>0</v>
       </c>
-      <c r="R39" s="33" t="e">
+      <c r="R39" s="31" t="e">
         <f>EXP((P39-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P40" s="61">
+      <c r="P40" s="59">
         <v>185</v>
       </c>
-      <c r="Q40" s="54">
+      <c r="Q40" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P40)-COUNTIF(Notas!D:D,"&lt;="&amp;P39)</f>
         <v>0</v>
       </c>
-      <c r="R40" s="33" t="e">
+      <c r="R40" s="31" t="e">
         <f>EXP((P40-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P41" s="61">
+      <c r="P41" s="59">
         <v>190</v>
       </c>
-      <c r="Q41" s="54">
+      <c r="Q41" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P41)-COUNTIF(Notas!D:D,"&lt;="&amp;P40)</f>
         <v>0</v>
       </c>
-      <c r="R41" s="33" t="e">
+      <c r="R41" s="31" t="e">
         <f>EXP((P41-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="42" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P42" s="61">
+      <c r="P42" s="59">
         <v>195</v>
       </c>
-      <c r="Q42" s="54">
+      <c r="Q42" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P42)-COUNTIF(Notas!D:D,"&lt;="&amp;P41)</f>
         <v>0</v>
       </c>
-      <c r="R42" s="33" t="e">
+      <c r="R42" s="31" t="e">
         <f>EXP((P42-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="43" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P43" s="61">
+      <c r="P43" s="59">
         <v>200</v>
       </c>
-      <c r="Q43" s="54">
+      <c r="Q43" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P43)-COUNTIF(Notas!D:D,"&lt;="&amp;P42)</f>
         <v>0</v>
       </c>
-      <c r="R43" s="33" t="e">
+      <c r="R43" s="31" t="e">
         <f>EXP((P43-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="44" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P44" s="61">
+      <c r="P44" s="59">
         <v>205</v>
       </c>
-      <c r="Q44" s="54">
+      <c r="Q44" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P44)-COUNTIF(Notas!D:D,"&lt;="&amp;P43)</f>
         <v>0</v>
       </c>
-      <c r="R44" s="33" t="e">
+      <c r="R44" s="31" t="e">
         <f>EXP((P44-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="45" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P45" s="61">
+      <c r="P45" s="59">
         <v>210</v>
       </c>
-      <c r="Q45" s="54">
+      <c r="Q45" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P45)-COUNTIF(Notas!D:D,"&lt;="&amp;P44)</f>
         <v>0</v>
       </c>
-      <c r="R45" s="33" t="e">
+      <c r="R45" s="31" t="e">
         <f>EXP((P45-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="46" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P46" s="61">
+      <c r="P46" s="59">
         <v>215</v>
       </c>
-      <c r="Q46" s="54">
+      <c r="Q46" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P46)-COUNTIF(Notas!D:D,"&lt;="&amp;P45)</f>
         <v>0</v>
       </c>
-      <c r="R46" s="33" t="e">
+      <c r="R46" s="31" t="e">
         <f>EXP((P46-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="47" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P47" s="61">
+      <c r="P47" s="59">
         <v>220</v>
       </c>
-      <c r="Q47" s="54">
+      <c r="Q47" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P47)-COUNTIF(Notas!D:D,"&lt;="&amp;P46)</f>
         <v>0</v>
       </c>
-      <c r="R47" s="33" t="e">
+      <c r="R47" s="31" t="e">
         <f>EXP((P47-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="48" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P48" s="61">
+      <c r="P48" s="59">
         <v>225</v>
       </c>
-      <c r="Q48" s="54">
+      <c r="Q48" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P48)-COUNTIF(Notas!D:D,"&lt;="&amp;P47)</f>
         <v>0</v>
       </c>
-      <c r="R48" s="33" t="e">
+      <c r="R48" s="31" t="e">
         <f>EXP((P48-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="49" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P49" s="61">
+      <c r="P49" s="59">
         <v>230</v>
       </c>
-      <c r="Q49" s="54">
+      <c r="Q49" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P49)-COUNTIF(Notas!D:D,"&lt;="&amp;P48)</f>
         <v>0</v>
       </c>
-      <c r="R49" s="33" t="e">
+      <c r="R49" s="31" t="e">
         <f>EXP((P49-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="50" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P50" s="61">
+      <c r="P50" s="59">
         <v>235</v>
       </c>
-      <c r="Q50" s="54">
+      <c r="Q50" s="52">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P50)-COUNTIF(Notas!D:D,"&lt;="&amp;P49)</f>
         <v>0</v>
       </c>
-      <c r="R50" s="33" t="e">
+      <c r="R50" s="31" t="e">
         <f>EXP((P50-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="51" spans="16:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P51" s="62">
+      <c r="P51" s="60">
         <v>240</v>
       </c>
-      <c r="Q51" s="63">
+      <c r="Q51" s="61">
         <f>COUNTIF(Notas!D:D,"&lt;="&amp;P51)-COUNTIF(Notas!D:D,"&lt;="&amp;P50)</f>
         <v>0</v>
       </c>
-      <c r="R51" s="34" t="e">
+      <c r="R51" s="32" t="e">
         <f>EXP((P51-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
         <v>#DIV/0!</v>
       </c>
@@ -16763,604 +16713,604 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="38" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
+      <c r="B7" s="18">
         <v>0.5</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="33">
         <f>C8/2</f>
         <v>0</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="43">
         <f>COUNTIF(Notas!G:G,B7)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="69">
+      <c r="E7" s="67">
         <f>LOG(_xlfn.NORM.DIST($B7,$E$3,SQRT($E$4),TRUE)^$C7)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="69">
+      <c r="F7" s="67">
         <f>LOG(_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE)^D7)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="40">
         <f>_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE)*Pelis</f>
         <v>5.7925488621560443E-3</v>
       </c>
-      <c r="H7" s="50">
+      <c r="H7" s="48">
         <f>_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)*Pelis</f>
         <v>1.0670751456919622E-5</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>1</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="34">
         <f>COUNTIF(Notas!B:B,B8)/2</f>
         <v>0</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="44">
         <f>COUNTIF(Notas!G:G,B8)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="68">
         <f>LOG((_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE))^C8)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="70">
+      <c r="F8" s="68">
         <f>LOG((_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE))^$D8)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="41">
         <f t="shared" ref="G8:G26" si="0">(_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE))*Pelis</f>
         <v>5.3035236315983354E-3</v>
       </c>
-      <c r="H8" s="51">
+      <c r="H8" s="49">
         <f t="shared" ref="H8:H26" si="1">(_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE))*Pelis</f>
         <v>8.9532107336445599E-6</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>1.5</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="34">
         <f>(C8+C10)/2</f>
         <v>0.25</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="44">
         <f>COUNTIF(Notas!G:G,B9)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="68">
         <f t="shared" ref="E9:E26" si="2">LOG((_xlfn.NORM.DIST(B9,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE))^C9)</f>
         <v>-0.510165965966482</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="68">
         <f t="shared" ref="F9:F26" si="3">LOG((_xlfn.NORM.DIST(B9,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE))^$D9)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="41">
         <f t="shared" si="0"/>
         <v>9.1061780178500785E-3</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="49">
         <f t="shared" si="1"/>
         <v>4.6530954287035938E-5</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>2</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="34">
         <f>COUNTIF(Notas!B:B,B10)/2</f>
         <v>0.5</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="44">
         <f>COUNTIF(Notas!G:G,B10)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="70">
+      <c r="E10" s="68">
         <f t="shared" si="2"/>
         <v>-0.91513515531428258</v>
       </c>
-      <c r="F10" s="70">
+      <c r="F10" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="41">
         <f t="shared" si="0"/>
         <v>1.478188057990508E-2</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="49">
         <f t="shared" si="1"/>
         <v>2.0765310065299676E-4</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>2.5</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="34">
         <f>(C10+C12)/2</f>
         <v>0.25</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="44">
         <f>COUNTIF(Notas!G:G,B11)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="70">
+      <c r="E11" s="68">
         <f t="shared" si="2"/>
         <v>-0.41106363090054054</v>
       </c>
-      <c r="F11" s="70">
+      <c r="F11" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="41">
         <f t="shared" si="0"/>
         <v>2.2685349595145655E-2</v>
       </c>
-      <c r="H11" s="51">
+      <c r="H11" s="49">
         <f t="shared" si="1"/>
         <v>7.9576485490160656E-4</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="22">
+      <c r="B12" s="20">
         <v>3</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="34">
         <f>COUNTIF(Notas!B:B,B12)/2</f>
         <v>0</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="44">
         <f>COUNTIF(Notas!G:G,B12)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="70">
+      <c r="F12" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="41">
         <f t="shared" si="0"/>
         <v>3.2914235407240124E-2</v>
       </c>
-      <c r="H12" s="51">
+      <c r="H12" s="49">
         <f t="shared" si="1"/>
         <v>2.6187638771519059E-3</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
+      <c r="B13" s="20">
         <v>3.5</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="34">
         <f>(C12+C14)/2</f>
         <v>0</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="44">
         <f>COUNTIF(Notas!G:G,B13)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="70">
+      <c r="E13" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F13" s="70">
+      <c r="F13" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="41">
         <f t="shared" si="0"/>
         <v>4.5148654453109976E-2</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H13" s="49">
         <f t="shared" si="1"/>
         <v>7.400945940858444E-3</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="22">
+      <c r="B14" s="20">
         <v>4</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="34">
         <f>COUNTIF(Notas!B:B,B14)/2</f>
         <v>0</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="44">
         <f>COUNTIF(Notas!G:G,B14)</f>
         <v>1</v>
       </c>
-      <c r="E14" s="70">
+      <c r="E14" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F14" s="70">
+      <c r="F14" s="68">
         <f t="shared" si="3"/>
         <v>-1.7456299905769432</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="41">
         <f t="shared" si="0"/>
         <v>5.8550256516192611E-2</v>
       </c>
-      <c r="H14" s="51">
+      <c r="H14" s="49">
         <f t="shared" si="1"/>
         <v>1.796263352278547E-2</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="22">
+      <c r="B15" s="20">
         <v>4.5</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="34">
         <f>(C14+C16)/2</f>
         <v>0</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="44">
         <f>COUNTIF(Notas!G:G,B15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="70">
+      <c r="E15" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F15" s="70">
+      <c r="F15" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="41">
         <f t="shared" si="0"/>
         <v>7.1785364468036045E-2</v>
       </c>
-      <c r="H15" s="51">
+      <c r="H15" s="49">
         <f t="shared" si="1"/>
         <v>3.744170915363889E-2</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="22">
+      <c r="B16" s="20">
         <v>5</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C16" s="34">
         <f>COUNTIF(Notas!B:B,B16)/2</f>
         <v>0</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="44">
         <f>COUNTIF(Notas!G:G,B16)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="70">
+      <c r="E16" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F16" s="70">
+      <c r="F16" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="41">
         <f t="shared" si="0"/>
         <v>8.320822664083477E-2</v>
       </c>
-      <c r="H16" s="51">
+      <c r="H16" s="49">
         <f t="shared" si="1"/>
         <v>6.7027571512691578E-2</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="22">
+      <c r="B17" s="20">
         <v>5.5</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="34">
         <f>(C16+C18)/2</f>
         <v>0</v>
       </c>
-      <c r="D17" s="46">
+      <c r="D17" s="44">
         <f>COUNTIF(Notas!G:G,B17)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="70">
+      <c r="E17" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F17" s="70">
+      <c r="F17" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="41">
         <f t="shared" si="0"/>
         <v>9.1184278782524775E-2</v>
       </c>
-      <c r="H17" s="51">
+      <c r="H17" s="49">
         <f t="shared" si="1"/>
         <v>0.10305544605641351</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="22">
+      <c r="B18" s="20">
         <v>6</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="34">
         <f>COUNTIF(Notas!B:B,B18)/2</f>
         <v>0</v>
       </c>
-      <c r="D18" s="46">
+      <c r="D18" s="44">
         <f>COUNTIF(Notas!G:G,B18)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="70">
+      <c r="E18" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18" s="70">
+      <c r="F18" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="41">
         <f t="shared" si="0"/>
         <v>9.4470686747302468E-2</v>
       </c>
-      <c r="H18" s="51">
+      <c r="H18" s="49">
         <f t="shared" si="1"/>
         <v>0.13608606230328921</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="22">
+      <c r="B19" s="20">
         <v>6.5</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="34">
         <f>(C18+C20)/2</f>
         <v>0</v>
       </c>
-      <c r="D19" s="46">
+      <c r="D19" s="44">
         <f>COUNTIF(Notas!G:G,B19)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="70">
+      <c r="E19" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F19" s="70">
+      <c r="F19" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="41">
         <f t="shared" si="0"/>
         <v>9.2533204903991528E-2</v>
       </c>
-      <c r="H19" s="51">
+      <c r="H19" s="49">
         <f t="shared" si="1"/>
         <v>0.15434239427286445</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="22">
+      <c r="B20" s="20">
         <v>7</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="34">
         <f>COUNTIF(Notas!B:B,B20)/2</f>
         <v>0</v>
       </c>
-      <c r="D20" s="46">
+      <c r="D20" s="44">
         <f>COUNTIF(Notas!G:G,B20)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="70">
+      <c r="E20" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F20" s="70">
+      <c r="F20" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="41">
         <f t="shared" si="0"/>
         <v>8.5688304490451506E-2</v>
       </c>
-      <c r="H20" s="51">
+      <c r="H20" s="49">
         <f t="shared" si="1"/>
         <v>0.15034443690384314</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="22">
+      <c r="B21" s="20">
         <v>7.5</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="34">
         <f>(C20+C22)/2</f>
         <v>0</v>
       </c>
-      <c r="D21" s="46">
+      <c r="D21" s="44">
         <f>COUNTIF(Notas!G:G,B21)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="70">
+      <c r="E21" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F21" s="70">
+      <c r="F21" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G21" s="43">
+      <c r="G21" s="41">
         <f t="shared" si="0"/>
         <v>7.5018583302613351E-2</v>
       </c>
-      <c r="H21" s="51">
+      <c r="H21" s="49">
         <f t="shared" si="1"/>
         <v>0.12578234601277249</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="22">
+      <c r="B22" s="20">
         <v>8</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="34">
         <f>COUNTIF(Notas!B:B,B22)/2</f>
         <v>0</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D22" s="44">
         <f>COUNTIF(Notas!G:G,B22)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="70">
+      <c r="E22" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F22" s="70">
+      <c r="F22" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G22" s="41">
         <f t="shared" si="0"/>
         <v>6.2092542712243848E-2</v>
       </c>
-      <c r="H22" s="51">
+      <c r="H22" s="49">
         <f t="shared" si="1"/>
         <v>9.0381567263075557E-2</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="22">
+      <c r="B23" s="20">
         <v>8.5</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="34">
         <f>(C22+C24)/2</f>
         <v>0</v>
       </c>
-      <c r="D23" s="46">
+      <c r="D23" s="44">
         <f>COUNTIF(Notas!G:G,B23)</f>
         <v>0</v>
       </c>
-      <c r="E23" s="70">
+      <c r="E23" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23" s="70">
+      <c r="F23" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G23" s="41">
         <f t="shared" si="0"/>
         <v>4.8588465796543967E-2</v>
       </c>
-      <c r="H23" s="51">
+      <c r="H23" s="49">
         <f t="shared" si="1"/>
         <v>5.5778081184472583E-2</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="22">
+      <c r="B24" s="20">
         <v>9</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="34">
         <f>COUNTIF(Notas!B:B,B24)/2</f>
         <v>0</v>
       </c>
-      <c r="D24" s="46">
+      <c r="D24" s="44">
         <f>COUNTIF(Notas!G:G,B24)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="70">
+      <c r="E24" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24" s="70">
+      <c r="F24" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="41">
         <f t="shared" si="0"/>
         <v>3.5945946585823285E-2</v>
       </c>
-      <c r="H24" s="51">
+      <c r="H24" s="49">
         <f t="shared" si="1"/>
         <v>2.9564091935930681E-2</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="22">
+      <c r="B25" s="20">
         <v>9.5</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C25" s="34">
         <f>(C24+C26)/2</f>
         <v>0</v>
       </c>
-      <c r="D25" s="46">
+      <c r="D25" s="44">
         <f>COUNTIF(Notas!G:G,B25)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="70">
+      <c r="E25" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25" s="70">
+      <c r="F25" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="41">
         <f t="shared" si="0"/>
         <v>2.5141400473080999E-2</v>
       </c>
-      <c r="H25" s="51">
+      <c r="H25" s="49">
         <f t="shared" si="1"/>
         <v>1.345781882502084E-2</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="23">
+      <c r="B26" s="21">
         <v>10</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="35">
         <f>COUNTIF(Notas!B:B,B26)/2</f>
         <v>0</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="45">
         <f>COUNTIF(Notas!G:G,B26)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="71">
+      <c r="E26" s="69">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F26" s="71">
+      <c r="F26" s="69">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G26" s="44">
+      <c r="G26" s="42">
         <f t="shared" si="0"/>
         <v>1.6624614389095349E-2</v>
       </c>
-      <c r="H26" s="52">
+      <c r="H26" s="50">
         <f t="shared" si="1"/>
         <v>5.2611911884490326E-3</v>
       </c>
@@ -17391,21 +17341,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="72"/>
+    <col min="2" max="2" width="11.42578125" style="70"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="72">
+      <c r="B1" s="70">
         <f>AVERAGE(Visionados)</f>
         <v>26047</v>
       </c>
       <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="72">
+      <c r="E1" s="70">
         <f>MAX(Visionados)</f>
         <v>26047</v>
       </c>
@@ -17414,7 +17364,7 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="72">
+      <c r="B2" s="70">
         <f>MEDIAN(Visionados)</f>
         <v>26047</v>
       </c>
@@ -17430,7 +17380,7 @@
       <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="73">
+      <c r="B4" s="71">
         <v>62533</v>
       </c>
       <c r="C4" t="s">

</xml_diff>

<commit_message>
Set graph and axes for times
</commit_message>
<xml_diff>
--- a/res/Readdata/Plantilla.xlsx
+++ b/res/Readdata/Plantilla.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E1AEC5-5890-4D82-8D6E-5D763BC59F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF2D21-12B9-409C-8AD3-06D28176AEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,12 +937,6 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -1149,6 +1143,12 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="0.0"/>
     </dxf>
     <dxf>
@@ -1319,7 +1319,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>3.9809247423692589</c:v>
+                  <c:v>3.9774943511835543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1331,7 +1331,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.978746940923525</c:v>
+                  <c:v>2.3189350035238765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2296,7 +2296,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.978746940923525</c:v>
+                  <c:v>2.3189350035238765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5104,7 +5104,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.978746940923525</c:v>
+                  <c:v>2.3189350035238765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5131,6 +5131,8 @@
         <c:axId val="747100992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="250"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5193,6 +5195,8 @@
         <c:axId val="747098696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5463,6 +5467,8 @@
         <c:axId val="747103616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="250"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5525,6 +5531,8 @@
         <c:axId val="747102304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5884,6 +5892,7 @@
         <c:axId val="871117216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="250"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -13623,16 +13632,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13842,26 +13851,26 @@
     <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="15">
       <calculatedColumnFormula>C2+(RAND()-0.5)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="12">
   <autoFilter ref="B3:F13" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="10">
       <calculatedColumnFormula>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="8">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B3,MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="7">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13870,18 +13879,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="B19:F39" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="2">
       <calculatedColumnFormula>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="1">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="0">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B20,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14264,11 +14273,11 @@
       </c>
       <c r="K2" s="28">
         <f t="shared" ref="K2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>1.978746940923525</v>
+        <v>2.3189350035238765</v>
       </c>
       <c r="L2" s="28">
         <f t="shared" ref="L2" ca="1" si="4">C2+(RAND()-0.5)/10</f>
-        <v>3.9809247423692589</v>
+        <v>3.9774943511835543</v>
       </c>
       <c r="M2" s="68">
         <f t="shared" ref="M2" si="5">(B2-1)*10/9</f>
@@ -14930,7 +14939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB957686-4157-457C-B9AD-66FD2970B9E3}">
   <dimension ref="B3:S40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -15664,7 +15673,7 @@
   <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17335,7 +17344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B5ED56-93C2-495B-9ED0-E04AF59C2259}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Delete unused time table
</commit_message>
<xml_diff>
--- a/res/Readdata/Plantilla.xlsx
+++ b/res/Readdata/Plantilla.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF2D21-12B9-409C-8AD3-06D28176AEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F269890-7171-4DFC-AC7B-EEEF919684F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notas" sheetId="3" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>Media filmafinity</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>Minutos</t>
-  </si>
-  <si>
-    <t>Normal</t>
   </si>
   <si>
     <t>Normal &gt;60</t>
@@ -937,6 +934,28 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FF33CC33"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -1195,28 +1214,6 @@
         </right>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF33CC33"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1319,7 +1316,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>3.9774943511835543</c:v>
+                  <c:v>4.0012738448308918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1331,7 +1328,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.3189350035238765</c:v>
+                  <c:v>1.8889473243090102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2296,7 +2293,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.3189350035238765</c:v>
+                  <c:v>1.8889473243090102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5104,7 +5101,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>2.3189350035238765</c:v>
+                  <c:v>1.8889473243090102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5710,7 +5707,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tiempos!$T$4:$T$27</c:f>
+              <c:f>Tiempos!$Q$4:$Q$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -5791,7 +5788,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tiempos!$U$4:$U$27</c:f>
+              <c:f>Tiempos!$R$4:$R$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -13832,45 +13829,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:N1048576" totalsRowShown="0" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:N1048576" totalsRowShown="0" tableBorderDxfId="25">
   <autoFilter ref="A1:N1048576" xr:uid="{B7E8E3F6-4A56-4C38-9CDA-83612E98463A}"/>
   <tableColumns count="14">
-    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="22"/>
-    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{65EE12B7-2552-4910-A353-7AE48A3D7AA6}" name="FA"/>
-    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{2E72113E-50BE-41C7-8BFD-59035950093F}" name="Varianza_FA" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{2E72113E-50BE-41C7-8BFD-59035950093F}" name="Varianza_FA" dataDxfId="20"/>
     <tableColumn id="5" xr3:uid="{FF19B5AE-C56B-4CA5-B812-840E5C110430}" name="FA_redondeo"/>
     <tableColumn id="6" xr3:uid="{20BAA72D-A773-488D-B544-DAD2EF762D99}" name="Diferencia"/>
     <tableColumn id="7" xr3:uid="{E40D682E-5136-4AEB-BEE2-B6B87967AFB0}" name="Diferencia_abs"/>
-    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me_ha_gustado" dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me_ha_gustado" dataDxfId="19">
       <calculatedColumnFormula>IF($H2&gt;0,1,0.1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia_ruido" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia_ruido" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="17">
       <calculatedColumnFormula>C2+(RAND()-0.5)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="14">
   <autoFilter ref="B3:F13" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="12">
       <calculatedColumnFormula>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="10">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B3,MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="9">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13879,18 +13876,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="B19:F39" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="4">
       <calculatedColumnFormula>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="3">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="2">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B20,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14163,7 +14160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8703B0C1-9812-4468-A745-94BA8D5548CD}">
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -14194,46 +14191,46 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="70" t="s">
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="N1" s="68" t="s">
         <v>61</v>
-      </c>
-      <c r="N1" s="68" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -14273,11 +14270,11 @@
       </c>
       <c r="K2" s="28">
         <f t="shared" ref="K2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>2.3189350035238765</v>
+        <v>1.8889473243090102</v>
       </c>
       <c r="L2" s="28">
         <f t="shared" ref="L2" ca="1" si="4">C2+(RAND()-0.5)/10</f>
-        <v>3.9774943511835543</v>
+        <v>4.0012738448308918</v>
       </c>
       <c r="M2" s="68">
         <f t="shared" ref="M2" si="5">(B2-1)*10/9</f>
@@ -14543,10 +14540,10 @@
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14635,7 +14632,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <f>COUNT(Tabla1[FA])</f>
@@ -14822,13 +14819,13 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F14" s="25"/>
       <c r="G14" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" t="s">
         <v>65</v>
-      </c>
-      <c r="H14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" t="s">
-        <v>66</v>
       </c>
       <c r="J14" t="s">
         <v>17</v>
@@ -14869,7 +14866,7 @@
       </c>
       <c r="E16" s="63"/>
       <c r="F16" s="63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="72">
         <f>COUNTIF(NotasFA,"&lt;="&amp;G15)/Pelis_con_nota</f>
@@ -14905,7 +14902,7 @@
       </c>
       <c r="E17" s="63"/>
       <c r="F17" s="63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G17" s="73">
         <f>COUNTIF(NotasMias,"&lt;="&amp;G15)/Pelis</f>
@@ -14953,7 +14950,7 @@
   <sheetData>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="81" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="82" t="s">
         <v>9</v>
@@ -15226,7 +15223,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S20" s="30" t="e" cm="1">
         <f t="array" aca="1" ref="S20" ca="1">_xlfn.CHISQ.DIST(SUM((C22:C39-E22:E39)^2/E22:E39),18,TRUE)</f>
@@ -15254,7 +15251,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S21" s="30" t="e" cm="1">
         <f t="array" aca="1" ref="S21" ca="1">_xlfn.CHISQ.DIST(SUM((D25:D39-F25:F39)^2/F25:F39),18,TRUE)</f>
@@ -15670,10 +15667,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB35113E-0C06-4EAF-8941-AA6250700856}">
-  <dimension ref="A1:V52"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15685,11 +15682,10 @@
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="54"/>
       <c r="E1" t="s">
         <v>15</v>
@@ -15706,14 +15702,14 @@
         <v>130</v>
       </c>
       <c r="L1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M1">
         <f>MAX(Tabla1[Duracion])</f>
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C2">
         <f>COUNTIF(Tabla1[Duracion],"&gt;50")</f>
         <v>1</v>
@@ -15726,21 +15722,21 @@
         <v>130</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="17" cm="1">
         <f t="array" ref="H2">STDEVP(IF(Tabla1[Duracion]&gt;50,Tabla1[Duracion]))</f>
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2">
         <f>MIN(Tabla1[Duracion])</f>
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>17</v>
       </c>
@@ -15749,926 +15745,336 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" cm="1">
         <f t="array" ref="H3">_xlfn.VAR.P(IF(Tabla1[Duracion]&gt;50,Tabla1[Duracion],))</f>
         <v>1.6117095947250967E-2</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>27</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>28</v>
       </c>
-      <c r="T3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V3" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F4" s="17"/>
-      <c r="P4" s="57">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="58">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P4)</f>
+      <c r="Q4" s="57">
+        <v>10</v>
+      </c>
+      <c r="R4" s="58">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q4)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="39" t="e">
-        <f>EXP((P4-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
+      <c r="S4" s="39" t="e">
+        <f>EXP((Q4-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T4" s="57">
-        <v>10</v>
-      </c>
-      <c r="U4" s="58">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T4)</f>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q5" s="59">
+        <v>20</v>
+      </c>
+      <c r="R5" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q5)-COUNTIF(Notas!D:D,"&lt;="&amp;Q4)</f>
         <v>0</v>
       </c>
-      <c r="V4" s="39" t="e">
-        <f>EXP((T4-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
+      <c r="S5" s="31" t="e">
+        <f t="shared" ref="S5:S27" si="0">EXP((Q5-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P5" s="59">
-        <v>10</v>
-      </c>
-      <c r="Q5" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P5)-COUNTIF(Notas!D:D,"&lt;="&amp;P4)</f>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q6" s="59">
+        <v>30</v>
+      </c>
+      <c r="R6" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q6)-COUNTIF(Notas!D:D,"&lt;="&amp;Q5)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="31" t="e">
-        <f>EXP((P5-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T5" s="59">
-        <v>20</v>
-      </c>
-      <c r="U5" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T5)-COUNTIF(Notas!D:D,"&lt;="&amp;T4)</f>
+      <c r="S6" s="31" t="e">
+        <f>_xlfn.NORM.DIST($Q6,$F$2,SQRT($H$2),TRUE)*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q7" s="59">
+        <v>40</v>
+      </c>
+      <c r="R7" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q7)-COUNTIF(Notas!D:D,"&lt;="&amp;Q6)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="31" t="e">
-        <f t="shared" ref="V5:V27" si="0">EXP((T5-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
-        <v>#DIV/0!</v>
+      <c r="S7" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q7,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q6,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P6" s="59">
-        <v>15</v>
-      </c>
-      <c r="Q6" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P6)-COUNTIF(Notas!D:D,"&lt;="&amp;P5)</f>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q8" s="59">
+        <v>50</v>
+      </c>
+      <c r="R8" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q8)-COUNTIF(Notas!D:D,"&lt;="&amp;Q7)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="31" t="e">
-        <f>EXP((P6-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T6" s="59">
-        <v>30</v>
-      </c>
-      <c r="U6" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T6)-COUNTIF(Notas!D:D,"&lt;="&amp;T5)</f>
+      <c r="S8" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q8,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q7,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q9" s="59">
+        <v>60</v>
+      </c>
+      <c r="R9" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q9)-COUNTIF(Notas!D:D,"&lt;="&amp;Q8)</f>
         <v>0</v>
       </c>
-      <c r="V6" s="31" t="e">
-        <f>_xlfn.NORM.DIST($T6,$F$2,SQRT($H$2),TRUE)*$C$2</f>
+      <c r="S9" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q9,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q8,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P7" s="59">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P7)-COUNTIF(Notas!D:D,"&lt;="&amp;P6)</f>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q10" s="59">
+        <v>70</v>
+      </c>
+      <c r="R10" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q10)-COUNTIF(Notas!D:D,"&lt;="&amp;Q9)</f>
         <v>0</v>
       </c>
-      <c r="R7" s="31" t="e">
-        <f>EXP((P7-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T7" s="59">
-        <v>40</v>
-      </c>
-      <c r="U7" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T7)-COUNTIF(Notas!D:D,"&lt;="&amp;T6)</f>
+      <c r="S10" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q10,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q9,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q11" s="59">
+        <v>80</v>
+      </c>
+      <c r="R11" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q11)-COUNTIF(Notas!D:D,"&lt;="&amp;Q10)</f>
         <v>0</v>
       </c>
-      <c r="V7" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($T7,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($T6,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+      <c r="S11" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q11,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q10,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P8" s="59">
-        <v>25</v>
-      </c>
-      <c r="Q8" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P8)-COUNTIF(Notas!D:D,"&lt;="&amp;P7)</f>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q12" s="59">
+        <v>90</v>
+      </c>
+      <c r="R12" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q12)-COUNTIF(Notas!D:D,"&lt;="&amp;Q11)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="31" t="e">
-        <f>EXP((P8-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T8" s="59">
-        <v>50</v>
-      </c>
-      <c r="U8" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T8)-COUNTIF(Notas!D:D,"&lt;="&amp;T7)</f>
+      <c r="S12" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q12,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q11,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q13" s="59">
+        <v>100</v>
+      </c>
+      <c r="R13" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q13)-COUNTIF(Notas!D:D,"&lt;="&amp;Q12)</f>
         <v>0</v>
       </c>
-      <c r="V8" s="31" t="e">
-        <f t="shared" ref="V8:V26" si="1">(_xlfn.NORM.DIST($T8,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($T7,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+      <c r="S13" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q13,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q12,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P9" s="59">
-        <v>30</v>
-      </c>
-      <c r="Q9" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P9)-COUNTIF(Notas!D:D,"&lt;="&amp;P8)</f>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q14" s="59">
+        <v>110</v>
+      </c>
+      <c r="R14" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q14)-COUNTIF(Notas!D:D,"&lt;="&amp;Q13)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="31" t="e">
-        <f>EXP((P9-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T9" s="59">
-        <v>60</v>
-      </c>
-      <c r="U9" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T9)-COUNTIF(Notas!D:D,"&lt;="&amp;T8)</f>
+      <c r="S14" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q14,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q13,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q15" s="59">
+        <v>120</v>
+      </c>
+      <c r="R15" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q15)-COUNTIF(Notas!D:D,"&lt;="&amp;Q14)</f>
         <v>0</v>
       </c>
-      <c r="V9" s="31" t="e">
-        <f t="shared" si="1"/>
+      <c r="S15" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q15,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q14,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P10" s="59">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P10)-COUNTIF(Notas!D:D,"&lt;="&amp;P9)</f>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q16" s="59">
+        <v>130</v>
+      </c>
+      <c r="R16" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q16)-COUNTIF(Notas!D:D,"&lt;="&amp;Q15)</f>
+        <v>1</v>
+      </c>
+      <c r="S16" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q16,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q15,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q17" s="59">
+        <v>140</v>
+      </c>
+      <c r="R17" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q17)-COUNTIF(Notas!D:D,"&lt;="&amp;Q16)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="31" t="e">
-        <f>EXP((P10-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T10" s="59">
-        <v>70</v>
-      </c>
-      <c r="U10" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T10)-COUNTIF(Notas!D:D,"&lt;="&amp;T9)</f>
+      <c r="S17" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q17,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q16,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q18" s="59">
+        <v>150</v>
+      </c>
+      <c r="R18" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q18)-COUNTIF(Notas!D:D,"&lt;="&amp;Q17)</f>
         <v>0</v>
       </c>
-      <c r="V10" s="31" t="e">
-        <f t="shared" si="1"/>
+      <c r="S18" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q18,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q17,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P11" s="59">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P11)-COUNTIF(Notas!D:D,"&lt;="&amp;P10)</f>
+    <row r="19" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q19" s="59">
+        <v>160</v>
+      </c>
+      <c r="R19" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q19)-COUNTIF(Notas!D:D,"&lt;="&amp;Q18)</f>
         <v>0</v>
       </c>
-      <c r="R11" s="31" t="e">
-        <f>EXP((P11-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T11" s="59">
-        <v>80</v>
-      </c>
-      <c r="U11" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T11)-COUNTIF(Notas!D:D,"&lt;="&amp;T10)</f>
+      <c r="S19" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q19,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q18,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q20" s="59">
+        <v>170</v>
+      </c>
+      <c r="R20" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q20)-COUNTIF(Notas!D:D,"&lt;="&amp;Q19)</f>
         <v>0</v>
       </c>
-      <c r="V11" s="31" t="e">
-        <f t="shared" si="1"/>
+      <c r="S20" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q20,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q19,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P12" s="59">
-        <v>45</v>
-      </c>
-      <c r="Q12" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P12)-COUNTIF(Notas!D:D,"&lt;="&amp;P11)</f>
+    <row r="21" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q21" s="59">
+        <v>180</v>
+      </c>
+      <c r="R21" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q21)-COUNTIF(Notas!D:D,"&lt;="&amp;Q20)</f>
         <v>0</v>
       </c>
-      <c r="R12" s="31" t="e">
-        <f>EXP((P12-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T12" s="59">
-        <v>90</v>
-      </c>
-      <c r="U12" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T12)-COUNTIF(Notas!D:D,"&lt;="&amp;T11)</f>
+      <c r="S21" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q21,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q20,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="22" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q22" s="59">
+        <v>190</v>
+      </c>
+      <c r="R22" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q22)-COUNTIF(Notas!D:D,"&lt;="&amp;Q21)</f>
         <v>0</v>
       </c>
-      <c r="V12" s="31" t="e">
-        <f t="shared" si="1"/>
+      <c r="S22" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q22,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q21,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P13" s="59">
-        <v>50</v>
-      </c>
-      <c r="Q13" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P13)-COUNTIF(Notas!D:D,"&lt;="&amp;P12)</f>
+    <row r="23" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q23" s="59">
+        <v>200</v>
+      </c>
+      <c r="R23" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q23)-COUNTIF(Notas!D:D,"&lt;="&amp;Q22)</f>
         <v>0</v>
       </c>
-      <c r="R13" s="31" t="e">
-        <f>EXP((P13-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T13" s="59">
-        <v>100</v>
-      </c>
-      <c r="U13" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T13)-COUNTIF(Notas!D:D,"&lt;="&amp;T12)</f>
+      <c r="S23" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q23,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q22,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="24" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q24" s="59">
+        <v>210</v>
+      </c>
+      <c r="R24" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q24)-COUNTIF(Notas!D:D,"&lt;="&amp;Q23)</f>
         <v>0</v>
       </c>
-      <c r="V13" s="31" t="e">
-        <f t="shared" si="1"/>
+      <c r="S24" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q24,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q23,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P14" s="59">
-        <v>55</v>
-      </c>
-      <c r="Q14" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P14)-COUNTIF(Notas!D:D,"&lt;="&amp;P13)</f>
+    <row r="25" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q25" s="59">
+        <v>220</v>
+      </c>
+      <c r="R25" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q25)-COUNTIF(Notas!D:D,"&lt;="&amp;Q24)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="31" t="e">
-        <f>EXP((P14-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T14" s="59">
-        <v>110</v>
-      </c>
-      <c r="U14" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T14)-COUNTIF(Notas!D:D,"&lt;="&amp;T13)</f>
+      <c r="S25" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q25,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q24,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="26" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q26" s="59">
+        <v>230</v>
+      </c>
+      <c r="R26" s="52">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q26)-COUNTIF(Notas!D:D,"&lt;="&amp;Q25)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="31" t="e">
-        <f t="shared" si="1"/>
+      <c r="S26" s="31" t="e">
+        <f>(_xlfn.NORM.DIST($Q26,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q25,$F$2,SQRT($H$2),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P15" s="59">
-        <v>60</v>
-      </c>
-      <c r="Q15" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P15)-COUNTIF(Notas!D:D,"&lt;="&amp;P14)</f>
+    <row r="27" spans="17:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q27" s="60">
+        <v>240</v>
+      </c>
+      <c r="R27" s="61">
+        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q27)-COUNTIF(Notas!D:D,"&lt;="&amp;Q26)</f>
         <v>0</v>
       </c>
-      <c r="R15" s="31" t="e">
-        <f>EXP((P15-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T15" s="59">
-        <v>120</v>
-      </c>
-      <c r="U15" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T15)-COUNTIF(Notas!D:D,"&lt;="&amp;T14)</f>
-        <v>0</v>
-      </c>
-      <c r="V15" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P16" s="59">
-        <v>65</v>
-      </c>
-      <c r="Q16" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P16)-COUNTIF(Notas!D:D,"&lt;="&amp;P15)</f>
-        <v>0</v>
-      </c>
-      <c r="R16" s="31" t="e">
-        <f>EXP((P16-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T16" s="59">
-        <v>130</v>
-      </c>
-      <c r="U16" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T16)-COUNTIF(Notas!D:D,"&lt;="&amp;T15)</f>
-        <v>1</v>
-      </c>
-      <c r="V16" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="17" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P17" s="59">
-        <v>70</v>
-      </c>
-      <c r="Q17" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P17)-COUNTIF(Notas!D:D,"&lt;="&amp;P16)</f>
-        <v>0</v>
-      </c>
-      <c r="R17" s="31" t="e">
-        <f>EXP((P17-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T17" s="59">
-        <v>140</v>
-      </c>
-      <c r="U17" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T17)-COUNTIF(Notas!D:D,"&lt;="&amp;T16)</f>
-        <v>0</v>
-      </c>
-      <c r="V17" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P18" s="59">
-        <v>75</v>
-      </c>
-      <c r="Q18" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P18)-COUNTIF(Notas!D:D,"&lt;="&amp;P17)</f>
-        <v>0</v>
-      </c>
-      <c r="R18" s="31" t="e">
-        <f>EXP((P18-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T18" s="59">
-        <v>150</v>
-      </c>
-      <c r="U18" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T18)-COUNTIF(Notas!D:D,"&lt;="&amp;T17)</f>
-        <v>0</v>
-      </c>
-      <c r="V18" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="19" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P19" s="59">
-        <v>80</v>
-      </c>
-      <c r="Q19" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P19)-COUNTIF(Notas!D:D,"&lt;="&amp;P18)</f>
-        <v>0</v>
-      </c>
-      <c r="R19" s="31" t="e">
-        <f>EXP((P19-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T19" s="59">
-        <v>160</v>
-      </c>
-      <c r="U19" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T19)-COUNTIF(Notas!D:D,"&lt;="&amp;T18)</f>
-        <v>0</v>
-      </c>
-      <c r="V19" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="20" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P20" s="59">
-        <v>85</v>
-      </c>
-      <c r="Q20" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P20)-COUNTIF(Notas!D:D,"&lt;="&amp;P19)</f>
-        <v>0</v>
-      </c>
-      <c r="R20" s="31" t="e">
-        <f>EXP((P20-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T20" s="59">
-        <v>170</v>
-      </c>
-      <c r="U20" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T20)-COUNTIF(Notas!D:D,"&lt;="&amp;T19)</f>
-        <v>0</v>
-      </c>
-      <c r="V20" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="21" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P21" s="59">
-        <v>90</v>
-      </c>
-      <c r="Q21" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P21)-COUNTIF(Notas!D:D,"&lt;="&amp;P20)</f>
-        <v>0</v>
-      </c>
-      <c r="R21" s="31" t="e">
-        <f>EXP((P21-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T21" s="59">
-        <v>180</v>
-      </c>
-      <c r="U21" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T21)-COUNTIF(Notas!D:D,"&lt;="&amp;T20)</f>
-        <v>0</v>
-      </c>
-      <c r="V21" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="22" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P22" s="59">
-        <v>95</v>
-      </c>
-      <c r="Q22" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P22)-COUNTIF(Notas!D:D,"&lt;="&amp;P21)</f>
-        <v>0</v>
-      </c>
-      <c r="R22" s="31" t="e">
-        <f>EXP((P22-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T22" s="59">
-        <v>190</v>
-      </c>
-      <c r="U22" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T22)-COUNTIF(Notas!D:D,"&lt;="&amp;T21)</f>
-        <v>0</v>
-      </c>
-      <c r="V22" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="23" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P23" s="59">
-        <v>100</v>
-      </c>
-      <c r="Q23" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P23)-COUNTIF(Notas!D:D,"&lt;="&amp;P22)</f>
-        <v>0</v>
-      </c>
-      <c r="R23" s="31" t="e">
-        <f>EXP((P23-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T23" s="59">
-        <v>200</v>
-      </c>
-      <c r="U23" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T23)-COUNTIF(Notas!D:D,"&lt;="&amp;T22)</f>
-        <v>0</v>
-      </c>
-      <c r="V23" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="24" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P24" s="59">
-        <v>105</v>
-      </c>
-      <c r="Q24" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P24)-COUNTIF(Notas!D:D,"&lt;="&amp;P23)</f>
-        <v>0</v>
-      </c>
-      <c r="R24" s="31" t="e">
-        <f>EXP((P24-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T24" s="59">
-        <v>210</v>
-      </c>
-      <c r="U24" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T24)-COUNTIF(Notas!D:D,"&lt;="&amp;T23)</f>
-        <v>0</v>
-      </c>
-      <c r="V24" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="25" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P25" s="59">
-        <v>110</v>
-      </c>
-      <c r="Q25" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P25)-COUNTIF(Notas!D:D,"&lt;="&amp;P24)</f>
-        <v>0</v>
-      </c>
-      <c r="R25" s="31" t="e">
-        <f>EXP((P25-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T25" s="59">
-        <v>220</v>
-      </c>
-      <c r="U25" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T25)-COUNTIF(Notas!D:D,"&lt;="&amp;T24)</f>
-        <v>0</v>
-      </c>
-      <c r="V25" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="26" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P26" s="59">
-        <v>115</v>
-      </c>
-      <c r="Q26" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P26)-COUNTIF(Notas!D:D,"&lt;="&amp;P25)</f>
-        <v>0</v>
-      </c>
-      <c r="R26" s="31" t="e">
-        <f>EXP((P26-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T26" s="59">
-        <v>230</v>
-      </c>
-      <c r="U26" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T26)-COUNTIF(Notas!D:D,"&lt;="&amp;T25)</f>
-        <v>0</v>
-      </c>
-      <c r="V26" s="31" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="27" spans="16:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P27" s="59">
-        <v>120</v>
-      </c>
-      <c r="Q27" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P27)-COUNTIF(Notas!D:D,"&lt;="&amp;P26)</f>
-        <v>0</v>
-      </c>
-      <c r="R27" s="31" t="e">
-        <f>EXP((P27-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T27" s="60">
-        <v>240</v>
-      </c>
-      <c r="U27" s="61">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;T27)-COUNTIF(Notas!D:D,"&lt;="&amp;T26)</f>
-        <v>0</v>
-      </c>
-      <c r="V27" s="32" t="e">
+      <c r="S27" s="32" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P28" s="59">
-        <v>125</v>
-      </c>
-      <c r="Q28" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P28)-COUNTIF(Notas!D:D,"&lt;="&amp;P27)</f>
-        <v>0</v>
-      </c>
-      <c r="R28" s="31" t="e">
-        <f>EXP((P28-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T28" s="25"/>
-      <c r="V28" s="17" t="e">
-        <f>SUM(V4:V27)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P29" s="59">
-        <v>130</v>
-      </c>
-      <c r="Q29" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P29)-COUNTIF(Notas!D:D,"&lt;="&amp;P28)</f>
-        <v>1</v>
-      </c>
-      <c r="R29" s="31" t="e">
-        <f>EXP((P29-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P30" s="59">
-        <v>135</v>
-      </c>
-      <c r="Q30" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P30)-COUNTIF(Notas!D:D,"&lt;="&amp;P29)</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="31" t="e">
-        <f>EXP((P30-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P31" s="59">
-        <v>140</v>
-      </c>
-      <c r="Q31" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P31)-COUNTIF(Notas!D:D,"&lt;="&amp;P30)</f>
-        <v>0</v>
-      </c>
-      <c r="R31" s="31" t="e">
-        <f>EXP((P31-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P32" s="59">
-        <v>145</v>
-      </c>
-      <c r="Q32" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P32)-COUNTIF(Notas!D:D,"&lt;="&amp;P31)</f>
-        <v>0</v>
-      </c>
-      <c r="R32" s="31" t="e">
-        <f>EXP((P32-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="33" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P33" s="59">
-        <v>150</v>
-      </c>
-      <c r="Q33" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P33)-COUNTIF(Notas!D:D,"&lt;="&amp;P32)</f>
-        <v>0</v>
-      </c>
-      <c r="R33" s="31" t="e">
-        <f>EXP((P33-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P34" s="59">
-        <v>155</v>
-      </c>
-      <c r="Q34" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P34)-COUNTIF(Notas!D:D,"&lt;="&amp;P33)</f>
-        <v>0</v>
-      </c>
-      <c r="R34" s="31" t="e">
-        <f>EXP((P34-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P35" s="59">
-        <v>160</v>
-      </c>
-      <c r="Q35" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P35)-COUNTIF(Notas!D:D,"&lt;="&amp;P34)</f>
-        <v>0</v>
-      </c>
-      <c r="R35" s="31" t="e">
-        <f>EXP((P35-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P36" s="59">
-        <v>165</v>
-      </c>
-      <c r="Q36" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P36)-COUNTIF(Notas!D:D,"&lt;="&amp;P35)</f>
-        <v>0</v>
-      </c>
-      <c r="R36" s="31" t="e">
-        <f>EXP((P36-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P37" s="59">
-        <v>170</v>
-      </c>
-      <c r="Q37" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P37)-COUNTIF(Notas!D:D,"&lt;="&amp;P36)</f>
-        <v>0</v>
-      </c>
-      <c r="R37" s="31" t="e">
-        <f>EXP((P37-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P38" s="59">
-        <v>175</v>
-      </c>
-      <c r="Q38" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P38)-COUNTIF(Notas!D:D,"&lt;="&amp;P37)</f>
-        <v>0</v>
-      </c>
-      <c r="R38" s="31" t="e">
-        <f>EXP((P38-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P39" s="59">
-        <v>180</v>
-      </c>
-      <c r="Q39" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P39)-COUNTIF(Notas!D:D,"&lt;="&amp;P38)</f>
-        <v>0</v>
-      </c>
-      <c r="R39" s="31" t="e">
-        <f>EXP((P39-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P40" s="59">
-        <v>185</v>
-      </c>
-      <c r="Q40" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P40)-COUNTIF(Notas!D:D,"&lt;="&amp;P39)</f>
-        <v>0</v>
-      </c>
-      <c r="R40" s="31" t="e">
-        <f>EXP((P40-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P41" s="59">
-        <v>190</v>
-      </c>
-      <c r="Q41" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P41)-COUNTIF(Notas!D:D,"&lt;="&amp;P40)</f>
-        <v>0</v>
-      </c>
-      <c r="R41" s="31" t="e">
-        <f>EXP((P41-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P42" s="59">
-        <v>195</v>
-      </c>
-      <c r="Q42" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P42)-COUNTIF(Notas!D:D,"&lt;="&amp;P41)</f>
-        <v>0</v>
-      </c>
-      <c r="R42" s="31" t="e">
-        <f>EXP((P42-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P43" s="59">
-        <v>200</v>
-      </c>
-      <c r="Q43" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P43)-COUNTIF(Notas!D:D,"&lt;="&amp;P42)</f>
-        <v>0</v>
-      </c>
-      <c r="R43" s="31" t="e">
-        <f>EXP((P43-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P44" s="59">
-        <v>205</v>
-      </c>
-      <c r="Q44" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P44)-COUNTIF(Notas!D:D,"&lt;="&amp;P43)</f>
-        <v>0</v>
-      </c>
-      <c r="R44" s="31" t="e">
-        <f>EXP((P44-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P45" s="59">
-        <v>210</v>
-      </c>
-      <c r="Q45" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P45)-COUNTIF(Notas!D:D,"&lt;="&amp;P44)</f>
-        <v>0</v>
-      </c>
-      <c r="R45" s="31" t="e">
-        <f>EXP((P45-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="46" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P46" s="59">
-        <v>215</v>
-      </c>
-      <c r="Q46" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P46)-COUNTIF(Notas!D:D,"&lt;="&amp;P45)</f>
-        <v>0</v>
-      </c>
-      <c r="R46" s="31" t="e">
-        <f>EXP((P46-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P47" s="59">
-        <v>220</v>
-      </c>
-      <c r="Q47" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P47)-COUNTIF(Notas!D:D,"&lt;="&amp;P46)</f>
-        <v>0</v>
-      </c>
-      <c r="R47" s="31" t="e">
-        <f>EXP((P47-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="48" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P48" s="59">
-        <v>225</v>
-      </c>
-      <c r="Q48" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P48)-COUNTIF(Notas!D:D,"&lt;="&amp;P47)</f>
-        <v>0</v>
-      </c>
-      <c r="R48" s="31" t="e">
-        <f>EXP((P48-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="49" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P49" s="59">
-        <v>230</v>
-      </c>
-      <c r="Q49" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P49)-COUNTIF(Notas!D:D,"&lt;="&amp;P48)</f>
-        <v>0</v>
-      </c>
-      <c r="R49" s="31" t="e">
-        <f>EXP((P49-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="50" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P50" s="59">
-        <v>235</v>
-      </c>
-      <c r="Q50" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P50)-COUNTIF(Notas!D:D,"&lt;="&amp;P49)</f>
-        <v>0</v>
-      </c>
-      <c r="R50" s="31" t="e">
-        <f>EXP((P50-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="51" spans="16:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P51" s="60">
-        <v>240</v>
-      </c>
-      <c r="Q51" s="61">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;P51)-COUNTIF(Notas!D:D,"&lt;="&amp;P50)</f>
-        <v>0</v>
-      </c>
-      <c r="R51" s="32" t="e">
-        <f>EXP((P51-$F$1)^2/(-2*$F$3))/SQRT(2*PI()*$F$3)*Estadística!$B$1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="52" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="Q52">
-        <f>SUM(Q4:Q51)</f>
-        <v>1</v>
-      </c>
-      <c r="R52" t="e">
-        <f>SUM(R4:R51)</f>
+    <row r="28" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q28" s="25"/>
+      <c r="S28" s="17" t="e">
+        <f>SUM(S4:S27)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -16694,13 +16100,13 @@
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>5.8154074312521944</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>6.4137430340189105</v>
@@ -16708,13 +16114,13 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>4.4331233333245637</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4">
         <v>1.6223375982874726</v>
@@ -16732,10 +16138,10 @@
         <v>12</v>
       </c>
       <c r="E6" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="66" t="s">
         <v>40</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>41</v>
       </c>
       <c r="G6" s="62" t="s">
         <v>24</v>
@@ -17355,14 +16761,14 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="70">
         <f>AVERAGE(Visionados)</f>
         <v>26047</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="70">
         <f>MAX(Visionados)</f>
@@ -17378,7 +16784,7 @@
         <v>26047</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <f>MIN(Visionados)</f>
@@ -17387,13 +16793,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="71">
         <v>62533</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2">
         <f>COUNTIF(Visionados,"&lt;="&amp;B4)/Pelis</f>

</xml_diff>

<commit_message>
Calculus normal time distribution
</commit_message>
<xml_diff>
--- a/res/Readdata/Plantilla.xlsx
+++ b/res/Readdata/Plantilla.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F269890-7171-4DFC-AC7B-EEEF919684F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0F0896-988F-44FD-AA28-F815A7A80D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notas" sheetId="3" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>Media filmafinity</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>Minutos</t>
-  </si>
-  <si>
-    <t>Normal &gt;60</t>
   </si>
   <si>
     <t>Chi cuad Yo</t>
@@ -334,6 +331,12 @@
   </si>
   <si>
     <t>Duración</t>
+  </si>
+  <si>
+    <t>Ocurrencias</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
 </sst>
 </file>
@@ -802,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -874,7 +877,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -927,33 +929,51 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="29">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF33CC33"/>
-      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1214,6 +1234,28 @@
         </right>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FF33CC33"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1316,7 +1358,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>4.0012738448308918</c:v>
+                  <c:v>3.9574904473039503</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1328,7 +1370,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.8889473243090102</c:v>
+                  <c:v>2.4339596031261825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2293,7 +2335,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.8889473243090102</c:v>
+                  <c:v>2.4339596031261825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5101,7 +5143,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>1.8889473243090102</c:v>
+                  <c:v>2.4339596031261825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5790,9 +5832,9 @@
             <c:numRef>
               <c:f>Tiempos!$R$4:$R$27</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="24"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -5871,6 +5913,215 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-62E0-47DF-9E76-C4F90E81E81A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="871117216"/>
+        <c:axId val="871118528"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tiempos!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tiempos!$Q$4:$Q$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tiempos!$S$4:$S$27</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C325-42C5-A687-967C66B51C3F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13829,45 +14080,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:N1048576" totalsRowShown="0" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:N1048576" totalsRowShown="0" tableBorderDxfId="26">
   <autoFilter ref="A1:N1048576" xr:uid="{B7E8E3F6-4A56-4C38-9CDA-83612E98463A}"/>
   <tableColumns count="14">
-    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="24"/>
-    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{65EE12B7-2552-4910-A353-7AE48A3D7AA6}" name="FA"/>
-    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{2E72113E-50BE-41C7-8BFD-59035950093F}" name="Varianza_FA" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{2E72113E-50BE-41C7-8BFD-59035950093F}" name="Varianza_FA" dataDxfId="21"/>
     <tableColumn id="5" xr3:uid="{FF19B5AE-C56B-4CA5-B812-840E5C110430}" name="FA_redondeo"/>
     <tableColumn id="6" xr3:uid="{20BAA72D-A773-488D-B544-DAD2EF762D99}" name="Diferencia"/>
     <tableColumn id="7" xr3:uid="{E40D682E-5136-4AEB-BEE2-B6B87967AFB0}" name="Diferencia_abs"/>
-    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me_ha_gustado" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me_ha_gustado" dataDxfId="20">
       <calculatedColumnFormula>IF($H2&gt;0,1,0.1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia_ruido" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia_ruido" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="18">
       <calculatedColumnFormula>C2+(RAND()-0.5)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="15">
   <autoFilter ref="B3:F13" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="13">
       <calculatedColumnFormula>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="11">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B3,MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="10">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13876,19 +14127,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="B19:F39" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="5">
       <calculatedColumnFormula>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="4">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="3">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B20,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5AFFC25-E554-49FC-9485-58BDC89F7ED4}" name="Tiempos_normal" displayName="Tiempos_normal" ref="Q3:S27" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="Q3:S27" xr:uid="{E5AFFC25-E554-49FC-9485-58BDC89F7ED4}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9480A362-FEE1-48D4-8ACA-A2492EA7E360}" name="Minutos" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A2427276-3F9C-4E12-9EC9-F89716AF732E}" name="Ocurrencias">
+      <calculatedColumnFormula>COUNTIF(Notas!D:D,"&lt;="&amp;Q4)-COUNTIF(Notas!D:D,"&lt;="&amp;Q3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{FCC37941-690A-4CC1-A9C7-96E0FC9A264C}" name="Normal" dataDxfId="0">
+      <calculatedColumnFormula>(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -14160,7 +14427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8703B0C1-9812-4468-A745-94BA8D5548CD}">
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -14169,15 +14436,15 @@
     <col min="1" max="1" width="7.7109375" style="17" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="17" customWidth="1"/>
     <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="70" customWidth="1"/>
-    <col min="5" max="6" width="12.140625" style="70" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="69" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" style="69" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="75" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="74" customWidth="1"/>
     <col min="11" max="12" width="7.42578125" style="28" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="68" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="68" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="67" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="67" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" style="52" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" customWidth="1"/>
     <col min="17" max="17" width="8.28515625" customWidth="1"/>
@@ -14191,46 +14458,46 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="70" t="s">
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>58</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="N1" s="67" t="s">
         <v>60</v>
-      </c>
-      <c r="N1" s="68" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -14243,13 +14510,13 @@
       <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2" s="70">
+      <c r="D2" s="69">
         <v>130</v>
       </c>
-      <c r="E2" s="70">
+      <c r="E2" s="69">
         <v>26047</v>
       </c>
-      <c r="F2" s="76">
+      <c r="F2" s="75">
         <v>2.1</v>
       </c>
       <c r="G2">
@@ -14264,23 +14531,23 @@
         <f t="shared" ref="I2" si="1">ABS(H2)</f>
         <v>2</v>
       </c>
-      <c r="J2" s="75">
+      <c r="J2" s="74">
         <f t="shared" ref="J2" si="2">IF($H2&gt;0,1,0.1)</f>
         <v>0.1</v>
       </c>
       <c r="K2" s="28">
         <f t="shared" ref="K2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>1.8889473243090102</v>
+        <v>2.4339596031261825</v>
       </c>
       <c r="L2" s="28">
         <f t="shared" ref="L2" ca="1" si="4">C2+(RAND()-0.5)/10</f>
-        <v>4.0012738448308918</v>
-      </c>
-      <c r="M2" s="68">
+        <v>3.9574904473039503</v>
+      </c>
+      <c r="M2" s="67">
         <f t="shared" ref="M2" si="5">(B2-1)*10/9</f>
         <v>1.1111111111111112</v>
       </c>
-      <c r="N2" s="68">
+      <c r="N2" s="67">
         <f t="shared" ref="N2" si="6">(C2-1)*10/9</f>
         <v>3.3333333333333335</v>
       </c>
@@ -14292,7 +14559,7 @@
       <c r="W2" s="52"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O3" s="63"/>
+      <c r="O3" s="62"/>
       <c r="P3" s="27"/>
       <c r="Q3" s="27"/>
       <c r="R3" s="25"/>
@@ -14300,7 +14567,7 @@
       <c r="W3" s="52"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O4" s="63"/>
+      <c r="O4" s="62"/>
       <c r="P4" s="27"/>
       <c r="Q4" s="27"/>
       <c r="R4" s="25"/>
@@ -14540,10 +14807,10 @@
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14609,7 +14876,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14632,7 +14899,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <f>COUNT(Tabla1[FA])</f>
@@ -14819,13 +15086,13 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F14" s="25"/>
       <c r="G14" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" t="s">
         <v>64</v>
-      </c>
-      <c r="H14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" t="s">
-        <v>65</v>
       </c>
       <c r="J14" t="s">
         <v>17</v>
@@ -14836,16 +15103,16 @@
         <v>13</v>
       </c>
       <c r="F15" s="25"/>
-      <c r="G15" s="74">
+      <c r="G15" s="73">
         <v>7.8</v>
       </c>
-      <c r="H15" s="90">
+      <c r="H15" s="89">
         <v>1000</v>
       </c>
-      <c r="I15" s="90">
+      <c r="I15" s="89">
         <v>90</v>
       </c>
-      <c r="J15" s="91">
+      <c r="J15" s="90">
         <v>1.6</v>
       </c>
     </row>
@@ -14864,23 +15131,23 @@
         <f>STDEVP(Tabla1[FA_rees])</f>
         <v>0</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="72">
+      <c r="E16" s="62"/>
+      <c r="F16" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="71">
         <f>COUNTIF(NotasFA,"&lt;="&amp;G15)/Pelis_con_nota</f>
         <v>1</v>
       </c>
-      <c r="H16" s="72">
+      <c r="H16" s="71">
         <f>COUNTIF(Tabla1[Visionados],"&lt;="&amp;H15)/Pelis_con_nota</f>
         <v>0</v>
       </c>
-      <c r="I16" s="72">
+      <c r="I16" s="71">
         <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;I15)/Pelis_con_nota</f>
         <v>0</v>
       </c>
-      <c r="J16" s="72">
+      <c r="J16" s="71">
         <f>COUNTIF(Tabla1[Varianza_FA],"&lt;="&amp;J15)/Pelis_con_nota</f>
         <v>0</v>
       </c>
@@ -14900,11 +15167,11 @@
         <f>STDEVP(Tabla1[Mia_rees])</f>
         <v>0</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="73">
+      <c r="E17" s="62"/>
+      <c r="F17" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="72">
         <f>COUNTIF(NotasMias,"&lt;="&amp;G15)/Pelis</f>
         <v>1</v>
       </c>
@@ -14937,7 +15204,7 @@
   <dimension ref="B3:S40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14949,24 +15216,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="82" t="s">
+      <c r="B3" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="84" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="77">
+      <c r="B4" s="76">
         <v>1</v>
       </c>
       <c r="C4" s="19">
@@ -14981,13 +15248,13 @@
         <f>_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F4" s="64" t="e">
+      <c r="F4" s="63" t="e">
         <f>_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="78">
+      <c r="B5" s="77">
         <v>2</v>
       </c>
       <c r="C5" s="3">
@@ -15002,13 +15269,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F5" s="80" t="e">
+      <c r="F5" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="78">
+      <c r="B6" s="77">
         <v>3</v>
       </c>
       <c r="C6" s="3">
@@ -15023,13 +15290,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F6" s="80" t="e">
+      <c r="F6" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="78">
+      <c r="B7" s="77">
         <v>4</v>
       </c>
       <c r="C7" s="3">
@@ -15044,13 +15311,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F7" s="80" t="e">
+      <c r="F7" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="78">
+      <c r="B8" s="77">
         <v>5</v>
       </c>
       <c r="C8" s="3">
@@ -15065,13 +15332,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F8" s="80" t="e">
+      <c r="F8" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="78">
+      <c r="B9" s="77">
         <v>6</v>
       </c>
       <c r="C9" s="3">
@@ -15086,13 +15353,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F9" s="80" t="e">
+      <c r="F9" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="78">
+      <c r="B10" s="77">
         <v>7</v>
       </c>
       <c r="C10" s="3">
@@ -15107,13 +15374,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F10" s="80" t="e">
+      <c r="F10" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="78">
+      <c r="B11" s="77">
         <v>8</v>
       </c>
       <c r="C11" s="3">
@@ -15128,13 +15395,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F11" s="80" t="e">
+      <c r="F11" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="78">
+      <c r="B12" s="77">
         <v>9</v>
       </c>
       <c r="C12" s="3">
@@ -15149,13 +15416,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F12" s="80" t="e">
+      <c r="F12" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="79">
+      <c r="B13" s="78">
         <v>10</v>
       </c>
       <c r="C13" s="22">
@@ -15170,40 +15437,40 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F13" s="80" t="e">
+      <c r="F13" s="79" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="64" t="e">
+      <c r="E14" s="63" t="e">
         <f>SUM(E4:E13)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F14" s="64" t="e">
+      <c r="F14" s="63" t="e">
         <f>SUM(F4:F13)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="19" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="88" t="s">
+      <c r="D19" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="89" t="s">
+      <c r="E19" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="88" t="s">
+      <c r="F19" s="87" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="77">
+      <c r="B20" s="76">
         <v>0.5</v>
       </c>
       <c r="C20" s="33">
@@ -15218,12 +15485,12 @@
         <f>(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F20" s="86" t="e">
+      <c r="F20" s="85" t="e">
         <f>_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
       <c r="R20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S20" s="30" t="e" cm="1">
         <f t="array" aca="1" ref="S20" ca="1">_xlfn.CHISQ.DIST(SUM((C22:C39-E22:E39)^2/E22:E39),18,TRUE)</f>
@@ -15231,7 +15498,7 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="78">
+      <c r="B21" s="77">
         <v>1</v>
       </c>
       <c r="C21" s="34">
@@ -15246,12 +15513,12 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F21" s="87" t="e">
+      <c r="F21" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
       <c r="R21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S21" s="30" t="e" cm="1">
         <f t="array" aca="1" ref="S21" ca="1">_xlfn.CHISQ.DIST(SUM((D25:D39-F25:F39)^2/F25:F39),18,TRUE)</f>
@@ -15259,7 +15526,7 @@
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="78">
+      <c r="B22" s="77">
         <v>1.5</v>
       </c>
       <c r="C22" s="34">
@@ -15274,13 +15541,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F22" s="87" t="e">
+      <c r="F22" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="78">
+      <c r="B23" s="77">
         <v>2</v>
       </c>
       <c r="C23" s="34">
@@ -15295,13 +15562,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F23" s="87" t="e">
+      <c r="F23" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="78">
+      <c r="B24" s="77">
         <v>2.5</v>
       </c>
       <c r="C24" s="34">
@@ -15316,13 +15583,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F24" s="87" t="e">
+      <c r="F24" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="78">
+      <c r="B25" s="77">
         <v>3</v>
       </c>
       <c r="C25" s="34">
@@ -15337,13 +15604,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F25" s="87" t="e">
+      <c r="F25" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="78">
+      <c r="B26" s="77">
         <v>3.5</v>
       </c>
       <c r="C26" s="34">
@@ -15358,13 +15625,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F26" s="87" t="e">
+      <c r="F26" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="78">
+      <c r="B27" s="77">
         <v>4</v>
       </c>
       <c r="C27" s="34">
@@ -15379,13 +15646,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F27" s="87" t="e">
+      <c r="F27" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="78">
+      <c r="B28" s="77">
         <v>4.5</v>
       </c>
       <c r="C28" s="34">
@@ -15400,13 +15667,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F28" s="87" t="e">
+      <c r="F28" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="78">
+      <c r="B29" s="77">
         <v>5</v>
       </c>
       <c r="C29" s="34">
@@ -15421,13 +15688,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F29" s="87" t="e">
+      <c r="F29" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="78">
+      <c r="B30" s="77">
         <v>5.5</v>
       </c>
       <c r="C30" s="34">
@@ -15442,13 +15709,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F30" s="87" t="e">
+      <c r="F30" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="78">
+      <c r="B31" s="77">
         <v>6</v>
       </c>
       <c r="C31" s="34">
@@ -15463,13 +15730,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F31" s="87" t="e">
+      <c r="F31" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="78">
+      <c r="B32" s="77">
         <v>6.5</v>
       </c>
       <c r="C32" s="34">
@@ -15484,13 +15751,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F32" s="87" t="e">
+      <c r="F32" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="78">
+      <c r="B33" s="77">
         <v>7</v>
       </c>
       <c r="C33" s="34">
@@ -15505,13 +15772,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F33" s="87" t="e">
+      <c r="F33" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="78">
+      <c r="B34" s="77">
         <v>7.5</v>
       </c>
       <c r="C34" s="34">
@@ -15526,13 +15793,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F34" s="87" t="e">
+      <c r="F34" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="78">
+      <c r="B35" s="77">
         <v>8</v>
       </c>
       <c r="C35" s="34">
@@ -15547,13 +15814,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F35" s="87" t="e">
+      <c r="F35" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="78">
+      <c r="B36" s="77">
         <v>8.5</v>
       </c>
       <c r="C36" s="34">
@@ -15568,13 +15835,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F36" s="87" t="e">
+      <c r="F36" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="78">
+      <c r="B37" s="77">
         <v>9</v>
       </c>
       <c r="C37" s="34">
@@ -15589,13 +15856,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F37" s="87" t="e">
+      <c r="F37" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="78">
+      <c r="B38" s="77">
         <v>9.5</v>
       </c>
       <c r="C38" s="34">
@@ -15610,13 +15877,13 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F38" s="87" t="e">
+      <c r="F38" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="79">
+      <c r="B39" s="78">
         <v>10</v>
       </c>
       <c r="C39" s="35">
@@ -15631,7 +15898,7 @@
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
         <v>#NUM!</v>
       </c>
-      <c r="F39" s="87" t="e">
+      <c r="F39" s="86" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
         <v>#NUM!</v>
       </c>
@@ -15645,11 +15912,11 @@
         <f>SUM(Normal_continua[FilmAffinity])</f>
         <v>1</v>
       </c>
-      <c r="E40" s="64" t="e">
+      <c r="E40" s="63" t="e">
         <f>SUM(Normal_continua[Normal Yo])</f>
         <v>#NUM!</v>
       </c>
-      <c r="F40" s="64" t="e">
+      <c r="F40" s="63" t="e">
         <f>SUM(Normal_continua[Normal F.A.])</f>
         <v>#NUM!</v>
       </c>
@@ -15669,8 +15936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB35113E-0C06-4EAF-8941-AA6250700856}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15682,7 +15949,8 @@
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -15702,7 +15970,7 @@
         <v>130</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1">
         <f>MAX(Tabla1[Duracion])</f>
@@ -15722,14 +15990,14 @@
         <v>130</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="17" cm="1">
         <f t="array" ref="H2">STDEVP(IF(Tabla1[Duracion]&gt;50,Tabla1[Duracion]))</f>
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2">
         <f>MIN(Tabla1[Duracion])</f>
@@ -15740,12 +16008,12 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="17" t="e">
-        <f>_xlfn.VAR.S(Tabla1[Duracion])</f>
-        <v>#DIV/0!</v>
+      <c r="F3" s="17">
+        <f>_xlfn.VAR.P(Tabla1[Duracion])</f>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" cm="1">
         <f t="array" ref="H3">_xlfn.VAR.P(IF(Tabla1[Duracion]&gt;50,Tabla1[Duracion],))</f>
@@ -15754,8 +16022,11 @@
       <c r="Q3" t="s">
         <v>27</v>
       </c>
+      <c r="R3" t="s">
+        <v>65</v>
+      </c>
       <c r="S3" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -15768,33 +16039,33 @@
         <v>0</v>
       </c>
       <c r="S4" s="39" t="e">
-        <f>EXP((Q4-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
-        <v>#DIV/0!</v>
+        <f>(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE))*$C$2</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q5" s="59">
         <v>20</v>
       </c>
-      <c r="R5" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q5)-COUNTIF(Notas!D:D,"&lt;="&amp;Q4)</f>
+      <c r="R5" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q5)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q4)</f>
         <v>0</v>
       </c>
       <c r="S5" s="31" t="e">
-        <f t="shared" ref="S5:S27" si="0">EXP((Q5-$F$2)^2/(-2*$H$2))/SQRT(2*PI()*$H$2)*$C$2*10</f>
-        <v>#DIV/0!</v>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q6" s="59">
         <v>30</v>
       </c>
-      <c r="R6" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q6)-COUNTIF(Notas!D:D,"&lt;="&amp;Q5)</f>
+      <c r="R6" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q6)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q5)</f>
         <v>0</v>
       </c>
       <c r="S6" s="31" t="e">
-        <f>_xlfn.NORM.DIST($Q6,$F$2,SQRT($H$2),TRUE)*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15802,12 +16073,12 @@
       <c r="Q7" s="59">
         <v>40</v>
       </c>
-      <c r="R7" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q7)-COUNTIF(Notas!D:D,"&lt;="&amp;Q6)</f>
+      <c r="R7" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q7)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q6)</f>
         <v>0</v>
       </c>
       <c r="S7" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q7,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q6,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15815,12 +16086,12 @@
       <c r="Q8" s="59">
         <v>50</v>
       </c>
-      <c r="R8" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q8)-COUNTIF(Notas!D:D,"&lt;="&amp;Q7)</f>
+      <c r="R8" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q8)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q7)</f>
         <v>0</v>
       </c>
       <c r="S8" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q8,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q7,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15828,12 +16099,12 @@
       <c r="Q9" s="59">
         <v>60</v>
       </c>
-      <c r="R9" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q9)-COUNTIF(Notas!D:D,"&lt;="&amp;Q8)</f>
+      <c r="R9" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q9)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q8)</f>
         <v>0</v>
       </c>
       <c r="S9" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q9,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q8,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15841,12 +16112,12 @@
       <c r="Q10" s="59">
         <v>70</v>
       </c>
-      <c r="R10" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q10)-COUNTIF(Notas!D:D,"&lt;="&amp;Q9)</f>
+      <c r="R10" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q10)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q9)</f>
         <v>0</v>
       </c>
       <c r="S10" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q10,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q9,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15854,12 +16125,12 @@
       <c r="Q11" s="59">
         <v>80</v>
       </c>
-      <c r="R11" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q11)-COUNTIF(Notas!D:D,"&lt;="&amp;Q10)</f>
+      <c r="R11" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q11)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q10)</f>
         <v>0</v>
       </c>
       <c r="S11" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q11,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q10,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15867,12 +16138,12 @@
       <c r="Q12" s="59">
         <v>90</v>
       </c>
-      <c r="R12" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q12)-COUNTIF(Notas!D:D,"&lt;="&amp;Q11)</f>
+      <c r="R12" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q12)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q11)</f>
         <v>0</v>
       </c>
       <c r="S12" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q12,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q11,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15880,12 +16151,12 @@
       <c r="Q13" s="59">
         <v>100</v>
       </c>
-      <c r="R13" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q13)-COUNTIF(Notas!D:D,"&lt;="&amp;Q12)</f>
+      <c r="R13" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q13)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q12)</f>
         <v>0</v>
       </c>
       <c r="S13" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q13,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q12,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15893,12 +16164,12 @@
       <c r="Q14" s="59">
         <v>110</v>
       </c>
-      <c r="R14" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q14)-COUNTIF(Notas!D:D,"&lt;="&amp;Q13)</f>
+      <c r="R14" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q14)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q13)</f>
         <v>0</v>
       </c>
       <c r="S14" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q14,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q13,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15906,12 +16177,12 @@
       <c r="Q15" s="59">
         <v>120</v>
       </c>
-      <c r="R15" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q15)-COUNTIF(Notas!D:D,"&lt;="&amp;Q14)</f>
+      <c r="R15" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q15)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q14)</f>
         <v>0</v>
       </c>
       <c r="S15" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q15,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q14,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15919,12 +16190,12 @@
       <c r="Q16" s="59">
         <v>130</v>
       </c>
-      <c r="R16" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q16)-COUNTIF(Notas!D:D,"&lt;="&amp;Q15)</f>
+      <c r="R16" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q16)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q15)</f>
         <v>1</v>
       </c>
       <c r="S16" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q16,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q15,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15932,12 +16203,12 @@
       <c r="Q17" s="59">
         <v>140</v>
       </c>
-      <c r="R17" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q17)-COUNTIF(Notas!D:D,"&lt;="&amp;Q16)</f>
+      <c r="R17" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q17)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q16)</f>
         <v>0</v>
       </c>
       <c r="S17" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q17,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q16,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15945,12 +16216,12 @@
       <c r="Q18" s="59">
         <v>150</v>
       </c>
-      <c r="R18" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q18)-COUNTIF(Notas!D:D,"&lt;="&amp;Q17)</f>
+      <c r="R18" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q18)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q17)</f>
         <v>0</v>
       </c>
       <c r="S18" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q18,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q17,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15958,12 +16229,12 @@
       <c r="Q19" s="59">
         <v>160</v>
       </c>
-      <c r="R19" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q19)-COUNTIF(Notas!D:D,"&lt;="&amp;Q18)</f>
+      <c r="R19" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q19)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q18)</f>
         <v>0</v>
       </c>
       <c r="S19" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q19,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q18,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15971,12 +16242,12 @@
       <c r="Q20" s="59">
         <v>170</v>
       </c>
-      <c r="R20" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q20)-COUNTIF(Notas!D:D,"&lt;="&amp;Q19)</f>
+      <c r="R20" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q20)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q19)</f>
         <v>0</v>
       </c>
       <c r="S20" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q20,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q19,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15984,12 +16255,12 @@
       <c r="Q21" s="59">
         <v>180</v>
       </c>
-      <c r="R21" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q21)-COUNTIF(Notas!D:D,"&lt;="&amp;Q20)</f>
+      <c r="R21" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q21)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q20)</f>
         <v>0</v>
       </c>
       <c r="S21" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q21,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q20,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -15997,12 +16268,12 @@
       <c r="Q22" s="59">
         <v>190</v>
       </c>
-      <c r="R22" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q22)-COUNTIF(Notas!D:D,"&lt;="&amp;Q21)</f>
+      <c r="R22" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q22)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q21)</f>
         <v>0</v>
       </c>
       <c r="S22" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q22,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q21,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -16010,12 +16281,12 @@
       <c r="Q23" s="59">
         <v>200</v>
       </c>
-      <c r="R23" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q23)-COUNTIF(Notas!D:D,"&lt;="&amp;Q22)</f>
+      <c r="R23" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q23)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q22)</f>
         <v>0</v>
       </c>
       <c r="S23" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q23,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q22,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -16023,12 +16294,12 @@
       <c r="Q24" s="59">
         <v>210</v>
       </c>
-      <c r="R24" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q24)-COUNTIF(Notas!D:D,"&lt;="&amp;Q23)</f>
+      <c r="R24" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q24)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q23)</f>
         <v>0</v>
       </c>
       <c r="S24" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q24,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q23,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -16036,12 +16307,12 @@
       <c r="Q25" s="59">
         <v>220</v>
       </c>
-      <c r="R25" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q25)-COUNTIF(Notas!D:D,"&lt;="&amp;Q24)</f>
+      <c r="R25" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q25)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q24)</f>
         <v>0</v>
       </c>
       <c r="S25" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q25,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q24,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -16049,12 +16320,12 @@
       <c r="Q26" s="59">
         <v>230</v>
       </c>
-      <c r="R26" s="52">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q26)-COUNTIF(Notas!D:D,"&lt;="&amp;Q25)</f>
+      <c r="R26" s="91">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q26)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q25)</f>
         <v>0</v>
       </c>
       <c r="S26" s="31" t="e">
-        <f>(_xlfn.NORM.DIST($Q26,$F$2,SQRT($H$2),TRUE)-_xlfn.NORM.DIST($Q25,$F$2,SQRT($H$2),TRUE))*$C$2</f>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -16062,25 +16333,28 @@
       <c r="Q27" s="60">
         <v>240</v>
       </c>
-      <c r="R27" s="61">
-        <f>COUNTIF(Notas!D:D,"&lt;="&amp;Q27)-COUNTIF(Notas!D:D,"&lt;="&amp;Q26)</f>
+      <c r="R27" s="92">
+        <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q27)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;Q26)</f>
         <v>0</v>
       </c>
       <c r="S27" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$F$1,SQRT($F$3),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$F$1,SQRT($F$3),TRUE))*$C$2</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="28" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q28" s="25"/>
       <c r="S28" s="17" t="e">
         <f>SUM(S4:S27)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -16100,13 +16374,13 @@
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>5.8154074312521944</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3">
         <v>6.4137430340189105</v>
@@ -16114,13 +16388,13 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>4.4331233333245637</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4">
         <v>1.6223375982874726</v>
@@ -16137,13 +16411,13 @@
       <c r="D6" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="62" t="s">
+      <c r="G6" s="61" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="38" t="s">
@@ -16162,11 +16436,11 @@
         <f>COUNTIF(Notas!G:G,B7)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="67">
+      <c r="E7" s="66">
         <f>LOG(_xlfn.NORM.DIST($B7,$E$3,SQRT($E$4),TRUE)^$C7)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="67">
+      <c r="F7" s="66">
         <f>LOG(_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE)^D7)</f>
         <v>0</v>
       </c>
@@ -16191,11 +16465,11 @@
         <f>COUNTIF(Notas!G:G,B8)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="67">
         <f>LOG((_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE))^C8)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="67">
         <f>LOG((_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE))^$D8)</f>
         <v>0</v>
       </c>
@@ -16220,11 +16494,11 @@
         <f>COUNTIF(Notas!G:G,B9)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="67">
         <f t="shared" ref="E9:E26" si="2">LOG((_xlfn.NORM.DIST(B9,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE))^C9)</f>
         <v>-0.510165965966482</v>
       </c>
-      <c r="F9" s="68">
+      <c r="F9" s="67">
         <f t="shared" ref="F9:F26" si="3">LOG((_xlfn.NORM.DIST(B9,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE))^$D9)</f>
         <v>0</v>
       </c>
@@ -16249,11 +16523,11 @@
         <f>COUNTIF(Notas!G:G,B10)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="67">
         <f t="shared" si="2"/>
         <v>-0.91513515531428258</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16278,11 +16552,11 @@
         <f>COUNTIF(Notas!G:G,B11)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="68">
+      <c r="E11" s="67">
         <f t="shared" si="2"/>
         <v>-0.41106363090054054</v>
       </c>
-      <c r="F11" s="68">
+      <c r="F11" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16307,11 +16581,11 @@
         <f>COUNTIF(Notas!G:G,B12)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="68">
+      <c r="F12" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16336,11 +16610,11 @@
         <f>COUNTIF(Notas!G:G,B13)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="68">
+      <c r="E13" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16365,11 +16639,11 @@
         <f>COUNTIF(Notas!G:G,B14)</f>
         <v>1</v>
       </c>
-      <c r="E14" s="68">
+      <c r="E14" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F14" s="68">
+      <c r="F14" s="67">
         <f t="shared" si="3"/>
         <v>-1.7456299905769432</v>
       </c>
@@ -16394,11 +16668,11 @@
         <f>COUNTIF(Notas!G:G,B15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="68">
+      <c r="E15" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F15" s="68">
+      <c r="F15" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16423,11 +16697,11 @@
         <f>COUNTIF(Notas!G:G,B16)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="68">
+      <c r="E16" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F16" s="68">
+      <c r="F16" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16452,11 +16726,11 @@
         <f>COUNTIF(Notas!G:G,B17)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="68">
+      <c r="E17" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F17" s="68">
+      <c r="F17" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16481,11 +16755,11 @@
         <f>COUNTIF(Notas!G:G,B18)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="68">
+      <c r="E18" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18" s="68">
+      <c r="F18" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16510,11 +16784,11 @@
         <f>COUNTIF(Notas!G:G,B19)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="68">
+      <c r="E19" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F19" s="68">
+      <c r="F19" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16539,11 +16813,11 @@
         <f>COUNTIF(Notas!G:G,B20)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16568,11 +16842,11 @@
         <f>COUNTIF(Notas!G:G,B21)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="68">
+      <c r="E21" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F21" s="68">
+      <c r="F21" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16597,11 +16871,11 @@
         <f>COUNTIF(Notas!G:G,B22)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="68">
+      <c r="E22" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F22" s="68">
+      <c r="F22" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16626,11 +16900,11 @@
         <f>COUNTIF(Notas!G:G,B23)</f>
         <v>0</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23" s="68">
+      <c r="F23" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16655,11 +16929,11 @@
         <f>COUNTIF(Notas!G:G,B24)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="68">
+      <c r="E24" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16684,11 +16958,11 @@
         <f>COUNTIF(Notas!G:G,B25)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="68">
+      <c r="E25" s="67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25" s="68">
+      <c r="F25" s="67">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16713,11 +16987,11 @@
         <f>COUNTIF(Notas!G:G,B26)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="69">
+      <c r="E26" s="68">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F26" s="69">
+      <c r="F26" s="68">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -16756,21 +17030,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="70"/>
+    <col min="2" max="2" width="11.42578125" style="69"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="70">
+        <v>40</v>
+      </c>
+      <c r="B1" s="69">
         <f>AVERAGE(Visionados)</f>
         <v>26047</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="70">
+        <v>45</v>
+      </c>
+      <c r="E1" s="69">
         <f>MAX(Visionados)</f>
         <v>26047</v>
       </c>
@@ -16779,12 +17053,12 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="70">
+      <c r="B2" s="69">
         <f>MEDIAN(Visionados)</f>
         <v>26047</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <f>MIN(Visionados)</f>
@@ -16793,13 +17067,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="70">
+        <v>62533</v>
+      </c>
+      <c r="C4" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="71">
-        <v>62533</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
       </c>
       <c r="D4" s="2">
         <f>COUNTIF(Visionados,"&lt;="&amp;B4)/Pelis</f>

</xml_diff>

<commit_message>
Clean excel first row
</commit_message>
<xml_diff>
--- a/res/Readdata/Plantilla.xlsx
+++ b/res/Readdata/Plantilla.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27050E3D-502E-43BD-907F-6285F159D325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2EE8E1-7BBF-4135-BAC2-1FC93FAFE0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -932,31 +932,6 @@
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF33CC33"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
@@ -1250,6 +1225,9 @@
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -1261,6 +1239,28 @@
           <color indexed="64"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FF33CC33"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1363,9 +1363,6 @@
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>3.9899655051561691</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1375,9 +1372,6 @@
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>1.9167363412716298</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1725,13 +1719,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1910,64 +1904,64 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5.7925488621560443E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3035236315983354E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1061780178500785E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.478188057990508E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2685349595145655E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2914235407240124E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5148654453109976E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.8550256516192611E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.1785364468036045E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.320822664083477E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.1184278782524775E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.4470686747302468E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.2533204903991528E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.5688304490451506E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.5018583302613351E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.2092542712243848E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.8588465796543967E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.5945946585823285E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5141400473080999E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.6624614389095349E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,9 +2322,6 @@
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>26047</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2340,9 +2331,6 @@
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>1.9167363412716298</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2678,9 +2666,6 @@
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>26047</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2690,9 +2675,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3125,7 +3107,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -3421,127 +3403,127 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.17466068512885846</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14415433019917617</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11897623612229652</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.8195765207123142E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1044825579294599E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6889480817466263E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5206518269973914E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.5564109965361421E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.7605851301524718E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1037587548346401E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5616541242405422E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.114233859837511E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.7449603253556711E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4401843594063601E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.188640772480587E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.8103196078703769E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.0968424638265812E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6826424117142347E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.5154475096130806E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.5521156687917674E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.7570400272948223E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.1008328420708553E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.5592392534048436E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.1122407719963432E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.7433153516024369E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.4388266978958564E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.1875202410597252E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9.8010714215179817E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8.089209572039735E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.6763426860350084E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.5102480983382218E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.54782439025192E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.7534982664044758E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.0979096875649592E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.5568266590669797E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.1102495630387352E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.741671928565669E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.4374703162522984E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.1864007659645459E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.7918319534207043E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8.0815838757852809E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3799,9 +3781,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3811,9 +3790,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4163,7 +4139,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4757,13 +4733,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -4949,7 +4925,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -5374,13 +5350,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -5977,9 +5953,6 @@
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>130</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5989,9 +5962,6 @@
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>1.9167363412716298</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6313,9 +6283,6 @@
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>130</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6325,9 +6292,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048575"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6718,7 +6682,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -7311,7 +7275,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -7473,64 +7437,64 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.0670751456919622E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.9532107336445599E-6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6530954287035938E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0765310065299676E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.9576485490160656E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6187638771519059E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.400945940858444E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.796263352278547E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.744170915363889E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.7027571512691578E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.10305544605641351</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13608606230328921</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.15434239427286445</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.15034443690384314</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.12578234601277249</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.0381567263075557E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.5778081184472583E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.9564091935930681E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.345781882502084E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2611911884490326E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15519,46 +15483,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:O1048576" totalsRowShown="0" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E78E77D8-C91F-4F8B-8288-E3F750D0DE1E}" name="Tabla1" displayName="Tabla1" ref="A1:O1048576" totalsRowShown="0" tableBorderDxfId="31">
   <autoFilter ref="A1:O1048576" xr:uid="{B7E8E3F6-4A56-4C38-9CDA-83612E98463A}"/>
   <tableColumns count="15">
-    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="32"/>
-    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{0AB4C432-387A-4CA4-B057-810DBFBD7743}" name="Id" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{D4B468C3-7CDA-4F31-9638-09A527779C87}" name="Mia" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{65EE12B7-2552-4910-A353-7AE48A3D7AA6}" name="FA"/>
-    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{2E72113E-50BE-41C7-8BFD-59035950093F}" name="Varianza_FA" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{7EA2D8C1-B85E-4AD7-8EDB-8F6DF95FD884}" name="Prop_aprobados_FA" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1D6E5D7A-6668-40F4-BA00-3A91CC9AC5BF}" name="Duracion" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{E8F61A2B-CC2B-4DF4-AE8C-8C20147ABC40}" name="Visionados" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{2E72113E-50BE-41C7-8BFD-59035950093F}" name="Varianza_FA" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{7EA2D8C1-B85E-4AD7-8EDB-8F6DF95FD884}" name="Prop_aprobados_FA" dataDxfId="25"/>
     <tableColumn id="5" xr3:uid="{FF19B5AE-C56B-4CA5-B812-840E5C110430}" name="FA_redondeo"/>
     <tableColumn id="6" xr3:uid="{20BAA72D-A773-488D-B544-DAD2EF762D99}" name="Diferencia"/>
     <tableColumn id="7" xr3:uid="{E40D682E-5136-4AEB-BEE2-B6B87967AFB0}" name="Diferencia_abs"/>
-    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me_ha_gustado" dataDxfId="27">
+    <tableColumn id="8" xr3:uid="{7FF8C3DD-322A-4235-83BB-7D30EE81A4BF}" name="Me_ha_gustado" dataDxfId="24">
       <calculatedColumnFormula>IF($I2&gt;0,1,0.1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia_ruido" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{C6FE0FC6-41FF-42DC-95D7-3BA16482D743}" name="Mia_ruido" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{F6539847-A910-4F63-B100-298A992D7D82}" name="FA_ruido" dataDxfId="22">
       <calculatedColumnFormula>C2+(RAND()-0.5)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{1D5E088C-37BD-4B8F-BD0A-602AB1027E68}" name="Mia_rees" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{19C47E50-9952-473E-A08A-65D82E3962A6}" name="FA_rees" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}" name="Normal_discreta" displayName="Normal_discreta" ref="B3:F13" totalsRowShown="0" tableBorderDxfId="19">
   <autoFilter ref="B3:F13" xr:uid="{B2653B35-92CE-4059-8AD4-DBAEE93A2DB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{AF390C70-03AA-431F-A8ED-30C0DCB9DFDF}" name="Puntos" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{598A8C01-1D1C-420B-8694-D25317E8EB25}" name="Yo" dataDxfId="17">
       <calculatedColumnFormula>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="18">
+    <tableColumn id="3" xr3:uid="{B4249F61-8354-492B-A8D7-1FC4AD8817B0}" name="FilmAffinity" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{02468E76-7BC0-4435-8771-BCB059D4E47D}" name="Normal yo" dataDxfId="15">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(B4,MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(B3,MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="17">
+    <tableColumn id="5" xr3:uid="{A770DBA5-7A85-4CE1-BE0D-42E2474C56E7}" name="Normal F.A." dataDxfId="14">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B4,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15567,18 +15531,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}" name="Normal_continua" displayName="Normal_continua" ref="B19:F39" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="B19:F39" xr:uid="{E0D9576F-E16E-4D59-8D7E-7FCBC06A5729}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{0239E3C8-6B59-4E95-8128-0CA23E525DC8}" name="Puntos " dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{DD42BB33-62C8-4E24-BD0D-81BEC813AAE5}" name="Yo" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{22EF7FA5-DCB7-4C87-8C5D-261E5B9E0111}" name="FilmAffinity" dataDxfId="9">
       <calculatedColumnFormula>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="11">
+    <tableColumn id="4" xr3:uid="{7D5AFCB4-B113-4668-BD2B-91ABFA1287DC}" name="Normal Yo" dataDxfId="8">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="10">
+    <tableColumn id="5" xr3:uid="{236D39DF-9177-499F-BE2C-6E237E4F9DE9}" name="Normal F.A." dataDxfId="7">
       <calculatedColumnFormula>_xlfn.NORM.DIST(B20,MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15587,14 +15551,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5AFFC25-E554-49FC-9485-58BDC89F7ED4}" name="Tiempos_normal" displayName="Tiempos_normal" ref="P3:R27" totalsRowShown="0" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5AFFC25-E554-49FC-9485-58BDC89F7ED4}" name="Tiempos_normal" displayName="Tiempos_normal" ref="P3:R27" totalsRowShown="0" tableBorderDxfId="6">
   <autoFilter ref="P3:R27" xr:uid="{E5AFFC25-E554-49FC-9485-58BDC89F7ED4}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9480A362-FEE1-48D4-8ACA-A2492EA7E360}" name="Minutos" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{9480A362-FEE1-48D4-8ACA-A2492EA7E360}" name="Minutos" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{A2427276-3F9C-4E12-9EC9-F89716AF732E}" name="Ocurrencias">
       <calculatedColumnFormula>COUNTIF(Notas!D:D,"&lt;="&amp;P4)-COUNTIF(Notas!D:D,"&lt;="&amp;P3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FCC37941-690A-4CC1-A9C7-96E0FC9A264C}" name="Normal" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{FCC37941-690A-4CC1-A9C7-96E0FC9A264C}" name="Normal" dataDxfId="4">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],$E$1,SQRT($I$1),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),$E$1,SQRT($I$1),TRUE))*$A$2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15603,14 +15567,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F0A7F444-E539-4385-B444-E33603B4FE15}" name="TablaVisionados" displayName="TablaVisionados" ref="L25:N66" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F0A7F444-E539-4385-B444-E33603B4FE15}" name="TablaVisionados" displayName="TablaVisionados" ref="L25:N66" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="L25:N66" xr:uid="{F0A7F444-E539-4385-B444-E33603B4FE15}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9AF17232-92AF-4207-B009-B6B5AF654446}" name="Visionados" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{99199FEC-59E2-4E0B-8DE1-0FB18D37FACC}" name="Ocurrencias" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{9AF17232-92AF-4207-B009-B6B5AF654446}" name="Visionados" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{99199FEC-59E2-4E0B-8DE1-0FB18D37FACC}" name="Ocurrencias" dataDxfId="1">
       <calculatedColumnFormula>COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E4F3B18F-C843-48A1-92DE-26F131488BFD}" name="Normal" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{E4F3B18F-C843-48A1-92DE-26F131488BFD}" name="Normal" dataDxfId="0">
       <calculatedColumnFormula>(_xlfn.NORM.DIST(TablaVisionados[[#This Row],[Visionados]],MediaVisionados,SQRT(VarianzaVisionados),TRUE)-_xlfn.NORM.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),MediaVisionados,SQRT(VarianzaVisionados),TRUE))*Pelis</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15960,59 +15924,8 @@
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
-        <v>555555</v>
-      </c>
-      <c r="B2" s="17">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2" s="67">
-        <v>130</v>
-      </c>
-      <c r="E2" s="67">
-        <v>26047</v>
-      </c>
-      <c r="F2" s="73">
-        <v>2.1</v>
-      </c>
-      <c r="G2" s="73">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H2">
-        <f t="shared" ref="H2" si="0">ROUND($C2*2, 0)/2</f>
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <f>B2-C2</f>
-        <v>-2</v>
-      </c>
-      <c r="J2">
-        <f t="shared" ref="J2" si="1">ABS(I2)</f>
-        <v>2</v>
-      </c>
-      <c r="K2" s="72">
-        <f t="shared" ref="K2" si="2">IF($I2&gt;0,1,0.1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="L2" s="28">
-        <f t="shared" ref="L2" ca="1" si="3">B2+RAND()-0.5</f>
-        <v>1.9167363412716298</v>
-      </c>
-      <c r="M2" s="28">
-        <f t="shared" ref="M2" ca="1" si="4">C2+(RAND()-0.5)/10</f>
-        <v>3.9899655051561691</v>
-      </c>
-      <c r="N2" s="65">
-        <f t="shared" ref="N2" si="5">(B2-1)*10/9</f>
-        <v>1.1111111111111112</v>
-      </c>
-      <c r="O2" s="65">
-        <f t="shared" ref="O2" si="6">(C2-1)*10/9</f>
-        <v>3.3333333333333335</v>
-      </c>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
       <c r="P2" s="52"/>
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
@@ -16269,10 +16182,10 @@
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16355,7 +16268,7 @@
       </c>
       <c r="B1">
         <f>COUNT(Tabla1[Mia])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="25"/>
     </row>
@@ -16365,7 +16278,7 @@
       </c>
       <c r="B2">
         <f>COUNT(Tabla1[FA])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="25"/>
     </row>
@@ -16373,30 +16286,30 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="7" t="e">
         <f>AVERAGE(Tabla1[FA])</f>
-        <v>4</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="8" t="e">
         <f>STDEVP(Tabla1[FA])</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="8" t="e">
         <f>_xlfn.VAR.P(Tabla1[FA])</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="7" t="e">
         <f>MEDIAN(Tabla1[FA])</f>
-        <v>4</v>
+        <v>#NUM!</v>
       </c>
       <c r="I3" s="27" t="s">
         <v>19</v>
@@ -16410,44 +16323,44 @@
       </c>
       <c r="L3" s="53">
         <f>MAX(Tabla1[FA])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
       </c>
       <c r="N3" s="53">
         <f>MIN(Notas!C:C)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="5" t="e">
         <f>AVERAGE(Tabla1[Mia])</f>
-        <v>2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="6" t="e">
         <f>STDEVP(NotasMias)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="6" t="e">
         <f>_xlfn.VAR.P(NotasMias)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="5" t="e">
         <f>MEDIAN(NotasMias)</f>
-        <v>2</v>
+        <v>#NUM!</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>19</v>
@@ -16461,23 +16374,23 @@
       </c>
       <c r="L4" s="54">
         <f>MAX(NotasMias)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M4" t="s">
         <v>23</v>
       </c>
       <c r="N4" s="54">
         <f>MIN(NotasMias)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="e">
         <f>AVERAGE(Tabla1[Diferencia])</f>
-        <v>-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G5" s="25"/>
     </row>
@@ -16485,16 +16398,16 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="e">
         <f>AVERAGE(Tabla1[Diferencia_abs])</f>
-        <v>2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="e">
         <f>STDEVP(Tabla1[Diferencia_abs])</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="1"/>
@@ -16506,7 +16419,7 @@
       </c>
       <c r="B8">
         <f>MAX(Tabla1[Diferencia_abs])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -16524,7 +16437,7 @@
       </c>
       <c r="B9">
         <f>MIN(Tabla1[Diferencia])</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -16533,16 +16446,16 @@
       </c>
       <c r="B10">
         <f>MAX(Tabla1[Diferencia])</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="2" t="e">
         <f>AVERAGE(Tabla1[Me_ha_gustado])</f>
-        <v>0.1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -16582,60 +16495,60 @@
       <c r="A16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="15" t="e">
         <f>(MediaFA-1)*10/9</f>
-        <v>3.3333333333333335</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="15" t="e">
         <f>STDEVP(Tabla1[FA_rees])</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E16" s="60"/>
       <c r="F16" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="69">
+      <c r="G16" s="69" t="e">
         <f>COUNTIF(NotasFA,"&lt;="&amp;G15)/Pelis_con_nota</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="69">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="69" t="e">
         <f>COUNTIF(Tabla1[Visionados],"&lt;="&amp;H15)/Pelis_con_nota</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="69">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="69" t="e">
         <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;I15)/Pelis_con_nota</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="69">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="69" t="e">
         <f>COUNTIF(Tabla1[Varianza_FA],"&lt;="&amp;J15)/Pelis_con_nota</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="16" t="e">
         <f>(MediaMia-1)*10/9</f>
-        <v>1.1111111111111112</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="11" t="e">
         <f>STDEVP(Tabla1[Mia_rees])</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E17" s="60"/>
       <c r="F17" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="70">
+      <c r="G17" s="70" t="e">
         <f>COUNTIF(NotasMias,"&lt;="&amp;G15)/Pelis</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -16708,11 +16621,11 @@
       </c>
       <c r="E4" s="39" t="e">
         <f>_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F4" s="61" t="e">
         <f>_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -16721,7 +16634,7 @@
       </c>
       <c r="C5" s="3">
         <f>COUNTIF(NotasMias,Normal_discreta[[#This Row],[Puntos]])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
@@ -16729,11 +16642,11 @@
       </c>
       <c r="E5" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F5" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -16750,11 +16663,11 @@
       </c>
       <c r="E6" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F6" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -16767,15 +16680,15 @@
       </c>
       <c r="D7" s="4">
         <f ca="1">COUNTIFS(NotasFA,"&gt;"&amp;OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0)+0.5,NotasFA,"&lt;="&amp;(Normal_discreta[[#This Row],[Puntos]]+0.5))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F7" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -16792,11 +16705,11 @@
       </c>
       <c r="E8" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F8" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -16813,11 +16726,11 @@
       </c>
       <c r="E9" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F9" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -16834,11 +16747,11 @@
       </c>
       <c r="E10" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F10" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -16855,11 +16768,11 @@
       </c>
       <c r="E11" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F11" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -16876,11 +16789,11 @@
       </c>
       <c r="E12" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F12" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16897,21 +16810,21 @@
       </c>
       <c r="E13" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F13" s="77" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_discreta[[#This Row],[Puntos]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_discreta[[#This Row],[Puntos]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E14" s="61" t="e">
         <f>SUM(E4:E13)</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F14" s="61" t="e">
         <f>SUM(F4:F13)</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16945,18 +16858,18 @@
       </c>
       <c r="E20" s="39" t="e">
         <f>(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F20" s="83" t="e">
         <f>_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R20" t="s">
         <v>25</v>
       </c>
       <c r="S20" s="30" t="e" cm="1">
         <f t="array" aca="1" ref="S20" ca="1">_xlfn.CHISQ.DIST(SUM((C22:C39-E22:E39)^2/E22:E39),18,TRUE)</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
@@ -16973,18 +16886,18 @@
       </c>
       <c r="E21" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F21" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R21" t="s">
         <v>26</v>
       </c>
       <c r="S21" s="30" t="e" cm="1">
         <f t="array" aca="1" ref="S21" ca="1">_xlfn.CHISQ.DIST(SUM((D25:D39-F25:F39)^2/F25:F39),18,TRUE)</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -16993,7 +16906,7 @@
       </c>
       <c r="C22" s="33">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D22" s="43">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
@@ -17001,11 +16914,11 @@
       </c>
       <c r="E22" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F22" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -17014,7 +16927,7 @@
       </c>
       <c r="C23" s="33">
         <f>COUNTIF(NotasMias,Normal_continua[[#This Row],[Puntos ]])/2</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D23" s="43">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
@@ -17022,11 +16935,11 @@
       </c>
       <c r="E23" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F23" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -17035,7 +16948,7 @@
       </c>
       <c r="C24" s="33">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())),INDIRECT(ADDRESS(ROW()+1,COLUMN())))</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D24" s="43">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
@@ -17043,11 +16956,11 @@
       </c>
       <c r="E24" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F24" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -17064,11 +16977,11 @@
       </c>
       <c r="E25" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F25" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -17085,11 +16998,11 @@
       </c>
       <c r="E26" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F26" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
@@ -17102,15 +17015,15 @@
       </c>
       <c r="D27" s="43">
         <f>COUNTIF(Tabla1[FA_redondeo],Normal_continua[[#This Row],[Puntos ]])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F27" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
@@ -17127,11 +17040,11 @@
       </c>
       <c r="E28" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F28" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
@@ -17148,11 +17061,11 @@
       </c>
       <c r="E29" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F29" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
@@ -17169,11 +17082,11 @@
       </c>
       <c r="E30" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F30" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
@@ -17190,11 +17103,11 @@
       </c>
       <c r="E31" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F31" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
@@ -17211,11 +17124,11 @@
       </c>
       <c r="E32" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F32" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -17232,11 +17145,11 @@
       </c>
       <c r="E33" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F33" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -17253,11 +17166,11 @@
       </c>
       <c r="E34" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F34" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -17274,11 +17187,11 @@
       </c>
       <c r="E35" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F35" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -17295,11 +17208,11 @@
       </c>
       <c r="E36" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F36" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -17316,11 +17229,11 @@
       </c>
       <c r="E37" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F37" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -17337,11 +17250,11 @@
       </c>
       <c r="E38" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F38" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17358,29 +17271,29 @@
       </c>
       <c r="E39" s="40" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaMia,SQRT(VarMia),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaMia,SQRT(VarMia),TRUE))*Pelis</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F39" s="84" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Normal_continua[[#This Row],[Puntos ]],MediaFA,SQRT(VarFA),TRUE)-_xlfn.NORM.DIST(OFFSET(Normal_continua[[#This Row],[Puntos ]],-1,0),MediaFA,SQRT(VarFA),TRUE))*Pelis_con_nota</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C40" s="46">
         <f ca="1">SUM(Normal_continua[Yo])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="17">
         <f>SUM(Normal_continua[FilmAffinity])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="61" t="e">
         <f>SUM(Normal_continua[Normal Yo])</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F40" s="61" t="e">
         <f>SUM(Normal_continua[Normal F.A.])</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -17425,35 +17338,35 @@
       </c>
       <c r="C1">
         <f>COUNT(Tabla1[Duracion])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="17">
+      <c r="E1" s="17" t="e">
         <f>AVERAGE(Tabla1[Duracion])</f>
-        <v>130</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="G1">
+      <c r="G1" t="e">
         <f>MEDIAN(Tabla1[Duracion])</f>
-        <v>130</v>
+        <v>#NUM!</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="91">
+      <c r="I1" s="91" t="e">
         <f>_xlfn.VAR.P(Tabla1[Duracion])</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K1" t="s">
         <v>27</v>
       </c>
       <c r="L1">
         <f>MAX(Tabla1[Duracion])</f>
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -17465,14 +17378,14 @@
       </c>
       <c r="C2">
         <f>COUNTIF(Tabla1[Duracion],"&gt;="&amp;60)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="17" t="e">
         <f>AVERAGEIF(Tabla1[Duracion],"&gt;50")</f>
-        <v>130</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
@@ -17486,14 +17399,14 @@
       </c>
       <c r="I2" s="91" cm="1">
         <f t="array" ref="I2">_xlfn.VAR.P(IF(Tabla1[Duracion]&gt;50,Tabla1[Duracion],))</f>
-        <v>1.6117095947250967E-2</v>
+        <v>0</v>
       </c>
       <c r="K2" t="s">
         <v>28</v>
       </c>
       <c r="L2">
         <f>MIN(Tabla1[Duracion])</f>
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17518,7 +17431,7 @@
       </c>
       <c r="R4" s="38" t="e">
         <f>(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -17531,7 +17444,7 @@
       </c>
       <c r="R5" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -17544,7 +17457,7 @@
       </c>
       <c r="R6" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -17557,7 +17470,7 @@
       </c>
       <c r="R7" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -17570,7 +17483,7 @@
       </c>
       <c r="R8" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -17583,7 +17496,7 @@
       </c>
       <c r="R9" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -17596,7 +17509,7 @@
       </c>
       <c r="R10" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -17609,7 +17522,7 @@
       </c>
       <c r="R11" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -17622,7 +17535,7 @@
       </c>
       <c r="R12" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -17635,7 +17548,7 @@
       </c>
       <c r="R13" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -17648,7 +17561,7 @@
       </c>
       <c r="R14" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -17661,7 +17574,7 @@
       </c>
       <c r="R15" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -17670,11 +17583,11 @@
       </c>
       <c r="Q16" s="89">
         <f>COUNTIF(Tabla1[Duracion],"&lt;="&amp;P16)-COUNTIF(Tabla1[Duracion],"&lt;="&amp;P15)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="16:18" x14ac:dyDescent="0.25">
@@ -17687,7 +17600,7 @@
       </c>
       <c r="R17" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="16:18" x14ac:dyDescent="0.25">
@@ -17700,7 +17613,7 @@
       </c>
       <c r="R18" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="16:18" x14ac:dyDescent="0.25">
@@ -17713,7 +17626,7 @@
       </c>
       <c r="R19" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="16:18" x14ac:dyDescent="0.25">
@@ -17726,7 +17639,7 @@
       </c>
       <c r="R20" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="16:18" x14ac:dyDescent="0.25">
@@ -17739,7 +17652,7 @@
       </c>
       <c r="R21" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="16:18" x14ac:dyDescent="0.25">
@@ -17752,7 +17665,7 @@
       </c>
       <c r="R22" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="16:18" x14ac:dyDescent="0.25">
@@ -17765,7 +17678,7 @@
       </c>
       <c r="R23" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="16:18" x14ac:dyDescent="0.25">
@@ -17778,7 +17691,7 @@
       </c>
       <c r="R24" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="16:18" x14ac:dyDescent="0.25">
@@ -17791,7 +17704,7 @@
       </c>
       <c r="R25" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="16:18" x14ac:dyDescent="0.25">
@@ -17804,7 +17717,7 @@
       </c>
       <c r="R26" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="16:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17817,14 +17730,14 @@
       </c>
       <c r="R27" s="31" t="e">
         <f ca="1">(_xlfn.NORM.DIST(Tiempos_normal[[#This Row],[Minutos]],DuracionMedia,SQRT(DuracionVarianza),TRUE)-_xlfn.NORM.DIST(OFFSET(Tiempos_normal[[#This Row],[Minutos]],-1,0),DuracionMedia,SQRT(DuracionVarianza),TRUE))*ContarDuraciones</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="16:18" x14ac:dyDescent="0.25">
       <c r="P28" s="25"/>
       <c r="R28" s="17" t="e">
         <f>SUM(R4:R27)</f>
-        <v>#NUM!</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -17924,11 +17837,11 @@
       </c>
       <c r="G7" s="39">
         <f>_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE)*Pelis</f>
-        <v>5.7925488621560443E-3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="47">
         <f>_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)*Pelis</f>
-        <v>1.0670751456919622E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -17953,11 +17866,11 @@
       </c>
       <c r="G8" s="40">
         <f t="shared" ref="G8:G26" si="0">(_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B7,$E$3,SQRT($E$4),TRUE))*Pelis</f>
-        <v>5.3035236315983354E-3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="48">
         <f t="shared" ref="H8:H26" si="1">(_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B7,$G$3,SQRT($G$4),TRUE))*Pelis</f>
-        <v>8.9532107336445599E-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -17966,7 +17879,7 @@
       </c>
       <c r="C9" s="33">
         <f>(C8+C10)/2</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D9" s="43">
         <f>COUNTIF(Notas!H:H,B9)</f>
@@ -17974,7 +17887,7 @@
       </c>
       <c r="E9" s="65">
         <f t="shared" ref="E9:E26" si="2">LOG((_xlfn.NORM.DIST(B9,$E$3,SQRT($E$4),TRUE)-_xlfn.NORM.DIST(B8,$E$3,SQRT($E$4),TRUE))^C9)</f>
-        <v>-0.510165965966482</v>
+        <v>0</v>
       </c>
       <c r="F9" s="65">
         <f t="shared" ref="F9:F26" si="3">LOG((_xlfn.NORM.DIST(B9,$G$3,SQRT($G$4),TRUE)-_xlfn.NORM.DIST(B8,$G$3,SQRT($G$4),TRUE))^$D9)</f>
@@ -17982,11 +17895,11 @@
       </c>
       <c r="G9" s="40">
         <f t="shared" si="0"/>
-        <v>9.1061780178500785E-3</v>
+        <v>0</v>
       </c>
       <c r="H9" s="48">
         <f t="shared" si="1"/>
-        <v>4.6530954287035938E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -17995,7 +17908,7 @@
       </c>
       <c r="C10" s="33">
         <f>COUNTIF(Notas!B:B,B10)/2</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D10" s="43">
         <f>COUNTIF(Notas!H:H,B10)</f>
@@ -18003,7 +17916,7 @@
       </c>
       <c r="E10" s="65">
         <f t="shared" si="2"/>
-        <v>-0.91513515531428258</v>
+        <v>0</v>
       </c>
       <c r="F10" s="65">
         <f t="shared" si="3"/>
@@ -18011,11 +17924,11 @@
       </c>
       <c r="G10" s="40">
         <f t="shared" si="0"/>
-        <v>1.478188057990508E-2</v>
+        <v>0</v>
       </c>
       <c r="H10" s="48">
         <f t="shared" si="1"/>
-        <v>2.0765310065299676E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -18024,7 +17937,7 @@
       </c>
       <c r="C11" s="33">
         <f>(C10+C12)/2</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D11" s="43">
         <f>COUNTIF(Notas!H:H,B11)</f>
@@ -18032,7 +17945,7 @@
       </c>
       <c r="E11" s="65">
         <f t="shared" si="2"/>
-        <v>-0.41106363090054054</v>
+        <v>0</v>
       </c>
       <c r="F11" s="65">
         <f t="shared" si="3"/>
@@ -18040,11 +17953,11 @@
       </c>
       <c r="G11" s="40">
         <f t="shared" si="0"/>
-        <v>2.2685349595145655E-2</v>
+        <v>0</v>
       </c>
       <c r="H11" s="48">
         <f t="shared" si="1"/>
-        <v>7.9576485490160656E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -18069,11 +17982,11 @@
       </c>
       <c r="G12" s="40">
         <f t="shared" si="0"/>
-        <v>3.2914235407240124E-2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="48">
         <f t="shared" si="1"/>
-        <v>2.6187638771519059E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -18098,11 +18011,11 @@
       </c>
       <c r="G13" s="40">
         <f t="shared" si="0"/>
-        <v>4.5148654453109976E-2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="48">
         <f t="shared" si="1"/>
-        <v>7.400945940858444E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -18115,7 +18028,7 @@
       </c>
       <c r="D14" s="43">
         <f>COUNTIF(Notas!H:H,B14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="65">
         <f t="shared" si="2"/>
@@ -18123,15 +18036,15 @@
       </c>
       <c r="F14" s="65">
         <f t="shared" si="3"/>
-        <v>-1.7456299905769432</v>
+        <v>0</v>
       </c>
       <c r="G14" s="40">
         <f t="shared" si="0"/>
-        <v>5.8550256516192611E-2</v>
+        <v>0</v>
       </c>
       <c r="H14" s="48">
         <f t="shared" si="1"/>
-        <v>1.796263352278547E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -18156,11 +18069,11 @@
       </c>
       <c r="G15" s="40">
         <f t="shared" si="0"/>
-        <v>7.1785364468036045E-2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="48">
         <f t="shared" si="1"/>
-        <v>3.744170915363889E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -18185,11 +18098,11 @@
       </c>
       <c r="G16" s="40">
         <f t="shared" si="0"/>
-        <v>8.320822664083477E-2</v>
+        <v>0</v>
       </c>
       <c r="H16" s="48">
         <f t="shared" si="1"/>
-        <v>6.7027571512691578E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -18214,11 +18127,11 @@
       </c>
       <c r="G17" s="40">
         <f t="shared" si="0"/>
-        <v>9.1184278782524775E-2</v>
+        <v>0</v>
       </c>
       <c r="H17" s="48">
         <f t="shared" si="1"/>
-        <v>0.10305544605641351</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -18243,11 +18156,11 @@
       </c>
       <c r="G18" s="40">
         <f t="shared" si="0"/>
-        <v>9.4470686747302468E-2</v>
+        <v>0</v>
       </c>
       <c r="H18" s="48">
         <f t="shared" si="1"/>
-        <v>0.13608606230328921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -18272,11 +18185,11 @@
       </c>
       <c r="G19" s="40">
         <f t="shared" si="0"/>
-        <v>9.2533204903991528E-2</v>
+        <v>0</v>
       </c>
       <c r="H19" s="48">
         <f t="shared" si="1"/>
-        <v>0.15434239427286445</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -18301,11 +18214,11 @@
       </c>
       <c r="G20" s="40">
         <f t="shared" si="0"/>
-        <v>8.5688304490451506E-2</v>
+        <v>0</v>
       </c>
       <c r="H20" s="48">
         <f t="shared" si="1"/>
-        <v>0.15034443690384314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -18330,11 +18243,11 @@
       </c>
       <c r="G21" s="40">
         <f t="shared" si="0"/>
-        <v>7.5018583302613351E-2</v>
+        <v>0</v>
       </c>
       <c r="H21" s="48">
         <f t="shared" si="1"/>
-        <v>0.12578234601277249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -18359,11 +18272,11 @@
       </c>
       <c r="G22" s="40">
         <f t="shared" si="0"/>
-        <v>6.2092542712243848E-2</v>
+        <v>0</v>
       </c>
       <c r="H22" s="48">
         <f t="shared" si="1"/>
-        <v>9.0381567263075557E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -18388,11 +18301,11 @@
       </c>
       <c r="G23" s="40">
         <f t="shared" si="0"/>
-        <v>4.8588465796543967E-2</v>
+        <v>0</v>
       </c>
       <c r="H23" s="48">
         <f t="shared" si="1"/>
-        <v>5.5778081184472583E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -18417,11 +18330,11 @@
       </c>
       <c r="G24" s="40">
         <f t="shared" si="0"/>
-        <v>3.5945946585823285E-2</v>
+        <v>0</v>
       </c>
       <c r="H24" s="48">
         <f t="shared" si="1"/>
-        <v>2.9564091935930681E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -18446,11 +18359,11 @@
       </c>
       <c r="G25" s="40">
         <f t="shared" si="0"/>
-        <v>2.5141400473080999E-2</v>
+        <v>0</v>
       </c>
       <c r="H25" s="48">
         <f t="shared" si="1"/>
-        <v>1.345781882502084E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18475,21 +18388,21 @@
       </c>
       <c r="G26" s="41">
         <f t="shared" si="0"/>
-        <v>1.6624614389095349E-2</v>
+        <v>0</v>
       </c>
       <c r="H26" s="49">
         <f t="shared" si="1"/>
-        <v>5.2611911884490326E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E28">
         <f>SUM(E7:E26)</f>
-        <v>-1.8363647521813053</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <f>SUM(F7:F26)</f>
-        <v>-1.7456299905769432</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -18518,39 +18431,39 @@
       <c r="A1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="67">
+      <c r="B1" s="67" t="e">
         <f>AVERAGE(Visionados)*Pelis_con_nota/Pelis+10*(1-Pelis_con_nota)/Pelis</f>
-        <v>26047</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D1" t="s">
         <v>40</v>
       </c>
       <c r="E1" s="67">
         <f>MAX(Visionados)</f>
-        <v>26047</v>
+        <v>0</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" cm="1">
+      <c r="H1" t="e" cm="1">
         <f t="array" ref="H1">SUM(IF(Tabla1[Visionados],POWER(Tabla1[Visionados]-MediaVisionados,2),0)/Pelis)+POWER(10-MediaVisionados,2)*(Pelis-Pelis_con_nota)/Pelis</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="67">
+      <c r="B2" s="67" t="e">
         <f>MEDIAN(Visionados)</f>
-        <v>26047</v>
+        <v>#NUM!</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="67">
         <f>MIN(Visionados)</f>
-        <v>26047</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -18563,9 +18476,9 @@
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="2" t="e">
         <f>COUNTIF(Visionados,"&lt;="&amp;B4)/Pelis</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="12:14" x14ac:dyDescent="0.25">
@@ -18587,9 +18500,9 @@
         <f t="array" ref="M26">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])+Pelis_sin_nota</f>
         <v>0</v>
       </c>
-      <c r="N26" s="67">
+      <c r="N26" s="67" t="e">
         <f>(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE))*Pelis</f>
-        <v>0.17466068512885846</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="12:14" x14ac:dyDescent="0.25">
@@ -18600,9 +18513,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N27" s="67">
+      <c r="N27" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>0.14415433019917617</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="12:14" x14ac:dyDescent="0.25">
@@ -18613,9 +18526,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N28" s="67">
+      <c r="N28" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>0.11897623612229652</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="12:14" x14ac:dyDescent="0.25">
@@ -18626,9 +18539,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N29" s="67">
+      <c r="N29" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>9.8195765207123142E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="12:14" x14ac:dyDescent="0.25">
@@ -18639,9 +18552,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N30" s="67">
+      <c r="N30" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>8.1044825579294599E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="12:14" x14ac:dyDescent="0.25">
@@ -18650,11 +18563,11 @@
       </c>
       <c r="M31" s="67">
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="N31" s="67">
+        <v>0</v>
+      </c>
+      <c r="N31" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>6.6889480817466263E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="12:14" x14ac:dyDescent="0.25">
@@ -18665,9 +18578,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N32" s="67">
+      <c r="N32" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>5.5206518269973914E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="12:14" x14ac:dyDescent="0.25">
@@ -18678,9 +18591,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N33" s="67">
+      <c r="N33" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>4.5564109965361421E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="12:14" x14ac:dyDescent="0.25">
@@ -18691,9 +18604,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N34" s="67">
+      <c r="N34" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>3.7605851301524718E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="12:14" x14ac:dyDescent="0.25">
@@ -18704,9 +18617,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N35" s="67">
+      <c r="N35" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>3.1037587548346401E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="12:14" x14ac:dyDescent="0.25">
@@ -18717,9 +18630,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N36" s="67">
+      <c r="N36" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>2.5616541242405422E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="12:14" x14ac:dyDescent="0.25">
@@ -18730,9 +18643,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N37" s="67">
+      <c r="N37" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>2.114233859837511E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="12:14" x14ac:dyDescent="0.25">
@@ -18743,9 +18656,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N38" s="67">
+      <c r="N38" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.7449603253556711E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="12:14" x14ac:dyDescent="0.25">
@@ -18756,9 +18669,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N39" s="67">
+      <c r="N39" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.4401843594063601E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="12:14" x14ac:dyDescent="0.25">
@@ -18769,9 +18682,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N40" s="67">
+      <c r="N40" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.188640772480587E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="12:14" x14ac:dyDescent="0.25">
@@ -18782,9 +18695,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N41" s="67">
+      <c r="N41" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>9.8103196078703769E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="42" spans="12:14" x14ac:dyDescent="0.25">
@@ -18795,9 +18708,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N42" s="67">
+      <c r="N42" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>8.0968424638265812E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="43" spans="12:14" x14ac:dyDescent="0.25">
@@ -18808,9 +18721,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N43" s="67">
+      <c r="N43" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>6.6826424117142347E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="44" spans="12:14" x14ac:dyDescent="0.25">
@@ -18821,9 +18734,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N44" s="67">
+      <c r="N44" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>5.5154475096130806E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="45" spans="12:14" x14ac:dyDescent="0.25">
@@ -18834,9 +18747,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N45" s="67">
+      <c r="N45" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>4.5521156687917674E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="46" spans="12:14" x14ac:dyDescent="0.25">
@@ -18847,9 +18760,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N46" s="67">
+      <c r="N46" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>3.7570400272948223E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="47" spans="12:14" x14ac:dyDescent="0.25">
@@ -18860,9 +18773,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N47" s="67">
+      <c r="N47" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>3.1008328420708553E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="48" spans="12:14" x14ac:dyDescent="0.25">
@@ -18873,9 +18786,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N48" s="67">
+      <c r="N48" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>2.5592392534048436E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="49" spans="12:14" x14ac:dyDescent="0.25">
@@ -18886,9 +18799,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N49" s="67">
+      <c r="N49" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>2.1122407719963432E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="50" spans="12:14" x14ac:dyDescent="0.25">
@@ -18899,9 +18812,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N50" s="67">
+      <c r="N50" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.7433153516024369E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="51" spans="12:14" x14ac:dyDescent="0.25">
@@ -18912,9 +18825,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N51" s="67">
+      <c r="N51" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.4388266978958564E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="52" spans="12:14" x14ac:dyDescent="0.25">
@@ -18925,9 +18838,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N52" s="67">
+      <c r="N52" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.1875202410597252E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="53" spans="12:14" x14ac:dyDescent="0.25">
@@ -18938,9 +18851,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N53" s="67">
+      <c r="N53" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>9.8010714215179817E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="54" spans="12:14" x14ac:dyDescent="0.25">
@@ -18951,9 +18864,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N54" s="67">
+      <c r="N54" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>8.089209572039735E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="55" spans="12:14" x14ac:dyDescent="0.25">
@@ -18964,9 +18877,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N55" s="67">
+      <c r="N55" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>6.6763426860350084E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="56" spans="12:14" x14ac:dyDescent="0.25">
@@ -18977,9 +18890,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N56" s="67">
+      <c r="N56" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>5.5102480983382218E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="57" spans="12:14" x14ac:dyDescent="0.25">
@@ -18990,9 +18903,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N57" s="67">
+      <c r="N57" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>4.54782439025192E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="58" spans="12:14" x14ac:dyDescent="0.25">
@@ -19003,9 +18916,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N58" s="67">
+      <c r="N58" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>3.7534982664044758E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="59" spans="12:14" x14ac:dyDescent="0.25">
@@ -19016,9 +18929,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N59" s="67">
+      <c r="N59" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>3.0979096875649592E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="60" spans="12:14" x14ac:dyDescent="0.25">
@@ -19029,9 +18942,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N60" s="67">
+      <c r="N60" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>2.5568266590669797E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="61" spans="12:14" x14ac:dyDescent="0.25">
@@ -19042,9 +18955,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N61" s="67">
+      <c r="N61" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>2.1102495630387352E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="62" spans="12:14" x14ac:dyDescent="0.25">
@@ -19055,9 +18968,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N62" s="67">
+      <c r="N62" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.741671928565669E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="63" spans="12:14" x14ac:dyDescent="0.25">
@@ -19068,9 +18981,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N63" s="67">
+      <c r="N63" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.4374703162522984E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="64" spans="12:14" x14ac:dyDescent="0.25">
@@ -19081,9 +18994,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N64" s="67">
+      <c r="N64" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>1.1864007659645459E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="65" spans="12:14" x14ac:dyDescent="0.25">
@@ -19094,9 +19007,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N65" s="67">
+      <c r="N65" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>9.7918319534207043E-5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="66" spans="12:14" x14ac:dyDescent="0.25">
@@ -19107,9 +19020,9 @@
         <f ca="1">COUNTIF(Tabla1[Visionados],"&lt;="&amp;TablaVisionados[[#This Row],[Visionados]])-COUNTIF(Tabla1[Visionados],"&lt;="&amp;OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0))</f>
         <v>0</v>
       </c>
-      <c r="N66" s="67">
+      <c r="N66" s="67" t="e">
         <f ca="1">(_xlfn.EXPON.DIST(TablaVisionados[[#This Row],[Visionados]],1/MediaVisionados,TRUE)-_xlfn.EXPON.DIST(OFFSET(TablaVisionados[[#This Row],[Visionados]],-1,0),1/MediaVisionados,TRUE))*Pelis</f>
-        <v>8.0815838757852809E-5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="67" spans="12:14" x14ac:dyDescent="0.25">

</xml_diff>